<commit_message>
All reduce numbers updated for all GPUs and KNL
</commit_message>
<xml_diff>
--- a/results/train/DeepBench_NV_1080Ti.xlsx
+++ b/results/train/DeepBench_NV_1080Ti.xlsx
@@ -1,29 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patwarymostofa/Documents/mostofa/deepbench-internal/DeepBench-internal/results/train/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6240" yWindow="720" windowWidth="26160" windowHeight="19580" tabRatio="500"/>
+    <workbookView xWindow="6240" yWindow="460" windowWidth="26160" windowHeight="19280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Results - FP32" sheetId="3" r:id="rId1"/>
     <sheet name="Specs" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="80">
   <si>
     <t>Dense Matrix Multiplication</t>
   </si>
@@ -231,6 +236,39 @@
   <si>
     <t>6.0.21</t>
   </si>
+  <si>
+    <t>All-Reduce</t>
+  </si>
+  <si>
+    <t>Size # floats</t>
+  </si>
+  <si>
+    <t># chips / accelerator cards</t>
+  </si>
+  <si>
+    <t>Mean All Reduce Time (msec)</t>
+  </si>
+  <si>
+    <t>Gigabytes/sec</t>
+  </si>
+  <si>
+    <t>Selected Algorithm</t>
+  </si>
+  <si>
+    <t>Std Dev All Reduce Time (msec)</t>
+  </si>
+  <si>
+    <t>NCCL 2.0 MPI</t>
+  </si>
+  <si>
+    <t>OSU Allreduce</t>
+  </si>
+  <si>
+    <t>NCCL 2.0 Single</t>
+  </si>
+  <si>
+    <t>Baidu RingAllReduce</t>
+  </si>
 </sst>
 </file>
 
@@ -266,6 +304,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -294,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -329,6 +368,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -601,7 +643,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -609,13 +651,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE339"/>
+  <dimension ref="A1:AE384"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A345" workbookViewId="0">
+      <selection activeCell="B370" sqref="B370"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28" style="5" customWidth="1"/>
     <col min="2" max="3" width="11" style="5"/>
@@ -636,7 +678,7 @@
     <col min="23" max="16384" width="11" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>62</v>
       </c>
@@ -644,7 +686,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -670,7 +712,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C4" s="5">
         <v>1760</v>
       </c>
@@ -696,7 +738,7 @@
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C5" s="5">
         <v>1760</v>
       </c>
@@ -722,7 +764,7 @@
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C6" s="5">
         <v>1760</v>
       </c>
@@ -748,7 +790,7 @@
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C7" s="5">
         <v>1760</v>
       </c>
@@ -774,7 +816,7 @@
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C8" s="5">
         <v>1760</v>
       </c>
@@ -800,7 +842,7 @@
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C9" s="5">
         <v>2048</v>
       </c>
@@ -826,7 +868,7 @@
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C10" s="5">
         <v>2048</v>
       </c>
@@ -852,7 +894,7 @@
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C11" s="5">
         <v>2048</v>
       </c>
@@ -878,7 +920,7 @@
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C12" s="5">
         <v>2048</v>
       </c>
@@ -904,7 +946,7 @@
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C13" s="5">
         <v>2048</v>
       </c>
@@ -930,7 +972,7 @@
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C14" s="5">
         <v>2560</v>
       </c>
@@ -956,7 +998,7 @@
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C15" s="5">
         <v>2560</v>
       </c>
@@ -982,7 +1024,7 @@
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C16" s="5">
         <v>2560</v>
       </c>
@@ -1008,7 +1050,7 @@
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
     </row>
-    <row r="17" spans="3:12">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C17" s="5">
         <v>2560</v>
       </c>
@@ -1034,7 +1076,7 @@
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
     </row>
-    <row r="18" spans="3:12">
+    <row r="18" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C18" s="5">
         <v>2560</v>
       </c>
@@ -1060,7 +1102,7 @@
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
     </row>
-    <row r="19" spans="3:12">
+    <row r="19" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C19" s="5">
         <v>4096</v>
       </c>
@@ -1086,7 +1128,7 @@
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
     </row>
-    <row r="20" spans="3:12">
+    <row r="20" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C20" s="5">
         <v>4096</v>
       </c>
@@ -1112,7 +1154,7 @@
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
     </row>
-    <row r="21" spans="3:12">
+    <row r="21" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C21" s="5">
         <v>4096</v>
       </c>
@@ -1138,7 +1180,7 @@
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
     </row>
-    <row r="22" spans="3:12">
+    <row r="22" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C22" s="5">
         <v>4096</v>
       </c>
@@ -1164,7 +1206,7 @@
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
     </row>
-    <row r="23" spans="3:12">
+    <row r="23" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C23" s="5">
         <v>4096</v>
       </c>
@@ -1190,7 +1232,7 @@
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
     </row>
-    <row r="24" spans="3:12">
+    <row r="24" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C24" s="5">
         <v>1760</v>
       </c>
@@ -1216,7 +1258,7 @@
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
     </row>
-    <row r="25" spans="3:12">
+    <row r="25" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C25" s="5">
         <v>1760</v>
       </c>
@@ -1242,7 +1284,7 @@
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
     </row>
-    <row r="26" spans="3:12">
+    <row r="26" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C26" s="5">
         <v>1760</v>
       </c>
@@ -1268,7 +1310,7 @@
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
     </row>
-    <row r="27" spans="3:12">
+    <row r="27" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C27" s="5">
         <v>1760</v>
       </c>
@@ -1294,7 +1336,7 @@
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
     </row>
-    <row r="28" spans="3:12">
+    <row r="28" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C28" s="5">
         <v>1760</v>
       </c>
@@ -1320,7 +1362,7 @@
       <c r="K28" s="6"/>
       <c r="L28" s="6"/>
     </row>
-    <row r="29" spans="3:12">
+    <row r="29" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C29" s="5">
         <v>2048</v>
       </c>
@@ -1346,7 +1388,7 @@
       <c r="K29" s="6"/>
       <c r="L29" s="6"/>
     </row>
-    <row r="30" spans="3:12">
+    <row r="30" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C30" s="5">
         <v>2048</v>
       </c>
@@ -1372,7 +1414,7 @@
       <c r="K30" s="6"/>
       <c r="L30" s="6"/>
     </row>
-    <row r="31" spans="3:12">
+    <row r="31" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C31" s="5">
         <v>2048</v>
       </c>
@@ -1398,7 +1440,7 @@
       <c r="K31" s="6"/>
       <c r="L31" s="6"/>
     </row>
-    <row r="32" spans="3:12">
+    <row r="32" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C32" s="5">
         <v>2048</v>
       </c>
@@ -1424,7 +1466,7 @@
       <c r="K32" s="6"/>
       <c r="L32" s="6"/>
     </row>
-    <row r="33" spans="3:12">
+    <row r="33" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C33" s="5">
         <v>2048</v>
       </c>
@@ -1450,7 +1492,7 @@
       <c r="K33" s="6"/>
       <c r="L33" s="6"/>
     </row>
-    <row r="34" spans="3:12">
+    <row r="34" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C34" s="5">
         <v>2560</v>
       </c>
@@ -1476,7 +1518,7 @@
       <c r="K34" s="6"/>
       <c r="L34" s="6"/>
     </row>
-    <row r="35" spans="3:12">
+    <row r="35" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C35" s="5">
         <v>2560</v>
       </c>
@@ -1502,7 +1544,7 @@
       <c r="K35" s="6"/>
       <c r="L35" s="6"/>
     </row>
-    <row r="36" spans="3:12">
+    <row r="36" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C36" s="5">
         <v>2560</v>
       </c>
@@ -1528,7 +1570,7 @@
       <c r="K36" s="6"/>
       <c r="L36" s="6"/>
     </row>
-    <row r="37" spans="3:12">
+    <row r="37" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C37" s="5">
         <v>2560</v>
       </c>
@@ -1554,7 +1596,7 @@
       <c r="K37" s="6"/>
       <c r="L37" s="6"/>
     </row>
-    <row r="38" spans="3:12">
+    <row r="38" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C38" s="5">
         <v>2560</v>
       </c>
@@ -1580,7 +1622,7 @@
       <c r="K38" s="6"/>
       <c r="L38" s="6"/>
     </row>
-    <row r="39" spans="3:12">
+    <row r="39" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C39" s="5">
         <v>4096</v>
       </c>
@@ -1606,7 +1648,7 @@
       <c r="K39" s="6"/>
       <c r="L39" s="6"/>
     </row>
-    <row r="40" spans="3:12">
+    <row r="40" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C40" s="5">
         <v>4096</v>
       </c>
@@ -1632,7 +1674,7 @@
       <c r="K40" s="6"/>
       <c r="L40" s="6"/>
     </row>
-    <row r="41" spans="3:12">
+    <row r="41" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C41" s="5">
         <v>4096</v>
       </c>
@@ -1658,7 +1700,7 @@
       <c r="K41" s="6"/>
       <c r="L41" s="6"/>
     </row>
-    <row r="42" spans="3:12">
+    <row r="42" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C42" s="5">
         <v>4096</v>
       </c>
@@ -1684,7 +1726,7 @@
       <c r="K42" s="6"/>
       <c r="L42" s="6"/>
     </row>
-    <row r="43" spans="3:12">
+    <row r="43" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C43" s="5">
         <v>4096</v>
       </c>
@@ -1710,7 +1752,7 @@
       <c r="K43" s="6"/>
       <c r="L43" s="6"/>
     </row>
-    <row r="44" spans="3:12">
+    <row r="44" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C44" s="5">
         <v>1760</v>
       </c>
@@ -1739,7 +1781,7 @@
       <c r="K44" s="6"/>
       <c r="L44" s="6"/>
     </row>
-    <row r="45" spans="3:12">
+    <row r="45" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C45" s="5">
         <v>2048</v>
       </c>
@@ -1765,7 +1807,7 @@
       <c r="K45" s="6"/>
       <c r="L45" s="6"/>
     </row>
-    <row r="46" spans="3:12">
+    <row r="46" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C46" s="5">
         <v>2560</v>
       </c>
@@ -1791,7 +1833,7 @@
       <c r="K46" s="6"/>
       <c r="L46" s="6"/>
     </row>
-    <row r="47" spans="3:12">
+    <row r="47" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C47" s="7">
         <v>4096</v>
       </c>
@@ -1817,19 +1859,19 @@
       <c r="K47" s="6"/>
       <c r="L47" s="6"/>
     </row>
-    <row r="48" spans="3:12">
+    <row r="48" spans="3:12" x14ac:dyDescent="0.2">
       <c r="I48" s="6"/>
       <c r="J48" s="6"/>
       <c r="K48" s="6"/>
       <c r="L48" s="6"/>
     </row>
-    <row r="49" spans="3:12">
+    <row r="49" spans="3:12" x14ac:dyDescent="0.2">
       <c r="I49" s="6"/>
       <c r="J49" s="6"/>
       <c r="K49" s="6"/>
       <c r="L49" s="6"/>
     </row>
-    <row r="50" spans="3:12">
+    <row r="50" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C50" s="5">
         <v>5124</v>
       </c>
@@ -1855,7 +1897,7 @@
       <c r="K50" s="6"/>
       <c r="L50" s="6"/>
     </row>
-    <row r="51" spans="3:12">
+    <row r="51" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C51" s="5">
         <v>35</v>
       </c>
@@ -1881,7 +1923,7 @@
       <c r="K51" s="6"/>
       <c r="L51" s="6"/>
     </row>
-    <row r="52" spans="3:12">
+    <row r="52" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C52" s="5">
         <v>5124</v>
       </c>
@@ -1907,7 +1949,7 @@
       <c r="K52" s="6"/>
       <c r="L52" s="6"/>
     </row>
-    <row r="53" spans="3:12">
+    <row r="53" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C53" s="5">
         <v>35</v>
       </c>
@@ -1933,7 +1975,7 @@
       <c r="K53" s="6"/>
       <c r="L53" s="6"/>
     </row>
-    <row r="54" spans="3:12">
+    <row r="54" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C54" s="5">
         <v>5124</v>
       </c>
@@ -1959,7 +2001,7 @@
       <c r="K54" s="6"/>
       <c r="L54" s="6"/>
     </row>
-    <row r="55" spans="3:12">
+    <row r="55" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C55" s="5">
         <v>35</v>
       </c>
@@ -1985,7 +2027,7 @@
       <c r="K55" s="6"/>
       <c r="L55" s="6"/>
     </row>
-    <row r="56" spans="3:12">
+    <row r="56" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C56" s="5">
         <v>5124</v>
       </c>
@@ -2011,7 +2053,7 @@
       <c r="K56" s="6"/>
       <c r="L56" s="6"/>
     </row>
-    <row r="57" spans="3:12">
+    <row r="57" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C57" s="5">
         <v>35</v>
       </c>
@@ -2037,7 +2079,7 @@
       <c r="K57" s="6"/>
       <c r="L57" s="6"/>
     </row>
-    <row r="58" spans="3:12">
+    <row r="58" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C58" s="5">
         <v>5124</v>
       </c>
@@ -2063,7 +2105,7 @@
       <c r="K58" s="6"/>
       <c r="L58" s="6"/>
     </row>
-    <row r="59" spans="3:12">
+    <row r="59" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C59" s="5">
         <v>35</v>
       </c>
@@ -2089,7 +2131,7 @@
       <c r="K59" s="6"/>
       <c r="L59" s="6"/>
     </row>
-    <row r="60" spans="3:12">
+    <row r="60" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C60" s="5">
         <v>5124</v>
       </c>
@@ -2115,7 +2157,7 @@
       <c r="K60" s="6"/>
       <c r="L60" s="6"/>
     </row>
-    <row r="61" spans="3:12">
+    <row r="61" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C61" s="5">
         <v>35</v>
       </c>
@@ -2141,7 +2183,7 @@
       <c r="K61" s="6"/>
       <c r="L61" s="6"/>
     </row>
-    <row r="62" spans="3:12">
+    <row r="62" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C62" s="5">
         <v>5124</v>
       </c>
@@ -2167,7 +2209,7 @@
       <c r="K62" s="6"/>
       <c r="L62" s="6"/>
     </row>
-    <row r="63" spans="3:12">
+    <row r="63" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C63" s="5">
         <v>35</v>
       </c>
@@ -2193,7 +2235,7 @@
       <c r="K63" s="6"/>
       <c r="L63" s="6"/>
     </row>
-    <row r="64" spans="3:12">
+    <row r="64" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C64" s="5">
         <v>5124</v>
       </c>
@@ -2219,7 +2261,7 @@
       <c r="K64" s="6"/>
       <c r="L64" s="6"/>
     </row>
-    <row r="65" spans="3:12">
+    <row r="65" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C65" s="5">
         <v>35</v>
       </c>
@@ -2245,13 +2287,13 @@
       <c r="K65" s="6"/>
       <c r="L65" s="6"/>
     </row>
-    <row r="66" spans="3:12">
+    <row r="66" spans="3:12" x14ac:dyDescent="0.2">
       <c r="I66" s="6"/>
       <c r="J66" s="6"/>
       <c r="K66" s="6"/>
       <c r="L66" s="6"/>
     </row>
-    <row r="67" spans="3:12">
+    <row r="67" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C67" s="5">
         <v>7680</v>
       </c>
@@ -2277,7 +2319,7 @@
       <c r="K67" s="6"/>
       <c r="L67" s="6"/>
     </row>
-    <row r="68" spans="3:12">
+    <row r="68" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C68" s="5">
         <v>7680</v>
       </c>
@@ -2303,7 +2345,7 @@
       <c r="K68" s="6"/>
       <c r="L68" s="6"/>
     </row>
-    <row r="69" spans="3:12">
+    <row r="69" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C69" s="5">
         <v>7680</v>
       </c>
@@ -2329,7 +2371,7 @@
       <c r="K69" s="6"/>
       <c r="L69" s="6"/>
     </row>
-    <row r="70" spans="3:12">
+    <row r="70" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C70" s="5">
         <v>7680</v>
       </c>
@@ -2355,7 +2397,7 @@
       <c r="K70" s="6"/>
       <c r="L70" s="6"/>
     </row>
-    <row r="71" spans="3:12">
+    <row r="71" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C71" s="5">
         <v>7680</v>
       </c>
@@ -2381,7 +2423,7 @@
       <c r="K71" s="6"/>
       <c r="L71" s="6"/>
     </row>
-    <row r="72" spans="3:12">
+    <row r="72" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C72" s="5">
         <v>7680</v>
       </c>
@@ -2407,7 +2449,7 @@
       <c r="K72" s="6"/>
       <c r="L72" s="6"/>
     </row>
-    <row r="73" spans="3:12">
+    <row r="73" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C73" s="5">
         <v>7680</v>
       </c>
@@ -2433,7 +2475,7 @@
       <c r="K73" s="6"/>
       <c r="L73" s="6"/>
     </row>
-    <row r="74" spans="3:12">
+    <row r="74" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C74" s="5">
         <v>7680</v>
       </c>
@@ -2459,7 +2501,7 @@
       <c r="K74" s="6"/>
       <c r="L74" s="6"/>
     </row>
-    <row r="75" spans="3:12">
+    <row r="75" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C75" s="5">
         <f>3*1024</f>
         <v>3072</v>
@@ -2486,7 +2528,7 @@
       <c r="K75" s="6"/>
       <c r="L75" s="6"/>
     </row>
-    <row r="76" spans="3:12">
+    <row r="76" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C76" s="5">
         <f t="shared" ref="C76:C82" si="3">3*1024</f>
         <v>3072</v>
@@ -2513,7 +2555,7 @@
       <c r="K76" s="6"/>
       <c r="L76" s="6"/>
     </row>
-    <row r="77" spans="3:12">
+    <row r="77" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C77" s="5">
         <f t="shared" si="3"/>
         <v>3072</v>
@@ -2540,7 +2582,7 @@
       <c r="K77" s="6"/>
       <c r="L77" s="6"/>
     </row>
-    <row r="78" spans="3:12">
+    <row r="78" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C78" s="5">
         <f t="shared" si="3"/>
         <v>3072</v>
@@ -2567,7 +2609,7 @@
       <c r="K78" s="6"/>
       <c r="L78" s="6"/>
     </row>
-    <row r="79" spans="3:12">
+    <row r="79" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C79" s="5">
         <f t="shared" si="3"/>
         <v>3072</v>
@@ -2594,7 +2636,7 @@
       <c r="K79" s="6"/>
       <c r="L79" s="6"/>
     </row>
-    <row r="80" spans="3:12">
+    <row r="80" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C80" s="5">
         <f t="shared" si="3"/>
         <v>3072</v>
@@ -2621,7 +2663,7 @@
       <c r="K80" s="6"/>
       <c r="L80" s="6"/>
     </row>
-    <row r="81" spans="3:12">
+    <row r="81" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C81" s="5">
         <f t="shared" si="3"/>
         <v>3072</v>
@@ -2648,7 +2690,7 @@
       <c r="K81" s="6"/>
       <c r="L81" s="6"/>
     </row>
-    <row r="82" spans="3:12">
+    <row r="82" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C82" s="5">
         <f t="shared" si="3"/>
         <v>3072</v>
@@ -2675,13 +2717,13 @@
       <c r="K82" s="6"/>
       <c r="L82" s="6"/>
     </row>
-    <row r="83" spans="3:12">
+    <row r="83" spans="3:12" x14ac:dyDescent="0.2">
       <c r="I83" s="6"/>
       <c r="J83" s="6"/>
       <c r="K83" s="6"/>
       <c r="L83" s="6"/>
     </row>
-    <row r="84" spans="3:12">
+    <row r="84" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C84" s="5">
         <v>3072</v>
       </c>
@@ -2707,7 +2749,7 @@
       <c r="K84" s="6"/>
       <c r="L84" s="6"/>
     </row>
-    <row r="85" spans="3:12">
+    <row r="85" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C85" s="5">
         <v>7680</v>
       </c>
@@ -2733,11 +2775,11 @@
       <c r="K85" s="6"/>
       <c r="L85" s="6"/>
     </row>
-    <row r="86" spans="3:12">
+    <row r="86" spans="3:12" x14ac:dyDescent="0.2">
       <c r="I86" s="6"/>
       <c r="J86" s="6"/>
     </row>
-    <row r="87" spans="3:12">
+    <row r="87" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C87" s="5">
         <v>512</v>
       </c>
@@ -2761,7 +2803,7 @@
         <v>0.62192529608259939</v>
       </c>
     </row>
-    <row r="88" spans="3:12">
+    <row r="88" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C88" s="5">
         <v>1024</v>
       </c>
@@ -2785,7 +2827,7 @@
         <v>1.1606687446868802</v>
       </c>
     </row>
-    <row r="89" spans="3:12">
+    <row r="89" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C89" s="5">
         <v>512</v>
       </c>
@@ -2809,7 +2851,7 @@
         <v>1.2935417653560712</v>
       </c>
     </row>
-    <row r="90" spans="3:12">
+    <row r="90" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C90" s="5">
         <v>1024</v>
       </c>
@@ -2833,7 +2875,7 @@
         <v>2.0352795031055901</v>
       </c>
     </row>
-    <row r="91" spans="3:12">
+    <row r="91" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C91" s="5">
         <v>512</v>
       </c>
@@ -2857,7 +2899,7 @@
         <v>0.86068501786089513</v>
       </c>
     </row>
-    <row r="92" spans="3:12">
+    <row r="92" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C92" s="5">
         <v>1024</v>
       </c>
@@ -2881,7 +2923,7 @@
         <v>1.3950953678474116</v>
       </c>
     </row>
-    <row r="93" spans="3:12">
+    <row r="93" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C93" s="5">
         <v>512</v>
       </c>
@@ -2905,7 +2947,7 @@
         <v>1.2620551532891697</v>
       </c>
     </row>
-    <row r="94" spans="3:12">
+    <row r="94" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C94" s="5">
         <v>1024</v>
       </c>
@@ -2929,7 +2971,7 @@
         <v>1.2276337479394575</v>
       </c>
     </row>
-    <row r="95" spans="3:12">
+    <row r="95" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C95" s="5">
         <v>1024</v>
       </c>
@@ -2953,7 +2995,7 @@
         <v>8.6353317647058816</v>
       </c>
     </row>
-    <row r="96" spans="3:12">
+    <row r="96" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C96" s="5">
         <v>1024</v>
       </c>
@@ -2977,7 +3019,7 @@
         <v>8.0659692307692303</v>
       </c>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C97" s="5">
         <v>7680</v>
       </c>
@@ -3001,7 +3043,7 @@
         <v>11.183617747440273</v>
       </c>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C98" s="5">
         <v>6144</v>
       </c>
@@ -3025,7 +3067,7 @@
         <v>10.661602400706089</v>
       </c>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" s="7"/>
       <c r="C99" s="7">
         <v>4608</v>
@@ -3051,7 +3093,7 @@
         <v>11.319715589911038</v>
       </c>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" s="7"/>
       <c r="C100" s="7">
         <v>8448</v>
@@ -3077,7 +3119,7 @@
         <v>11.144177229520036</v>
       </c>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" s="7"/>
       <c r="C101" s="7">
         <v>3072</v>
@@ -3103,7 +3145,7 @@
         <v>11.15259206736096</v>
       </c>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C102" s="5">
         <v>7680</v>
       </c>
@@ -3127,7 +3169,7 @@
         <v>10.697268775398008</v>
       </c>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C103" s="5">
         <v>6144</v>
       </c>
@@ -3151,7 +3193,7 @@
         <v>10.690853633064872</v>
       </c>
     </row>
-    <row r="104" spans="1:10">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" s="7"/>
       <c r="C104" s="7">
         <v>4608</v>
@@ -3177,7 +3219,7 @@
         <v>10.772699495830297</v>
       </c>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" s="7"/>
       <c r="C105" s="7">
         <v>8448</v>
@@ -3203,7 +3245,7 @@
         <v>10.618120873143177</v>
       </c>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" s="7"/>
       <c r="C106" s="7">
         <v>3072</v>
@@ -3229,7 +3271,7 @@
         <v>10.961918327344005</v>
       </c>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C107" s="5">
         <v>7680</v>
       </c>
@@ -3253,7 +3295,7 @@
         <v>9.2426267078007935</v>
       </c>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C108" s="5">
         <v>6144</v>
       </c>
@@ -3277,7 +3319,7 @@
         <v>6.6922966869806091</v>
       </c>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" s="7"/>
       <c r="C109" s="7">
         <v>4608</v>
@@ -3303,7 +3345,7 @@
         <v>10.159040248788948</v>
       </c>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" s="7"/>
       <c r="C110" s="7">
         <v>8448</v>
@@ -3329,7 +3371,7 @@
         <v>9.1024253806297324</v>
       </c>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" s="7"/>
       <c r="C111" s="7">
         <v>3072</v>
@@ -3355,7 +3397,7 @@
         <v>11.118102054340623</v>
       </c>
     </row>
-    <row r="112" spans="1:10">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C112" s="5">
         <v>7680</v>
       </c>
@@ -3379,7 +3421,7 @@
         <v>9.6780711919680851</v>
       </c>
     </row>
-    <row r="113" spans="1:10">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C113" s="5">
         <v>6144</v>
       </c>
@@ -3403,7 +3445,7 @@
         <v>6.6565247809555306</v>
       </c>
     </row>
-    <row r="114" spans="1:10">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114" s="7"/>
       <c r="C114" s="7">
         <v>4608</v>
@@ -3429,7 +3471,7 @@
         <v>10.163903069466881</v>
       </c>
     </row>
-    <row r="115" spans="1:10">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115" s="7"/>
       <c r="C115" s="7">
         <v>8448</v>
@@ -3455,7 +3497,7 @@
         <v>9.5437825296597953</v>
       </c>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A116" s="7"/>
       <c r="C116" s="7">
         <v>3072</v>
@@ -3481,7 +3523,7 @@
         <v>10.721788255343322</v>
       </c>
     </row>
-    <row r="117" spans="1:10">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A117" s="7"/>
       <c r="C117" s="7">
         <v>6144</v>
@@ -3507,7 +3549,7 @@
         <v>0.75972298867924537</v>
       </c>
     </row>
-    <row r="118" spans="1:10">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A118" s="7"/>
       <c r="C118" s="7">
         <v>4608</v>
@@ -3533,7 +3575,7 @@
         <v>1.2177011612903226</v>
       </c>
     </row>
-    <row r="119" spans="1:10">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A119" s="7"/>
       <c r="C119" s="7">
         <v>8448</v>
@@ -3559,7 +3601,7 @@
         <v>0.86116083257918552</v>
       </c>
     </row>
-    <row r="120" spans="1:10">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A120" s="7"/>
       <c r="C120" s="7">
         <v>6144</v>
@@ -3585,7 +3627,7 @@
         <v>3.3554432000000003</v>
       </c>
     </row>
-    <row r="121" spans="1:10">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A121" s="7"/>
       <c r="C121" s="7">
         <v>4608</v>
@@ -3611,7 +3653,7 @@
         <v>5.6623104</v>
       </c>
     </row>
-    <row r="122" spans="1:10">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122" s="7"/>
       <c r="C122" s="7">
         <v>8448</v>
@@ -3637,7 +3679,7 @@
         <v>6.2914560000000002</v>
       </c>
     </row>
-    <row r="123" spans="1:10">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A123" s="7"/>
       <c r="C123" s="7">
         <v>6144</v>
@@ -3663,7 +3705,7 @@
         <v>1.2905550769230769</v>
       </c>
     </row>
-    <row r="124" spans="1:10">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A124" s="7"/>
       <c r="C124" s="7">
         <v>4608</v>
@@ -3689,7 +3731,7 @@
         <v>1.4518744615384618</v>
       </c>
     </row>
-    <row r="125" spans="1:10">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A125" s="7"/>
       <c r="C125" s="7">
         <v>8448</v>
@@ -3715,7 +3757,7 @@
         <v>1.4282667467166978</v>
       </c>
     </row>
-    <row r="126" spans="1:10">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A126" s="7"/>
       <c r="C126" s="7">
         <v>6144</v>
@@ -3741,7 +3783,7 @@
         <v>2.982616177777778</v>
       </c>
     </row>
-    <row r="127" spans="1:10">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127" s="7"/>
       <c r="C127" s="7">
         <v>4608</v>
@@ -3767,7 +3809,7 @@
         <v>4.1180439272727272</v>
       </c>
     </row>
-    <row r="128" spans="1:10">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A128" s="7"/>
       <c r="C128" s="7">
         <v>8448</v>
@@ -3793,7 +3835,7 @@
         <v>4.4388698309037888</v>
       </c>
     </row>
-    <row r="129" spans="2:10">
+    <row r="129" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C129" s="7">
         <v>512</v>
       </c>
@@ -3819,7 +3861,7 @@
         <v>10.766337274424394</v>
       </c>
     </row>
-    <row r="130" spans="2:10">
+    <row r="130" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C130" s="7">
         <v>512</v>
       </c>
@@ -3845,7 +3887,7 @@
         <v>10.784582815513177</v>
       </c>
     </row>
-    <row r="131" spans="2:10">
+    <row r="131" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B131" s="7"/>
       <c r="C131" s="7">
         <v>512</v>
@@ -3872,7 +3914,7 @@
         <v>10.741772238347275</v>
       </c>
     </row>
-    <row r="132" spans="2:10">
+    <row r="132" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B132" s="7"/>
       <c r="C132" s="7">
         <v>512</v>
@@ -3899,7 +3941,7 @@
         <v>10.657959183673471</v>
       </c>
     </row>
-    <row r="133" spans="2:10">
+    <row r="133" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C133" s="7">
         <v>1024</v>
       </c>
@@ -3925,7 +3967,7 @@
         <v>10.920081420118342</v>
       </c>
     </row>
-    <row r="134" spans="2:10">
+    <row r="134" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C134" s="7">
         <v>1024</v>
       </c>
@@ -3951,7 +3993,7 @@
         <v>10.969085322000653</v>
       </c>
     </row>
-    <row r="135" spans="2:10">
+    <row r="135" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B135" s="7"/>
       <c r="C135" s="7">
         <v>1024</v>
@@ -3978,7 +4020,7 @@
         <v>11.176862675430804</v>
       </c>
     </row>
-    <row r="136" spans="2:10">
+    <row r="136" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B136" s="7"/>
       <c r="C136" s="7">
         <v>1024</v>
@@ -4005,7 +4047,7 @@
         <v>10.952892513836293</v>
       </c>
     </row>
-    <row r="137" spans="2:10">
+    <row r="137" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B137" s="7"/>
       <c r="C137" s="7">
         <v>512</v>
@@ -4031,7 +4073,7 @@
         <v>0.76260072727272732</v>
       </c>
     </row>
-    <row r="138" spans="2:10">
+    <row r="138" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B138" s="7"/>
       <c r="C138" s="7">
         <v>1024</v>
@@ -4057,7 +4099,7 @@
         <v>1.5252014545454546</v>
       </c>
     </row>
-    <row r="139" spans="2:10">
+    <row r="139" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C139" s="7">
         <v>512</v>
       </c>
@@ -4083,7 +4125,7 @@
         <v>10.541662757044934</v>
       </c>
     </row>
-    <row r="140" spans="2:10">
+    <row r="140" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C140" s="7">
         <v>512</v>
       </c>
@@ -4109,7 +4151,7 @@
         <v>10.677057276198557</v>
       </c>
     </row>
-    <row r="141" spans="2:10">
+    <row r="141" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B141" s="7"/>
       <c r="C141" s="7">
         <v>512</v>
@@ -4136,7 +4178,7 @@
         <v>10.674340006786563</v>
       </c>
     </row>
-    <row r="142" spans="2:10">
+    <row r="142" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B142" s="7"/>
       <c r="C142" s="7">
         <v>512</v>
@@ -4163,7 +4205,7 @@
         <v>10.441899472368787</v>
       </c>
     </row>
-    <row r="143" spans="2:10">
+    <row r="143" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C143" s="7">
         <v>1024</v>
       </c>
@@ -4189,7 +4231,7 @@
         <v>10.290092335142367</v>
       </c>
     </row>
-    <row r="144" spans="2:10">
+    <row r="144" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C144" s="7">
         <v>1024</v>
       </c>
@@ -4215,7 +4257,7 @@
         <v>10.750031610422894</v>
       </c>
     </row>
-    <row r="145" spans="2:10">
+    <row r="145" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B145" s="7"/>
       <c r="C145" s="7">
         <v>1024</v>
@@ -4242,7 +4284,7 @@
         <v>10.820287213001979</v>
       </c>
     </row>
-    <row r="146" spans="2:10">
+    <row r="146" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B146" s="7"/>
       <c r="C146" s="7">
         <v>1024</v>
@@ -4269,7 +4311,7 @@
         <v>10.642875742994621</v>
       </c>
     </row>
-    <row r="147" spans="2:10">
+    <row r="147" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B147" s="7"/>
       <c r="C147" s="7">
         <v>512</v>
@@ -4295,7 +4337,7 @@
         <v>1.1983725714285716</v>
       </c>
     </row>
-    <row r="148" spans="2:10">
+    <row r="148" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B148" s="7"/>
       <c r="C148" s="7">
         <v>1024</v>
@@ -4321,7 +4363,7 @@
         <v>1.8641351111111111</v>
       </c>
     </row>
-    <row r="149" spans="2:10">
+    <row r="149" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C149" s="7">
         <v>512</v>
       </c>
@@ -4347,7 +4389,7 @@
         <v>10.852440959698917</v>
       </c>
     </row>
-    <row r="150" spans="2:10">
+    <row r="150" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C150" s="7">
         <v>512</v>
       </c>
@@ -4373,7 +4415,7 @@
         <v>11.078945190402816</v>
       </c>
     </row>
-    <row r="151" spans="2:10">
+    <row r="151" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B151" s="7"/>
       <c r="C151" s="7">
         <v>512</v>
@@ -4400,7 +4442,7 @@
         <v>10.685217391304347</v>
       </c>
     </row>
-    <row r="152" spans="2:10">
+    <row r="152" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B152" s="7"/>
       <c r="C152" s="7">
         <v>512</v>
@@ -4427,7 +4469,7 @@
         <v>10.457872340425533</v>
       </c>
     </row>
-    <row r="153" spans="2:10">
+    <row r="153" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C153" s="7">
         <v>1024</v>
       </c>
@@ -4453,7 +4495,7 @@
         <v>10.725457729562184</v>
       </c>
     </row>
-    <row r="154" spans="2:10">
+    <row r="154" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C154" s="7">
         <v>1024</v>
       </c>
@@ -4479,7 +4521,7 @@
         <v>10.947612398042414</v>
       </c>
     </row>
-    <row r="155" spans="2:10">
+    <row r="155" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B155" s="7"/>
       <c r="C155" s="7">
         <v>1024</v>
@@ -4506,7 +4548,7 @@
         <v>10.678416429753469</v>
       </c>
     </row>
-    <row r="156" spans="2:10">
+    <row r="156" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B156" s="7"/>
       <c r="C156" s="7">
         <v>1024</v>
@@ -4533,7 +4575,7 @@
         <v>10.587436294523441</v>
       </c>
     </row>
-    <row r="157" spans="2:10">
+    <row r="157" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B157" s="7"/>
       <c r="C157" s="7">
         <v>512</v>
@@ -4559,7 +4601,7 @@
         <v>2.7962026666666664</v>
       </c>
     </row>
-    <row r="158" spans="2:10">
+    <row r="158" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B158" s="7"/>
       <c r="C158" s="7">
         <v>1024</v>
@@ -4585,7 +4627,7 @@
         <v>3.7282702222222222</v>
       </c>
     </row>
-    <row r="159" spans="2:10">
+    <row r="159" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C159" s="7">
         <v>512</v>
       </c>
@@ -4611,7 +4653,7 @@
         <v>10.541662757044934</v>
       </c>
     </row>
-    <row r="160" spans="2:10">
+    <row r="160" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C160" s="7">
         <v>512</v>
       </c>
@@ -4637,7 +4679,7 @@
         <v>10.867245600777284</v>
       </c>
     </row>
-    <row r="161" spans="1:31">
+    <row r="161" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B161" s="7"/>
       <c r="C161" s="7">
         <v>512</v>
@@ -4664,7 +4706,7 @@
         <v>10.388797886393661</v>
       </c>
     </row>
-    <row r="162" spans="1:31">
+    <row r="162" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B162" s="7"/>
       <c r="C162" s="7">
         <v>512</v>
@@ -4691,7 +4733,7 @@
         <v>10.303131935881627</v>
       </c>
     </row>
-    <row r="163" spans="1:31">
+    <row r="163" spans="1:31" x14ac:dyDescent="0.2">
       <c r="C163" s="7">
         <v>1024</v>
       </c>
@@ -4717,7 +4759,7 @@
         <v>10.197224886727815</v>
       </c>
     </row>
-    <row r="164" spans="1:31">
+    <row r="164" spans="1:31" x14ac:dyDescent="0.2">
       <c r="C164" s="7">
         <v>1024</v>
       </c>
@@ -4743,7 +4785,7 @@
         <v>10.797886403861627</v>
       </c>
     </row>
-    <row r="165" spans="1:31">
+    <row r="165" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B165" s="7"/>
       <c r="C165" s="7">
         <v>1024</v>
@@ -4770,7 +4812,7 @@
         <v>10.101077305932407</v>
       </c>
     </row>
-    <row r="166" spans="1:31">
+    <row r="166" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B166" s="7"/>
       <c r="C166" s="7">
         <v>1024</v>
@@ -4797,7 +4839,7 @@
         <v>10.347077600440285</v>
       </c>
     </row>
-    <row r="167" spans="1:31">
+    <row r="167" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B167" s="7"/>
       <c r="C167" s="7">
         <v>512</v>
@@ -4823,7 +4865,7 @@
         <v>2.3967451428571431</v>
       </c>
     </row>
-    <row r="168" spans="1:31">
+    <row r="168" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B168" s="7"/>
       <c r="C168" s="7">
         <v>1024</v>
@@ -4849,26 +4891,26 @@
         <v>3.3554431999999994</v>
       </c>
     </row>
-    <row r="169" spans="1:31">
+    <row r="169" spans="1:31" x14ac:dyDescent="0.2">
       <c r="I169" s="6"/>
     </row>
-    <row r="170" spans="1:31">
+    <row r="170" spans="1:31" x14ac:dyDescent="0.2">
       <c r="I170" s="6"/>
     </row>
-    <row r="171" spans="1:31">
+    <row r="171" spans="1:31" x14ac:dyDescent="0.2">
       <c r="I171" s="6"/>
       <c r="J171" s="8"/>
     </row>
-    <row r="172" spans="1:31">
+    <row r="172" spans="1:31" x14ac:dyDescent="0.2">
       <c r="I172" s="6"/>
     </row>
-    <row r="173" spans="1:31">
+    <row r="173" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A173" s="5" t="s">
         <v>10</v>
       </c>
       <c r="I173" s="6"/>
     </row>
-    <row r="174" spans="1:31">
+    <row r="174" spans="1:31" x14ac:dyDescent="0.2">
       <c r="C174" s="5" t="s">
         <v>11</v>
       </c>
@@ -4933,7 +4975,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="175" spans="1:31">
+    <row r="175" spans="1:31" x14ac:dyDescent="0.2">
       <c r="C175" s="5">
         <v>700</v>
       </c>
@@ -5006,7 +5048,7 @@
       <c r="AA175" s="6"/>
       <c r="AE175" s="6"/>
     </row>
-    <row r="176" spans="1:31">
+    <row r="176" spans="1:31" x14ac:dyDescent="0.2">
       <c r="C176" s="5">
         <v>700</v>
       </c>
@@ -5079,7 +5121,7 @@
       <c r="AA176" s="6"/>
       <c r="AE176" s="6"/>
     </row>
-    <row r="177" spans="3:31">
+    <row r="177" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C177" s="5">
         <v>700</v>
       </c>
@@ -5152,7 +5194,7 @@
       <c r="AA177" s="6"/>
       <c r="AE177" s="6"/>
     </row>
-    <row r="178" spans="3:31">
+    <row r="178" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C178" s="5">
         <v>700</v>
       </c>
@@ -5225,7 +5267,7 @@
       <c r="AA178" s="6"/>
       <c r="AE178" s="6"/>
     </row>
-    <row r="179" spans="3:31">
+    <row r="179" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C179" s="5">
         <v>341</v>
       </c>
@@ -5298,7 +5340,7 @@
       <c r="AA179" s="6"/>
       <c r="AE179" s="6"/>
     </row>
-    <row r="180" spans="3:31">
+    <row r="180" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C180" s="5">
         <v>341</v>
       </c>
@@ -5371,7 +5413,7 @@
       <c r="AA180" s="6"/>
       <c r="AE180" s="6"/>
     </row>
-    <row r="181" spans="3:31">
+    <row r="181" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C181" s="5">
         <v>341</v>
       </c>
@@ -5444,7 +5486,7 @@
       <c r="AA181" s="6"/>
       <c r="AE181" s="6"/>
     </row>
-    <row r="182" spans="3:31">
+    <row r="182" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C182" s="5">
         <v>341</v>
       </c>
@@ -5517,7 +5559,7 @@
       <c r="AA182" s="6"/>
       <c r="AE182" s="6"/>
     </row>
-    <row r="183" spans="3:31">
+    <row r="183" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C183" s="5">
         <v>480</v>
       </c>
@@ -5590,7 +5632,7 @@
       <c r="AA183" s="6"/>
       <c r="AE183" s="6"/>
     </row>
-    <row r="184" spans="3:31">
+    <row r="184" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C184" s="5">
         <v>240</v>
       </c>
@@ -5663,7 +5705,7 @@
       <c r="AA184" s="6"/>
       <c r="AE184" s="6"/>
     </row>
-    <row r="185" spans="3:31">
+    <row r="185" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C185" s="5">
         <v>120</v>
       </c>
@@ -5736,7 +5778,7 @@
       <c r="AA185" s="6"/>
       <c r="AE185" s="6"/>
     </row>
-    <row r="186" spans="3:31">
+    <row r="186" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C186" s="5">
         <v>60</v>
       </c>
@@ -5809,7 +5851,7 @@
       <c r="AA186" s="6"/>
       <c r="AE186" s="6"/>
     </row>
-    <row r="187" spans="3:31">
+    <row r="187" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C187" s="5">
         <v>108</v>
       </c>
@@ -5882,7 +5924,7 @@
       <c r="AA187" s="6"/>
       <c r="AE187" s="6"/>
     </row>
-    <row r="188" spans="3:31">
+    <row r="188" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C188" s="5">
         <v>54</v>
       </c>
@@ -5955,7 +5997,7 @@
       <c r="AA188" s="6"/>
       <c r="AE188" s="6"/>
     </row>
-    <row r="189" spans="3:31">
+    <row r="189" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C189" s="5">
         <v>27</v>
       </c>
@@ -6028,7 +6070,7 @@
       <c r="AA189" s="6"/>
       <c r="AE189" s="6"/>
     </row>
-    <row r="190" spans="3:31">
+    <row r="190" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C190" s="5">
         <v>14</v>
       </c>
@@ -6101,7 +6143,7 @@
       <c r="AA190" s="6"/>
       <c r="AE190" s="6"/>
     </row>
-    <row r="191" spans="3:31">
+    <row r="191" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C191" s="5">
         <v>7</v>
       </c>
@@ -6174,7 +6216,7 @@
       <c r="AA191" s="6"/>
       <c r="AE191" s="6"/>
     </row>
-    <row r="192" spans="3:31">
+    <row r="192" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C192" s="5">
         <v>224</v>
       </c>
@@ -6247,7 +6289,7 @@
       <c r="AA192" s="6"/>
       <c r="AE192" s="6"/>
     </row>
-    <row r="193" spans="3:31">
+    <row r="193" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C193" s="5">
         <v>112</v>
       </c>
@@ -6320,7 +6362,7 @@
       <c r="AA193" s="6"/>
       <c r="AE193" s="6"/>
     </row>
-    <row r="194" spans="3:31">
+    <row r="194" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C194" s="5">
         <f>112/2</f>
         <v>56</v>
@@ -6394,7 +6436,7 @@
       <c r="AA194" s="6"/>
       <c r="AE194" s="6"/>
     </row>
-    <row r="195" spans="3:31">
+    <row r="195" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C195" s="5">
         <f>56/2</f>
         <v>28</v>
@@ -6468,7 +6510,7 @@
       <c r="AA195" s="6"/>
       <c r="AE195" s="6"/>
     </row>
-    <row r="196" spans="3:31">
+    <row r="196" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C196" s="5">
         <v>14</v>
       </c>
@@ -6541,7 +6583,7 @@
       <c r="AA196" s="6"/>
       <c r="AE196" s="6"/>
     </row>
-    <row r="197" spans="3:31">
+    <row r="197" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C197" s="5">
         <v>7</v>
       </c>
@@ -6614,7 +6656,7 @@
       <c r="AA197" s="6"/>
       <c r="AE197" s="6"/>
     </row>
-    <row r="198" spans="3:31">
+    <row r="198" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C198" s="5">
         <v>224</v>
       </c>
@@ -6687,7 +6729,7 @@
       <c r="AA198" s="6"/>
       <c r="AE198" s="6"/>
     </row>
-    <row r="199" spans="3:31">
+    <row r="199" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C199" s="5">
         <v>112</v>
       </c>
@@ -6760,7 +6802,7 @@
       <c r="AA199" s="6"/>
       <c r="AE199" s="6"/>
     </row>
-    <row r="200" spans="3:31">
+    <row r="200" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C200" s="5">
         <f>112/2</f>
         <v>56</v>
@@ -6834,7 +6876,7 @@
       <c r="AA200" s="6"/>
       <c r="AE200" s="6"/>
     </row>
-    <row r="201" spans="3:31">
+    <row r="201" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C201" s="5">
         <f>56/2</f>
         <v>28</v>
@@ -6908,7 +6950,7 @@
       <c r="AA201" s="6"/>
       <c r="AE201" s="6"/>
     </row>
-    <row r="202" spans="3:31">
+    <row r="202" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C202" s="5">
         <v>14</v>
       </c>
@@ -6981,7 +7023,7 @@
       <c r="AA202" s="6"/>
       <c r="AE202" s="6"/>
     </row>
-    <row r="203" spans="3:31">
+    <row r="203" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C203" s="5">
         <v>7</v>
       </c>
@@ -7054,7 +7096,7 @@
       <c r="AA203" s="6"/>
       <c r="AE203" s="6"/>
     </row>
-    <row r="204" spans="3:31">
+    <row r="204" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C204" s="5">
         <v>224</v>
       </c>
@@ -7127,7 +7169,7 @@
       <c r="AA204" s="6"/>
       <c r="AE204" s="6"/>
     </row>
-    <row r="205" spans="3:31">
+    <row r="205" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C205" s="5">
         <v>28</v>
       </c>
@@ -7200,7 +7242,7 @@
       <c r="AA205" s="6"/>
       <c r="AE205" s="6"/>
     </row>
-    <row r="206" spans="3:31">
+    <row r="206" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C206" s="5">
         <v>28</v>
       </c>
@@ -7273,7 +7315,7 @@
       <c r="AA206" s="6"/>
       <c r="AE206" s="6"/>
     </row>
-    <row r="207" spans="3:31">
+    <row r="207" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C207" s="5">
         <v>14</v>
       </c>
@@ -7346,7 +7388,7 @@
       <c r="AA207" s="6"/>
       <c r="AE207" s="6"/>
     </row>
-    <row r="208" spans="3:31">
+    <row r="208" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C208" s="5">
         <v>14</v>
       </c>
@@ -7419,7 +7461,7 @@
       <c r="AA208" s="6"/>
       <c r="AE208" s="6"/>
     </row>
-    <row r="209" spans="2:31">
+    <row r="209" spans="2:31" x14ac:dyDescent="0.2">
       <c r="C209" s="5">
         <v>7</v>
       </c>
@@ -7492,7 +7534,7 @@
       <c r="AA209" s="6"/>
       <c r="AE209" s="6"/>
     </row>
-    <row r="210" spans="2:31">
+    <row r="210" spans="2:31" x14ac:dyDescent="0.2">
       <c r="C210" s="5">
         <v>7</v>
       </c>
@@ -7565,7 +7607,7 @@
       <c r="AA210" s="6"/>
       <c r="AE210" s="6"/>
     </row>
-    <row r="211" spans="2:31">
+    <row r="211" spans="2:31" x14ac:dyDescent="0.2">
       <c r="C211" s="5">
         <v>56</v>
       </c>
@@ -7636,7 +7678,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="212" spans="2:31">
+    <row r="212" spans="2:31" x14ac:dyDescent="0.2">
       <c r="C212" s="5">
         <v>56</v>
       </c>
@@ -7707,7 +7749,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="213" spans="2:31">
+    <row r="213" spans="2:31" x14ac:dyDescent="0.2">
       <c r="C213" s="5">
         <v>28</v>
       </c>
@@ -7778,7 +7820,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="214" spans="2:31">
+    <row r="214" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B214" s="7"/>
       <c r="C214" s="7">
         <v>28</v>
@@ -7850,7 +7892,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="215" spans="2:31">
+    <row r="215" spans="2:31" x14ac:dyDescent="0.2">
       <c r="C215" s="5">
         <v>14</v>
       </c>
@@ -7921,7 +7963,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="216" spans="2:31">
+    <row r="216" spans="2:31" x14ac:dyDescent="0.2">
       <c r="C216" s="5">
         <v>14</v>
       </c>
@@ -7992,7 +8034,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="217" spans="2:31">
+    <row r="217" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B217" s="7"/>
       <c r="C217" s="7">
         <v>14</v>
@@ -8064,7 +8106,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="218" spans="2:31">
+    <row r="218" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B218" s="7"/>
       <c r="C218" s="5">
         <v>7</v>
@@ -8136,7 +8178,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="219" spans="2:31">
+    <row r="219" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B219" s="7"/>
       <c r="C219" s="5">
         <v>7</v>
@@ -8208,7 +8250,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="220" spans="2:31">
+    <row r="220" spans="2:31" x14ac:dyDescent="0.2">
       <c r="C220" s="5">
         <v>56</v>
       </c>
@@ -8279,7 +8321,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="221" spans="2:31">
+    <row r="221" spans="2:31" x14ac:dyDescent="0.2">
       <c r="C221" s="5">
         <v>56</v>
       </c>
@@ -8350,7 +8392,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="222" spans="2:31">
+    <row r="222" spans="2:31" x14ac:dyDescent="0.2">
       <c r="C222" s="5">
         <v>28</v>
       </c>
@@ -8421,7 +8463,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="223" spans="2:31">
+    <row r="223" spans="2:31" x14ac:dyDescent="0.2">
       <c r="C223" s="7">
         <v>28</v>
       </c>
@@ -8492,7 +8534,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="224" spans="2:31">
+    <row r="224" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B224" s="7"/>
       <c r="C224" s="5">
         <v>14</v>
@@ -8564,7 +8606,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="225" spans="1:24">
+    <row r="225" spans="1:24" x14ac:dyDescent="0.2">
       <c r="C225" s="5">
         <v>14</v>
       </c>
@@ -8635,7 +8677,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="226" spans="1:24">
+    <row r="226" spans="1:24" x14ac:dyDescent="0.2">
       <c r="C226" s="7">
         <v>14</v>
       </c>
@@ -8706,7 +8748,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="227" spans="1:24">
+    <row r="227" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B227" s="7"/>
       <c r="C227" s="5">
         <v>7</v>
@@ -8778,7 +8820,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="228" spans="1:24">
+    <row r="228" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B228" s="7"/>
       <c r="C228" s="5">
         <v>7</v>
@@ -8850,7 +8892,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="229" spans="1:24">
+    <row r="229" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B229" s="7"/>
       <c r="C229" s="11">
         <v>700</v>
@@ -8922,7 +8964,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="230" spans="1:24">
+    <row r="230" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B230" s="7"/>
       <c r="C230" s="5">
         <v>350</v>
@@ -8994,7 +9036,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="231" spans="1:24">
+    <row r="231" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B231" s="7"/>
       <c r="C231" s="5">
         <v>350</v>
@@ -9066,7 +9108,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="232" spans="1:24">
+    <row r="232" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B232" s="7"/>
       <c r="C232" s="5">
         <v>175</v>
@@ -9138,7 +9180,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="233" spans="1:24">
+    <row r="233" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B233" s="7"/>
       <c r="C233" s="5">
         <v>175</v>
@@ -9210,7 +9252,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="234" spans="1:24">
+    <row r="234" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B234" s="7"/>
       <c r="C234" s="5">
         <v>84</v>
@@ -9282,7 +9324,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="235" spans="1:24">
+    <row r="235" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B235" s="7"/>
       <c r="C235" s="5">
         <v>84</v>
@@ -9354,7 +9396,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="236" spans="1:24">
+    <row r="236" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B236" s="7"/>
       <c r="C236" s="5">
         <v>42</v>
@@ -9426,7 +9468,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="237" spans="1:24">
+    <row r="237" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A237" s="7"/>
       <c r="B237" s="7"/>
       <c r="C237" s="5">
@@ -9499,7 +9541,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="238" spans="1:24">
+    <row r="238" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A238" s="7"/>
       <c r="B238" s="7"/>
       <c r="C238" s="5">
@@ -9572,7 +9614,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="239" spans="1:24">
+    <row r="239" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A239" s="7"/>
       <c r="B239" s="7"/>
       <c r="C239" s="5">
@@ -9645,7 +9687,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="240" spans="1:24">
+    <row r="240" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A240" s="7"/>
       <c r="B240" s="7"/>
       <c r="C240" s="5">
@@ -9718,7 +9760,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="241" spans="1:24">
+    <row r="241" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A241" s="7"/>
       <c r="B241" s="7"/>
       <c r="C241" s="7">
@@ -9791,7 +9833,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="242" spans="1:24">
+    <row r="242" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A242" s="7"/>
       <c r="B242" s="7"/>
       <c r="C242" s="7">
@@ -9864,7 +9906,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="243" spans="1:24">
+    <row r="243" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A243" s="7"/>
       <c r="B243" s="7"/>
       <c r="C243" s="7">
@@ -9937,7 +9979,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="244" spans="1:24">
+    <row r="244" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A244" s="7"/>
       <c r="B244" s="7"/>
       <c r="C244" s="7">
@@ -10010,7 +10052,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="245" spans="1:24">
+    <row r="245" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A245" s="7"/>
       <c r="B245" s="7"/>
       <c r="C245" s="7">
@@ -10083,7 +10125,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="246" spans="1:24">
+    <row r="246" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A246" s="7"/>
       <c r="B246" s="7"/>
       <c r="C246" s="7">
@@ -10156,7 +10198,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="247" spans="1:24">
+    <row r="247" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A247" s="7"/>
       <c r="B247" s="7"/>
       <c r="C247" s="7">
@@ -10229,7 +10271,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="248" spans="1:24">
+    <row r="248" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A248" s="7"/>
       <c r="B248" s="7"/>
       <c r="C248" s="7">
@@ -10302,7 +10344,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="249" spans="1:24">
+    <row r="249" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A249" s="7"/>
       <c r="B249" s="7"/>
       <c r="C249" s="7">
@@ -10375,7 +10417,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="250" spans="1:24">
+    <row r="250" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A250" s="7"/>
       <c r="B250" s="7"/>
       <c r="C250" s="7">
@@ -10448,7 +10490,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="251" spans="1:24">
+    <row r="251" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A251" s="7"/>
       <c r="B251" s="7"/>
       <c r="C251" s="7">
@@ -10521,7 +10563,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="252" spans="1:24">
+    <row r="252" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A252" s="7"/>
       <c r="B252" s="7"/>
       <c r="C252" s="7">
@@ -10594,7 +10636,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="253" spans="1:24">
+    <row r="253" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A253" s="7"/>
       <c r="B253" s="7"/>
       <c r="C253" s="5">
@@ -10667,7 +10709,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="254" spans="1:24">
+    <row r="254" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A254" s="7"/>
       <c r="B254" s="7"/>
       <c r="C254" s="5">
@@ -10740,7 +10782,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="255" spans="1:24">
+    <row r="255" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A255" s="7"/>
       <c r="B255" s="7"/>
       <c r="C255" s="5">
@@ -10813,7 +10855,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="256" spans="1:24">
+    <row r="256" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A256" s="7"/>
       <c r="B256" s="7"/>
       <c r="C256" s="5">
@@ -10886,7 +10928,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="257" spans="1:24">
+    <row r="257" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A257" s="7"/>
       <c r="B257" s="7"/>
       <c r="C257" s="7">
@@ -10959,7 +11001,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="258" spans="1:24">
+    <row r="258" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A258" s="7"/>
       <c r="B258" s="7"/>
       <c r="C258" s="7">
@@ -11032,7 +11074,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="259" spans="1:24">
+    <row r="259" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A259" s="7"/>
       <c r="B259" s="7"/>
       <c r="C259" s="7">
@@ -11105,7 +11147,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="260" spans="1:24">
+    <row r="260" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A260" s="7"/>
       <c r="B260" s="7"/>
       <c r="C260" s="7">
@@ -11178,7 +11220,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="261" spans="1:24">
+    <row r="261" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A261" s="7"/>
       <c r="B261" s="7"/>
       <c r="C261" s="7">
@@ -11251,7 +11293,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="262" spans="1:24">
+    <row r="262" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A262" s="7"/>
       <c r="B262" s="7"/>
       <c r="C262" s="7">
@@ -11324,7 +11366,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="263" spans="1:24">
+    <row r="263" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A263" s="7"/>
       <c r="B263" s="7"/>
       <c r="C263" s="7">
@@ -11397,7 +11439,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="264" spans="1:24">
+    <row r="264" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A264" s="7"/>
       <c r="B264" s="7"/>
       <c r="C264" s="7">
@@ -11470,7 +11512,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="265" spans="1:24">
+    <row r="265" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A265" s="7"/>
       <c r="B265" s="7"/>
       <c r="C265" s="7">
@@ -11543,7 +11585,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="266" spans="1:24">
+    <row r="266" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A266" s="7"/>
       <c r="B266" s="7"/>
       <c r="C266" s="7">
@@ -11616,7 +11658,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="267" spans="1:24">
+    <row r="267" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A267" s="7"/>
       <c r="B267" s="7"/>
       <c r="C267" s="7">
@@ -11689,7 +11731,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="268" spans="1:24">
+    <row r="268" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A268" s="7"/>
       <c r="B268" s="7"/>
       <c r="C268" s="7">
@@ -11762,18 +11804,18 @@
         <v>31</v>
       </c>
     </row>
-    <row r="270" spans="1:24">
+    <row r="270" spans="1:24" x14ac:dyDescent="0.2">
       <c r="T270" s="6"/>
     </row>
-    <row r="271" spans="1:24">
+    <row r="271" spans="1:24" x14ac:dyDescent="0.2">
       <c r="D271" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="277" spans="1:12">
+    <row r="277" spans="1:12" x14ac:dyDescent="0.2">
       <c r="L277" s="8"/>
     </row>
-    <row r="278" spans="1:12">
+    <row r="278" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A278" s="5" t="s">
         <v>35</v>
       </c>
@@ -11799,7 +11841,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="280" spans="1:12">
+    <row r="280" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C280" s="5">
         <v>1760</v>
       </c>
@@ -11824,7 +11866,7 @@
         <v>1.5713369255150553</v>
       </c>
     </row>
-    <row r="281" spans="1:12">
+    <row r="281" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C281" s="5">
         <v>1760</v>
       </c>
@@ -11849,7 +11891,7 @@
         <v>1.0603289487755319</v>
       </c>
     </row>
-    <row r="282" spans="1:12">
+    <row r="282" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C282" s="5">
         <v>1760</v>
       </c>
@@ -11874,7 +11916,7 @@
         <v>4.5419770957398073</v>
       </c>
     </row>
-    <row r="283" spans="1:12">
+    <row r="283" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C283" s="5">
         <v>1760</v>
       </c>
@@ -11899,7 +11941,7 @@
         <v>6.7599359127322316</v>
       </c>
     </row>
-    <row r="284" spans="1:12">
+    <row r="284" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C284" s="5">
         <v>2048</v>
       </c>
@@ -11924,7 +11966,7 @@
         <v>1.4093060676044509</v>
       </c>
     </row>
-    <row r="285" spans="1:12">
+    <row r="285" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C285" s="5">
         <v>2048</v>
       </c>
@@ -11949,7 +11991,7 @@
         <v>1.2677100661000944</v>
       </c>
     </row>
-    <row r="286" spans="1:12">
+    <row r="286" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C286" s="5">
         <v>2048</v>
       </c>
@@ -11974,7 +12016,7 @@
         <v>2.9143709106697058</v>
       </c>
     </row>
-    <row r="287" spans="1:12">
+    <row r="287" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C287" s="5">
         <v>2048</v>
       </c>
@@ -11999,7 +12041,7 @@
         <v>6.7504963419233182</v>
       </c>
     </row>
-    <row r="288" spans="1:12">
+    <row r="288" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C288" s="5">
         <v>2560</v>
       </c>
@@ -12024,7 +12066,7 @@
         <v>1.3738286612522923</v>
       </c>
     </row>
-    <row r="289" spans="1:10">
+    <row r="289" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C289" s="5">
         <v>2560</v>
       </c>
@@ -12049,7 +12091,7 @@
         <v>1.6128885813148786</v>
       </c>
     </row>
-    <row r="290" spans="1:10">
+    <row r="290" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C290" s="5">
         <v>2560</v>
       </c>
@@ -12074,7 +12116,7 @@
         <v>3.6174210571699579</v>
       </c>
     </row>
-    <row r="291" spans="1:10">
+    <row r="291" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C291" s="5">
         <v>2560</v>
       </c>
@@ -12099,7 +12141,7 @@
         <v>6.9381017117340615</v>
       </c>
     </row>
-    <row r="295" spans="1:10">
+    <row r="295" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A295" s="5" t="s">
         <v>42</v>
       </c>
@@ -12125,7 +12167,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="296" spans="1:10">
+    <row r="296" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C296" s="5">
         <v>512</v>
       </c>
@@ -12150,7 +12192,7 @@
         <v>0.70551791421362486</v>
       </c>
     </row>
-    <row r="297" spans="1:10">
+    <row r="297" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C297" s="5">
         <v>512</v>
       </c>
@@ -12175,7 +12217,7 @@
         <v>0.31732960090788725</v>
       </c>
     </row>
-    <row r="298" spans="1:10">
+    <row r="298" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C298" s="5">
         <v>512</v>
       </c>
@@ -12200,7 +12242,7 @@
         <v>1.7233914740626604</v>
       </c>
     </row>
-    <row r="299" spans="1:10">
+    <row r="299" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C299" s="5">
         <v>512</v>
       </c>
@@ -12225,7 +12267,7 @@
         <v>3.082630408819476</v>
       </c>
     </row>
-    <row r="300" spans="1:10">
+    <row r="300" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C300" s="5">
         <v>1024</v>
       </c>
@@ -12250,7 +12292,7 @@
         <v>1.5384883998165977</v>
       </c>
     </row>
-    <row r="301" spans="1:10">
+    <row r="301" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C301" s="5">
         <v>1024</v>
       </c>
@@ -12275,7 +12317,7 @@
         <v>0.68674645927138767</v>
       </c>
     </row>
-    <row r="302" spans="1:10">
+    <row r="302" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C302" s="5">
         <v>1024</v>
       </c>
@@ -12300,7 +12342,7 @@
         <v>4.3704893520026049</v>
       </c>
     </row>
-    <row r="303" spans="1:10">
+    <row r="303" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C303" s="5">
         <v>1024</v>
       </c>
@@ -12325,7 +12367,7 @@
         <v>6.0994195864576239</v>
       </c>
     </row>
-    <row r="304" spans="1:10">
+    <row r="304" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C304" s="5">
         <v>2048</v>
       </c>
@@ -12350,7 +12392,7 @@
         <v>1.4568297840008682</v>
       </c>
     </row>
-    <row r="305" spans="1:10">
+    <row r="305" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C305" s="5">
         <v>2048</v>
       </c>
@@ -12375,7 +12417,7 @@
         <v>1.416246997995146</v>
       </c>
     </row>
-    <row r="306" spans="1:10">
+    <row r="306" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C306" s="5">
         <v>2048</v>
       </c>
@@ -12400,7 +12442,7 @@
         <v>2.739976074308462</v>
       </c>
     </row>
-    <row r="307" spans="1:10">
+    <row r="307" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C307" s="5">
         <v>2048</v>
       </c>
@@ -12425,7 +12467,7 @@
         <v>8.6731972859450721</v>
       </c>
     </row>
-    <row r="308" spans="1:10">
+    <row r="308" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C308" s="5">
         <v>4096</v>
       </c>
@@ -12450,7 +12492,7 @@
         <v>1.0894517177702467</v>
       </c>
     </row>
-    <row r="309" spans="1:10">
+    <row r="309" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C309" s="5">
         <v>4096</v>
       </c>
@@ -12475,7 +12517,7 @@
         <v>2.4597205781962295</v>
       </c>
     </row>
-    <row r="310" spans="1:10">
+    <row r="310" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C310" s="5">
         <v>4096</v>
       </c>
@@ -12500,7 +12542,7 @@
         <v>4.2892197415463285</v>
       </c>
     </row>
-    <row r="311" spans="1:10">
+    <row r="311" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C311" s="5">
         <v>4096</v>
       </c>
@@ -12525,7 +12567,7 @@
         <v>6.6182311637080868</v>
       </c>
     </row>
-    <row r="312" spans="1:10">
+    <row r="312" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C312" s="5">
         <v>1536</v>
       </c>
@@ -12550,7 +12592,7 @@
         <v>1.2258073063809061</v>
       </c>
     </row>
-    <row r="313" spans="1:10">
+    <row r="313" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C313" s="5">
         <v>1536</v>
       </c>
@@ -12575,7 +12617,7 @@
         <v>1.5523279942428294</v>
       </c>
     </row>
-    <row r="314" spans="1:10">
+    <row r="314" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C314" s="5">
         <v>1536</v>
       </c>
@@ -12600,7 +12642,7 @@
         <v>1.0399100826446281</v>
       </c>
     </row>
-    <row r="315" spans="1:10">
+    <row r="315" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C315" s="5">
         <v>256</v>
       </c>
@@ -12625,7 +12667,7 @@
         <v>0.36303843046739753</v>
       </c>
     </row>
-    <row r="316" spans="1:10">
+    <row r="316" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C316" s="5">
         <v>256</v>
       </c>
@@ -12650,7 +12692,7 @@
         <v>0.17540826653655817</v>
       </c>
     </row>
-    <row r="317" spans="1:10">
+    <row r="317" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C317" s="5">
         <v>256</v>
       </c>
@@ -12675,15 +12717,15 @@
         <v>0.62765491956603059</v>
       </c>
     </row>
-    <row r="318" spans="1:10">
+    <row r="318" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G318" s="6"/>
       <c r="H318" s="6"/>
     </row>
-    <row r="319" spans="1:10">
+    <row r="319" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G319" s="6"/>
       <c r="H319" s="6"/>
     </row>
-    <row r="320" spans="1:10">
+    <row r="320" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A320" s="5" t="s">
         <v>64</v>
       </c>
@@ -12709,7 +12751,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="321" spans="3:10">
+    <row r="321" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C321" s="5">
         <v>2816</v>
       </c>
@@ -12734,7 +12776,7 @@
         <v>1.882635302031348</v>
       </c>
     </row>
-    <row r="322" spans="3:10">
+    <row r="322" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C322" s="5">
         <v>2816</v>
       </c>
@@ -12759,7 +12801,7 @@
         <v>1.8782658951170645</v>
       </c>
     </row>
-    <row r="323" spans="3:10">
+    <row r="323" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C323" s="5">
         <v>2816</v>
       </c>
@@ -12784,7 +12826,7 @@
         <v>1.8763276994718872</v>
       </c>
     </row>
-    <row r="324" spans="3:10">
+    <row r="324" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C324" s="5">
         <v>2816</v>
       </c>
@@ -12809,7 +12851,7 @@
         <v>1.8707278199140569</v>
       </c>
     </row>
-    <row r="325" spans="3:10">
+    <row r="325" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C325" s="5">
         <v>2048</v>
       </c>
@@ -12834,7 +12876,7 @@
         <v>1.3943926362521903</v>
       </c>
     </row>
-    <row r="326" spans="3:10">
+    <row r="326" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C326" s="5">
         <v>2048</v>
       </c>
@@ -12859,7 +12901,7 @@
         <v>1.398593431022026</v>
       </c>
     </row>
-    <row r="327" spans="3:10">
+    <row r="327" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C327" s="5">
         <v>2048</v>
       </c>
@@ -12884,7 +12926,7 @@
         <v>1.3884975585533395</v>
       </c>
     </row>
-    <row r="328" spans="3:10">
+    <row r="328" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C328" s="5">
         <v>2048</v>
       </c>
@@ -12909,7 +12951,7 @@
         <v>1.383560791738635</v>
       </c>
     </row>
-    <row r="329" spans="3:10">
+    <row r="329" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C329" s="5">
         <v>1536</v>
       </c>
@@ -12934,7 +12976,7 @@
         <v>1.0460544921039101</v>
       </c>
     </row>
-    <row r="330" spans="3:10">
+    <row r="330" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C330" s="5">
         <v>1536</v>
       </c>
@@ -12959,7 +13001,7 @@
         <v>1.0463412218348467</v>
       </c>
     </row>
-    <row r="331" spans="3:10">
+    <row r="331" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C331" s="5">
         <v>1536</v>
       </c>
@@ -12984,7 +13026,7 @@
         <v>1.040936043483323</v>
       </c>
     </row>
-    <row r="332" spans="3:10">
+    <row r="332" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C332" s="5">
         <v>1536</v>
       </c>
@@ -13009,7 +13051,7 @@
         <v>1.0276001550835223</v>
       </c>
     </row>
-    <row r="333" spans="3:10">
+    <row r="333" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C333" s="5">
         <v>2560</v>
       </c>
@@ -13034,7 +13076,7 @@
         <v>1.725399369054029</v>
       </c>
     </row>
-    <row r="334" spans="3:10">
+    <row r="334" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C334" s="5">
         <v>2560</v>
       </c>
@@ -13059,7 +13101,7 @@
         <v>1.7204656123239599</v>
       </c>
     </row>
-    <row r="335" spans="3:10">
+    <row r="335" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C335" s="5">
         <v>2560</v>
       </c>
@@ -13084,7 +13126,7 @@
         <v>1.7175879616485032</v>
       </c>
     </row>
-    <row r="336" spans="3:10">
+    <row r="336" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C336" s="5">
         <v>2560</v>
       </c>
@@ -13109,7 +13151,7 @@
         <v>1.7126586145906875</v>
       </c>
     </row>
-    <row r="337" spans="3:10">
+    <row r="337" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C337" s="5">
         <v>512</v>
       </c>
@@ -13134,7 +13176,7 @@
         <v>0.30690029268292685</v>
       </c>
     </row>
-    <row r="338" spans="3:10">
+    <row r="338" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C338" s="5">
         <v>1024</v>
       </c>
@@ -13159,7 +13201,7 @@
         <v>0.68520694850338526</v>
       </c>
     </row>
-    <row r="339" spans="3:10">
+    <row r="339" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C339" s="5">
         <v>1024</v>
       </c>
@@ -13184,14 +13226,885 @@
         <v>3.8577427361509424</v>
       </c>
     </row>
+    <row r="340" spans="1:15" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="341" spans="1:15" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="342" spans="1:15" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="343" spans="1:15" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="344" spans="1:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L344" s="12">
+        <f>1000/(SUM(U180:U215))</f>
+        <v>2.8057013201305985</v>
+      </c>
+    </row>
+    <row r="345" spans="1:15" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="346" spans="1:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I346" s="12"/>
+    </row>
+    <row r="347" spans="1:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G347" s="13"/>
+      <c r="H347" s="13"/>
+      <c r="I347" s="13"/>
+      <c r="K347" s="13"/>
+    </row>
+    <row r="348" spans="1:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A348" t="s">
+        <v>69</v>
+      </c>
+      <c r="C348" t="s">
+        <v>70</v>
+      </c>
+      <c r="D348" t="s">
+        <v>71</v>
+      </c>
+      <c r="G348" t="s">
+        <v>72</v>
+      </c>
+      <c r="I348" t="s">
+        <v>73</v>
+      </c>
+      <c r="J348" t="s">
+        <v>74</v>
+      </c>
+      <c r="K348" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="349" spans="1:15" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="350" spans="1:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C350">
+        <v>100000</v>
+      </c>
+      <c r="D350">
+        <v>2</v>
+      </c>
+      <c r="G350" s="13">
+        <v>6.2329095000000001E-2</v>
+      </c>
+      <c r="H350" s="13"/>
+      <c r="I350" s="13">
+        <v>12.835097316911146</v>
+      </c>
+      <c r="J350" t="s">
+        <v>76</v>
+      </c>
+      <c r="K350" s="13">
+        <v>2.771354371816102E-3</v>
+      </c>
+      <c r="L350" s="14"/>
+      <c r="N350" s="13"/>
+      <c r="O350" s="13"/>
+    </row>
+    <row r="351" spans="1:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C351">
+        <v>100000</v>
+      </c>
+      <c r="D351">
+        <v>4</v>
+      </c>
+      <c r="G351" s="13">
+        <v>9.1073990000000007E-2</v>
+      </c>
+      <c r="H351" s="13"/>
+      <c r="I351" s="13">
+        <v>17.568133338618413</v>
+      </c>
+      <c r="J351" t="s">
+        <v>76</v>
+      </c>
+      <c r="K351" s="13">
+        <v>3.1081657181485163E-3</v>
+      </c>
+      <c r="L351" s="14"/>
+      <c r="N351" s="13"/>
+      <c r="O351" s="13"/>
+    </row>
+    <row r="352" spans="1:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C352">
+        <v>100000</v>
+      </c>
+      <c r="D352">
+        <v>8</v>
+      </c>
+      <c r="G352" s="13">
+        <v>0.1480535</v>
+      </c>
+      <c r="H352" s="13"/>
+      <c r="I352" s="13">
+        <v>21.613808521919442</v>
+      </c>
+      <c r="J352" t="s">
+        <v>76</v>
+      </c>
+      <c r="K352" s="13">
+        <v>2.7382020897316023E-3</v>
+      </c>
+      <c r="L352" s="14"/>
+      <c r="N352" s="13"/>
+      <c r="O352" s="13"/>
+    </row>
+    <row r="353" spans="3:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C353">
+        <v>100000</v>
+      </c>
+      <c r="D353">
+        <v>16</v>
+      </c>
+      <c r="E353">
+        <v>2</v>
+      </c>
+      <c r="G353" s="13">
+        <v>0.50460349999999987</v>
+      </c>
+      <c r="H353" s="13"/>
+      <c r="I353" s="13">
+        <v>12.683225542430842</v>
+      </c>
+      <c r="J353" t="s">
+        <v>76</v>
+      </c>
+      <c r="K353" s="13">
+        <v>1.4179616806863056E-2</v>
+      </c>
+      <c r="L353" s="14"/>
+    </row>
+    <row r="354" spans="3:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C354">
+        <v>100000</v>
+      </c>
+      <c r="D354">
+        <v>32</v>
+      </c>
+      <c r="E354">
+        <v>4</v>
+      </c>
+      <c r="G354" s="13">
+        <v>0.81057659999999987</v>
+      </c>
+      <c r="H354" s="13"/>
+      <c r="I354" s="13">
+        <v>15.79122812082165</v>
+      </c>
+      <c r="J354" t="s">
+        <v>77</v>
+      </c>
+      <c r="K354" s="13">
+        <v>2.8936258206434941E-2</v>
+      </c>
+      <c r="L354" s="14"/>
+    </row>
+    <row r="355" spans="3:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C355">
+        <v>3097600</v>
+      </c>
+      <c r="D355">
+        <v>2</v>
+      </c>
+      <c r="G355" s="13">
+        <v>1.0442000000000005</v>
+      </c>
+      <c r="H355" s="13"/>
+      <c r="I355" s="13">
+        <v>23.731852135606193</v>
+      </c>
+      <c r="J355" t="s">
+        <v>78</v>
+      </c>
+      <c r="K355" s="13">
+        <v>3.4120529396769019E-3</v>
+      </c>
+      <c r="L355" s="14"/>
+      <c r="N355" s="13"/>
+      <c r="O355" s="13"/>
+    </row>
+    <row r="356" spans="3:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C356">
+        <v>3097600</v>
+      </c>
+      <c r="D356">
+        <v>4</v>
+      </c>
+      <c r="G356" s="13">
+        <v>1.7197500000000001</v>
+      </c>
+      <c r="H356" s="13"/>
+      <c r="I356" s="13">
+        <v>28.819072539613313</v>
+      </c>
+      <c r="J356" t="s">
+        <v>78</v>
+      </c>
+      <c r="K356" s="13">
+        <v>2.1974866025578255E-3</v>
+      </c>
+      <c r="L356" s="14"/>
+      <c r="N356" s="13"/>
+      <c r="O356" s="13"/>
+    </row>
+    <row r="357" spans="3:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C357">
+        <v>3097600</v>
+      </c>
+      <c r="D357">
+        <v>8</v>
+      </c>
+      <c r="G357" s="13">
+        <v>2.5057269999999994</v>
+      </c>
+      <c r="H357" s="13"/>
+      <c r="I357" s="13">
+        <v>39.558659023908042</v>
+      </c>
+      <c r="J357" t="s">
+        <v>76</v>
+      </c>
+      <c r="K357" s="13">
+        <v>5.0596776473147715E-3</v>
+      </c>
+      <c r="L357" s="14"/>
+      <c r="N357" s="13"/>
+      <c r="O357" s="13"/>
+    </row>
+    <row r="358" spans="3:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C358">
+        <v>3097600</v>
+      </c>
+      <c r="D358">
+        <v>16</v>
+      </c>
+      <c r="E358">
+        <v>2</v>
+      </c>
+      <c r="G358" s="13">
+        <v>4.4925680000000003</v>
+      </c>
+      <c r="H358" s="13"/>
+      <c r="I358" s="13">
+        <v>44.12763479595634</v>
+      </c>
+      <c r="J358" t="s">
+        <v>76</v>
+      </c>
+      <c r="K358" s="13">
+        <v>0.13407438703550872</v>
+      </c>
+      <c r="L358" s="14"/>
+    </row>
+    <row r="359" spans="3:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C359">
+        <v>3097600</v>
+      </c>
+      <c r="D359">
+        <v>32</v>
+      </c>
+      <c r="E359">
+        <v>4</v>
+      </c>
+      <c r="G359" s="13">
+        <v>4.6311319999999991</v>
+      </c>
+      <c r="H359" s="13"/>
+      <c r="I359" s="13">
+        <v>85.614661814865158</v>
+      </c>
+      <c r="J359" t="s">
+        <v>76</v>
+      </c>
+      <c r="K359" s="13">
+        <v>9.5564268900705421E-2</v>
+      </c>
+      <c r="L359" s="14"/>
+    </row>
+    <row r="360" spans="3:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C360">
+        <v>4194304</v>
+      </c>
+      <c r="D360">
+        <v>2</v>
+      </c>
+      <c r="G360" s="13">
+        <v>1.3991499999999999</v>
+      </c>
+      <c r="H360" s="13"/>
+      <c r="I360" s="13">
+        <v>23.982011935818178</v>
+      </c>
+      <c r="J360" t="s">
+        <v>78</v>
+      </c>
+      <c r="K360" s="13">
+        <v>3.3130523372675203E-3</v>
+      </c>
+      <c r="L360" s="14"/>
+      <c r="N360" s="13"/>
+      <c r="O360" s="13"/>
+    </row>
+    <row r="361" spans="3:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C361">
+        <v>4194304</v>
+      </c>
+      <c r="D361">
+        <v>4</v>
+      </c>
+      <c r="G361" s="13">
+        <v>2.3129999999999997</v>
+      </c>
+      <c r="H361" s="13"/>
+      <c r="I361" s="13">
+        <v>29.01377604842197</v>
+      </c>
+      <c r="J361" t="s">
+        <v>78</v>
+      </c>
+      <c r="K361" s="13">
+        <v>2.3169853371637567E-3</v>
+      </c>
+      <c r="L361" s="14"/>
+      <c r="N361" s="13"/>
+      <c r="O361" s="13"/>
+    </row>
+    <row r="362" spans="3:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C362">
+        <v>4194304</v>
+      </c>
+      <c r="D362">
+        <v>8</v>
+      </c>
+      <c r="G362" s="13">
+        <v>3.3981140000000005</v>
+      </c>
+      <c r="H362" s="13"/>
+      <c r="I362" s="13">
+        <v>39.497711966108255</v>
+      </c>
+      <c r="J362" t="s">
+        <v>76</v>
+      </c>
+      <c r="K362" s="13">
+        <v>1.786874366036955E-3</v>
+      </c>
+      <c r="L362" s="14"/>
+      <c r="N362" s="13"/>
+      <c r="O362" s="13"/>
+    </row>
+    <row r="363" spans="3:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C363">
+        <v>4194304</v>
+      </c>
+      <c r="D363">
+        <v>16</v>
+      </c>
+      <c r="E363">
+        <v>2</v>
+      </c>
+      <c r="G363" s="13">
+        <v>5.9755724999999993</v>
+      </c>
+      <c r="H363" s="13"/>
+      <c r="I363" s="13">
+        <v>44.922131896148869</v>
+      </c>
+      <c r="J363" t="s">
+        <v>76</v>
+      </c>
+      <c r="K363" s="13">
+        <v>7.6055643584500903E-3</v>
+      </c>
+      <c r="L363" s="14"/>
+    </row>
+    <row r="364" spans="3:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C364">
+        <v>4194304</v>
+      </c>
+      <c r="D364">
+        <v>32</v>
+      </c>
+      <c r="E364">
+        <v>4</v>
+      </c>
+      <c r="G364" s="13">
+        <v>6.042124499999999</v>
+      </c>
+      <c r="H364" s="13"/>
+      <c r="I364" s="13">
+        <v>88.854658986255586</v>
+      </c>
+      <c r="J364" t="s">
+        <v>76</v>
+      </c>
+      <c r="K364" s="13">
+        <v>0.19492017565835568</v>
+      </c>
+      <c r="L364" s="14"/>
+    </row>
+    <row r="365" spans="3:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C365">
+        <v>6553600</v>
+      </c>
+      <c r="D365">
+        <v>2</v>
+      </c>
+      <c r="G365" s="13">
+        <v>2.1757000000000004</v>
+      </c>
+      <c r="H365" s="13"/>
+      <c r="I365" s="13">
+        <v>24.097439904398577</v>
+      </c>
+      <c r="J365" t="s">
+        <v>78</v>
+      </c>
+      <c r="K365" s="13">
+        <v>1.8945906376340066E-3</v>
+      </c>
+      <c r="L365" s="14"/>
+      <c r="N365" s="13"/>
+      <c r="O365" s="13"/>
+    </row>
+    <row r="366" spans="3:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C366">
+        <v>6553600</v>
+      </c>
+      <c r="D366">
+        <v>4</v>
+      </c>
+      <c r="G366" s="13">
+        <v>3.5747500000000003</v>
+      </c>
+      <c r="H366" s="13"/>
+      <c r="I366" s="13">
+        <v>29.332848450940624</v>
+      </c>
+      <c r="J366" t="s">
+        <v>78</v>
+      </c>
+      <c r="K366" s="13">
+        <v>3.1434978841042975E-3</v>
+      </c>
+      <c r="L366" s="14"/>
+      <c r="N366" s="13"/>
+      <c r="O366" s="13"/>
+    </row>
+    <row r="367" spans="3:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C367">
+        <v>6553600</v>
+      </c>
+      <c r="D367">
+        <v>8</v>
+      </c>
+      <c r="G367" s="13">
+        <v>5.3133999999999997</v>
+      </c>
+      <c r="H367" s="13"/>
+      <c r="I367" s="13">
+        <v>39.469115820378669</v>
+      </c>
+      <c r="J367" t="s">
+        <v>78</v>
+      </c>
+      <c r="K367" s="13">
+        <v>4.977845655343466E-3</v>
+      </c>
+      <c r="L367" s="14"/>
+      <c r="N367" s="13"/>
+      <c r="O367" s="13"/>
+    </row>
+    <row r="368" spans="3:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C368">
+        <v>6553600</v>
+      </c>
+      <c r="D368">
+        <v>16</v>
+      </c>
+      <c r="E368">
+        <v>2</v>
+      </c>
+      <c r="G368" s="13">
+        <v>9.2212789999999973</v>
+      </c>
+      <c r="H368" s="13"/>
+      <c r="I368" s="13">
+        <v>45.485056899373731</v>
+      </c>
+      <c r="J368" t="s">
+        <v>76</v>
+      </c>
+      <c r="K368" s="13">
+        <v>8.1828182637063429E-3</v>
+      </c>
+      <c r="L368" s="14"/>
+    </row>
+    <row r="369" spans="3:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C369">
+        <v>6553600</v>
+      </c>
+      <c r="D369">
+        <v>32</v>
+      </c>
+      <c r="E369">
+        <v>4</v>
+      </c>
+      <c r="G369" s="13">
+        <v>11.044095</v>
+      </c>
+      <c r="H369" s="13"/>
+      <c r="I369" s="13">
+        <v>75.955594369660886</v>
+      </c>
+      <c r="J369" t="s">
+        <v>76</v>
+      </c>
+      <c r="K369" s="13">
+        <v>0.34646444410114541</v>
+      </c>
+      <c r="L369" s="14"/>
+    </row>
+    <row r="370" spans="3:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C370">
+        <v>16777216</v>
+      </c>
+      <c r="D370">
+        <v>2</v>
+      </c>
+      <c r="G370" s="13">
+        <v>5.5324500000000016</v>
+      </c>
+      <c r="H370" s="13"/>
+      <c r="I370" s="13">
+        <v>24.260088749107531</v>
+      </c>
+      <c r="J370" t="s">
+        <v>78</v>
+      </c>
+      <c r="K370" s="13">
+        <v>3.4101242453056131E-3</v>
+      </c>
+      <c r="L370" s="14"/>
+      <c r="N370" s="13"/>
+      <c r="O370" s="13"/>
+    </row>
+    <row r="371" spans="3:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C371">
+        <v>16777216</v>
+      </c>
+      <c r="D371">
+        <v>4</v>
+      </c>
+      <c r="G371" s="13">
+        <v>9.1451000000000011</v>
+      </c>
+      <c r="H371" s="13"/>
+      <c r="I371" s="13">
+        <v>29.352927360006991</v>
+      </c>
+      <c r="J371" t="s">
+        <v>78</v>
+      </c>
+      <c r="K371" s="13">
+        <v>6.0341135484666842E-3</v>
+      </c>
+      <c r="L371" s="14"/>
+      <c r="N371" s="13"/>
+      <c r="O371" s="13"/>
+    </row>
+    <row r="372" spans="3:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C372">
+        <v>16777216</v>
+      </c>
+      <c r="D372">
+        <v>8</v>
+      </c>
+      <c r="G372" s="13">
+        <v>13.563550000000001</v>
+      </c>
+      <c r="H372" s="13"/>
+      <c r="I372" s="13">
+        <v>39.581887632662536</v>
+      </c>
+      <c r="J372" t="s">
+        <v>78</v>
+      </c>
+      <c r="K372" s="13">
+        <v>8.720665112249169E-3</v>
+      </c>
+      <c r="L372" s="14"/>
+      <c r="N372" s="13"/>
+      <c r="O372" s="13"/>
+    </row>
+    <row r="373" spans="3:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C373">
+        <v>16777216</v>
+      </c>
+      <c r="D373">
+        <v>16</v>
+      </c>
+      <c r="E373">
+        <v>2</v>
+      </c>
+      <c r="G373" s="13">
+        <v>56.937165000000007</v>
+      </c>
+      <c r="H373" s="13"/>
+      <c r="I373" s="13">
+        <v>18.858364725395088</v>
+      </c>
+      <c r="J373" t="s">
+        <v>79</v>
+      </c>
+      <c r="K373" s="13">
+        <v>0.53443442340576508</v>
+      </c>
+      <c r="L373" s="14"/>
+    </row>
+    <row r="374" spans="3:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C374">
+        <v>16777216</v>
+      </c>
+      <c r="D374">
+        <v>32</v>
+      </c>
+      <c r="E374">
+        <v>4</v>
+      </c>
+      <c r="G374" s="13">
+        <v>62.94492000000001</v>
+      </c>
+      <c r="H374" s="13"/>
+      <c r="I374" s="13">
+        <v>34.116869923736488</v>
+      </c>
+      <c r="J374" t="s">
+        <v>79</v>
+      </c>
+      <c r="K374" s="13">
+        <v>0.40676579786873596</v>
+      </c>
+      <c r="L374" s="14"/>
+    </row>
+    <row r="375" spans="3:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C375">
+        <v>38360000</v>
+      </c>
+      <c r="D375">
+        <v>2</v>
+      </c>
+      <c r="G375" s="13">
+        <v>12.584</v>
+      </c>
+      <c r="H375" s="13"/>
+      <c r="I375" s="13">
+        <v>24.386522568340752</v>
+      </c>
+      <c r="J375" t="s">
+        <v>78</v>
+      </c>
+      <c r="K375" s="13">
+        <v>7.5253956007218402E-3</v>
+      </c>
+    </row>
+    <row r="376" spans="3:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C376">
+        <v>38360000</v>
+      </c>
+      <c r="D376">
+        <v>4</v>
+      </c>
+      <c r="G376" s="13">
+        <v>20.795300000000001</v>
+      </c>
+      <c r="H376" s="13"/>
+      <c r="I376" s="13">
+        <v>29.51436141820507</v>
+      </c>
+      <c r="J376" t="s">
+        <v>78</v>
+      </c>
+      <c r="K376" s="13">
+        <v>1.4455375980472994E-2</v>
+      </c>
+    </row>
+    <row r="377" spans="3:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C377">
+        <v>38360000</v>
+      </c>
+      <c r="D377">
+        <v>8</v>
+      </c>
+      <c r="G377" s="13">
+        <v>30.862099999999998</v>
+      </c>
+      <c r="H377" s="13"/>
+      <c r="I377" s="13">
+        <v>39.774351064898376</v>
+      </c>
+      <c r="J377" t="s">
+        <v>78</v>
+      </c>
+      <c r="K377" s="13">
+        <v>1.0036250086036608E-2</v>
+      </c>
+    </row>
+    <row r="378" spans="3:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C378">
+        <v>38360000</v>
+      </c>
+      <c r="D378">
+        <v>16</v>
+      </c>
+      <c r="E378">
+        <v>2</v>
+      </c>
+      <c r="G378" s="13">
+        <v>53.914064999999979</v>
+      </c>
+      <c r="H378" s="13"/>
+      <c r="I378" s="13">
+        <v>45.536169457821465</v>
+      </c>
+      <c r="J378" t="s">
+        <v>76</v>
+      </c>
+      <c r="K378" s="13">
+        <v>4.3722356981296812E-2</v>
+      </c>
+    </row>
+    <row r="379" spans="3:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C379">
+        <v>38360000</v>
+      </c>
+      <c r="D379">
+        <v>32</v>
+      </c>
+      <c r="E379">
+        <v>4</v>
+      </c>
+      <c r="G379" s="13">
+        <v>92.531665000000004</v>
+      </c>
+      <c r="H379" s="13"/>
+      <c r="I379" s="13">
+        <v>53.063780922995392</v>
+      </c>
+      <c r="J379" t="s">
+        <v>76</v>
+      </c>
+      <c r="K379" s="13">
+        <v>2.0521634074351365</v>
+      </c>
+    </row>
+    <row r="380" spans="3:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C380">
+        <v>64500000</v>
+      </c>
+      <c r="D380">
+        <v>2</v>
+      </c>
+      <c r="G380" s="13">
+        <v>21.135300000000001</v>
+      </c>
+      <c r="H380" s="13"/>
+      <c r="I380" s="13">
+        <v>24.414131807923237</v>
+      </c>
+      <c r="J380" t="s">
+        <v>78</v>
+      </c>
+      <c r="K380" s="13">
+        <v>1.1580837166357418E-2</v>
+      </c>
+    </row>
+    <row r="381" spans="3:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C381">
+        <v>64500000</v>
+      </c>
+      <c r="D381">
+        <v>4</v>
+      </c>
+      <c r="G381" s="13">
+        <v>35.105649999999997</v>
+      </c>
+      <c r="H381" s="13"/>
+      <c r="I381" s="13">
+        <v>29.396977409619254</v>
+      </c>
+      <c r="J381" t="s">
+        <v>78</v>
+      </c>
+      <c r="K381" s="13">
+        <v>2.0194514627804788E-2</v>
+      </c>
+    </row>
+    <row r="382" spans="3:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C382">
+        <v>64500000</v>
+      </c>
+      <c r="D382">
+        <v>8</v>
+      </c>
+      <c r="G382" s="13">
+        <v>51.816849999999988</v>
+      </c>
+      <c r="H382" s="13"/>
+      <c r="I382" s="13">
+        <v>39.83260271513997</v>
+      </c>
+      <c r="J382" t="s">
+        <v>78</v>
+      </c>
+      <c r="K382" s="13">
+        <v>2.4471842035931668E-2</v>
+      </c>
+    </row>
+    <row r="383" spans="3:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C383">
+        <v>64500000</v>
+      </c>
+      <c r="D383">
+        <v>16</v>
+      </c>
+      <c r="E383">
+        <v>2</v>
+      </c>
+      <c r="G383" s="13">
+        <v>90.647529999999989</v>
+      </c>
+      <c r="H383" s="13"/>
+      <c r="I383" s="13">
+        <v>45.539023512278831</v>
+      </c>
+      <c r="J383" t="s">
+        <v>76</v>
+      </c>
+      <c r="K383" s="13">
+        <v>7.679382582089879E-2</v>
+      </c>
+    </row>
+    <row r="384" spans="3:15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C384">
+        <v>64500000</v>
+      </c>
+      <c r="D384">
+        <v>32</v>
+      </c>
+      <c r="E384">
+        <v>4</v>
+      </c>
+      <c r="G384" s="13">
+        <v>132.04199999999997</v>
+      </c>
+      <c r="H384" s="13"/>
+      <c r="I384" s="13">
+        <v>62.52556004907531</v>
+      </c>
+      <c r="J384" t="s">
+        <v>79</v>
+      </c>
+      <c r="K384" s="13">
+        <v>0.28406578185528109</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -13203,9 +14116,9 @@
       <selection sqref="A1:B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>45</v>
       </c>
@@ -13213,7 +14126,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>46</v>
       </c>
@@ -13221,7 +14134,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>47</v>
       </c>
@@ -13229,7 +14142,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>49</v>
       </c>
@@ -13237,7 +14150,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>50</v>
       </c>
@@ -13245,13 +14158,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>52</v>
       </c>
@@ -13259,7 +14172,7 @@
         <v>375.66</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>53</v>
       </c>
@@ -13267,7 +14180,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>55</v>
       </c>
@@ -13275,19 +14188,19 @@
         <v>3502</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B10" s="5"/>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B11" s="5"/>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>58</v>
       </c>
@@ -13295,10 +14208,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add RNN results for 1080Ti, P100, TitanXp, TitanX, and M40
</commit_message>
<xml_diff>
--- a/results/train/DeepBench_NV_1080Ti.xlsx
+++ b/results/train/DeepBench_NV_1080Ti.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patwarymostofa/Documents/mostofa/deepbench-internal/DeepBench-internal/results/train/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sharan/Desktop/svail_mnt/DeepBench-ext/results/train/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{226F128F-7D3F-894E-A0BC-08A1B326DC20}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6240" yWindow="460" windowWidth="26160" windowHeight="19280" tabRatio="500"/>
+    <workbookView xWindow="6240" yWindow="460" windowWidth="29840" windowHeight="20080" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results - FP32" sheetId="3" r:id="rId1"/>
     <sheet name="Specs" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="88">
   <si>
     <t>Dense Matrix Multiplication</t>
   </si>
@@ -147,9 +148,6 @@
     <t>Time Forward (msec)</t>
   </si>
   <si>
-    <t>Time Backward (msec)</t>
-  </si>
-  <si>
     <t>TERAFLOPS FWD</t>
   </si>
   <si>
@@ -160,9 +158,6 @@
   </si>
   <si>
     <t xml:space="preserve">Time Forward (msec) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time Backward (msec) </t>
   </si>
   <si>
     <t>CPU Model</t>
@@ -269,11 +264,41 @@
   <si>
     <t>Baidu RingAllReduce</t>
   </si>
+  <si>
+    <t>Time Backward wrt inputs (msec)</t>
+  </si>
+  <si>
+    <t>Time Backward wrt weights (msec)</t>
+  </si>
+  <si>
+    <t>TERAFLOPS BWD Inputs</t>
+  </si>
+  <si>
+    <t>TERAFLOPS BWD Params</t>
+  </si>
+  <si>
+    <t>Total Time</t>
+  </si>
+  <si>
+    <t>DeepSpeech</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Machine Translation</t>
+  </si>
+  <si>
+    <t>Language Modelling</t>
+  </si>
+  <si>
+    <t>Speaker ID</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -333,7 +358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -371,6 +396,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -650,11 +677,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE384"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A345" workbookViewId="0">
-      <selection activeCell="B370" sqref="B370"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -665,10 +692,10 @@
     <col min="5" max="6" width="11" style="5"/>
     <col min="7" max="7" width="22.5" style="5" customWidth="1"/>
     <col min="8" max="8" width="32.6640625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="26.1640625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="30.83203125" style="5" customWidth="1"/>
     <col min="10" max="10" width="20" style="5" customWidth="1"/>
-    <col min="11" max="11" width="18.6640625" style="5" customWidth="1"/>
-    <col min="12" max="12" width="19.83203125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="21.1640625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="23" style="5" customWidth="1"/>
     <col min="13" max="13" width="18" style="5" customWidth="1"/>
     <col min="14" max="14" width="20.83203125" style="5" customWidth="1"/>
     <col min="15" max="19" width="11" style="5"/>
@@ -680,10 +707,10 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -9321,7 +9348,7 @@
         <v>21.898438011049727</v>
       </c>
       <c r="X234" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="235" spans="1:24" x14ac:dyDescent="0.2">
@@ -9465,7 +9492,7 @@
         <v>20.457379509677423</v>
       </c>
       <c r="X236" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="237" spans="1:24" x14ac:dyDescent="0.2">
@@ -10487,7 +10514,7 @@
         <v>3.2112639999999999</v>
       </c>
       <c r="X250" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="251" spans="1:24" x14ac:dyDescent="0.2">
@@ -10560,7 +10587,7 @@
         <v>3.2557765702970296</v>
       </c>
       <c r="X251" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="252" spans="1:24" x14ac:dyDescent="0.2">
@@ -11812,1418 +11839,2385 @@
         <v>34</v>
       </c>
     </row>
-    <row r="277" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:13" x14ac:dyDescent="0.2">
       <c r="L277" s="8"/>
     </row>
-    <row r="278" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A278" s="5" t="s">
+    <row r="278" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A278" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C278" s="5" t="s">
+      <c r="B278" s="15"/>
+      <c r="C278" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D278" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E278" s="5" t="s">
+      <c r="D278" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E278" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="G278" s="5" t="s">
+      <c r="F278" s="15"/>
+      <c r="G278" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="H278" s="5" t="s">
+      <c r="H278" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="I278" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="J278" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="I278" s="5" t="s">
+      <c r="K278" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="L278" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="M278" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="279" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A279" s="15"/>
+      <c r="B279" s="15"/>
+      <c r="C279" s="15"/>
+      <c r="D279" s="15"/>
+      <c r="E279" s="15"/>
+      <c r="F279" s="15"/>
+      <c r="G279" s="15"/>
+      <c r="H279" s="15"/>
+      <c r="I279" s="15"/>
+      <c r="J279" s="15"/>
+      <c r="K279" s="15"/>
+      <c r="L279" s="15"/>
+      <c r="M279" s="15"/>
+    </row>
+    <row r="280" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A280" s="15"/>
+      <c r="B280" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C280" s="15">
+        <v>1760</v>
+      </c>
+      <c r="D280" s="15">
+        <v>16</v>
+      </c>
+      <c r="E280" s="15">
+        <v>50</v>
+      </c>
+      <c r="F280" s="15"/>
+      <c r="G280" s="13">
+        <v>4.0789999999999997</v>
+      </c>
+      <c r="H280" s="13">
+        <v>3.6709999999999998</v>
+      </c>
+      <c r="I280" s="13">
+        <v>0.624</v>
+      </c>
+      <c r="J280" s="13">
+        <f>(2*$E280*$D280*$C280*$C280+$E280*$D280*$C280)/(G280/1000)/10^12</f>
+        <v>1.2153880853150281</v>
+      </c>
+      <c r="K280" s="13">
+        <f>(2*$E280*$D280*$C280*$C280+$E280*$D280*$C280)/(H280/1000)/10^12</f>
+        <v>1.3504679923726506</v>
+      </c>
+      <c r="L280" s="13">
+        <f>(2*$E280*$D280*$C280*$C280+$E280*$D280*$C280)/(I280/1000)/10^12</f>
+        <v>7.9448205128205123</v>
+      </c>
+      <c r="M280" s="14">
+        <f>G280+H280+I280</f>
+        <v>8.3740000000000006</v>
+      </c>
+    </row>
+    <row r="281" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A281" s="15"/>
+      <c r="B281" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C281" s="15">
+        <v>1760</v>
+      </c>
+      <c r="D281" s="15">
+        <v>32</v>
+      </c>
+      <c r="E281" s="15">
+        <v>50</v>
+      </c>
+      <c r="F281" s="15"/>
+      <c r="G281" s="13">
+        <v>10.529</v>
+      </c>
+      <c r="H281" s="13">
+        <v>9.93</v>
+      </c>
+      <c r="I281" s="13">
+        <v>1.0620000000000001</v>
+      </c>
+      <c r="J281" s="13">
+        <f t="shared" ref="J281:L291" si="29">(2*$E281*$D281*$C281*$C281+$E281*$D281*$C281)/(G281/1000)/10^12</f>
+        <v>0.94169778706429863</v>
+      </c>
+      <c r="K281" s="13">
+        <f t="shared" si="29"/>
+        <v>0.99850312185297085</v>
+      </c>
+      <c r="L281" s="13">
+        <f t="shared" si="29"/>
+        <v>9.3362862523540482</v>
+      </c>
+      <c r="M281" s="14">
+        <f t="shared" ref="M281:M291" si="30">G281+H281+I281</f>
+        <v>21.521000000000001</v>
+      </c>
+    </row>
+    <row r="282" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A282" s="15"/>
+      <c r="B282" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C282" s="15">
+        <v>1760</v>
+      </c>
+      <c r="D282" s="15">
+        <v>64</v>
+      </c>
+      <c r="E282" s="15">
+        <v>50</v>
+      </c>
+      <c r="F282" s="15"/>
+      <c r="G282" s="13">
+        <v>5.7629999999999999</v>
+      </c>
+      <c r="H282" s="13">
+        <v>5.2110000000000003</v>
+      </c>
+      <c r="I282" s="13">
+        <v>1.9510000000000001</v>
+      </c>
+      <c r="J282" s="13">
+        <f t="shared" si="29"/>
+        <v>3.4409633871247611</v>
+      </c>
+      <c r="K282" s="13">
+        <f t="shared" si="29"/>
+        <v>3.8054638265208212</v>
+      </c>
+      <c r="L282" s="13">
+        <f t="shared" si="29"/>
+        <v>10.164157867760123</v>
+      </c>
+      <c r="M282" s="14">
+        <f t="shared" si="30"/>
+        <v>12.925000000000001</v>
+      </c>
+    </row>
+    <row r="283" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A283" s="15"/>
+      <c r="B283" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C283" s="15">
+        <v>1760</v>
+      </c>
+      <c r="D283" s="15">
+        <v>128</v>
+      </c>
+      <c r="E283" s="15">
+        <v>50</v>
+      </c>
+      <c r="F283" s="15"/>
+      <c r="G283" s="13">
+        <v>6.58</v>
+      </c>
+      <c r="H283" s="13">
+        <v>6.2279999999999998</v>
+      </c>
+      <c r="I283" s="13">
+        <v>3.8929999999999998</v>
+      </c>
+      <c r="J283" s="13">
+        <f t="shared" si="29"/>
+        <v>6.0274382978723411</v>
+      </c>
+      <c r="K283" s="13">
+        <f t="shared" si="29"/>
+        <v>6.3681027617212589</v>
+      </c>
+      <c r="L283" s="13">
+        <f t="shared" si="29"/>
+        <v>10.187655792447984</v>
+      </c>
+      <c r="M283" s="14">
+        <f t="shared" si="30"/>
+        <v>16.701000000000001</v>
+      </c>
+    </row>
+    <row r="284" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A284" s="15"/>
+      <c r="B284" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C284" s="15">
+        <v>2048</v>
+      </c>
+      <c r="D284" s="15">
+        <v>16</v>
+      </c>
+      <c r="E284" s="15">
+        <v>50</v>
+      </c>
+      <c r="F284" s="15"/>
+      <c r="G284" s="13">
+        <v>6.6550000000000002</v>
+      </c>
+      <c r="H284" s="13">
+        <v>5.7320000000000002</v>
+      </c>
+      <c r="I284" s="13">
+        <v>0.78</v>
+      </c>
+      <c r="J284" s="13">
+        <f t="shared" si="29"/>
+        <v>1.0086438467317804</v>
+      </c>
+      <c r="K284" s="13">
+        <f t="shared" si="29"/>
+        <v>1.1710615491974878</v>
+      </c>
+      <c r="L284" s="13">
+        <f t="shared" si="29"/>
+        <v>8.6058010256410249</v>
+      </c>
+      <c r="M284" s="14">
+        <f t="shared" si="30"/>
+        <v>13.167</v>
+      </c>
+    </row>
+    <row r="285" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A285" s="15"/>
+      <c r="B285" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C285" s="15">
+        <v>2048</v>
+      </c>
+      <c r="D285" s="15">
+        <v>32</v>
+      </c>
+      <c r="E285" s="15">
+        <v>50</v>
+      </c>
+      <c r="F285" s="15"/>
+      <c r="G285" s="13">
+        <v>11.954000000000001</v>
+      </c>
+      <c r="H285" s="13">
+        <v>11.215</v>
+      </c>
+      <c r="I285" s="13">
+        <v>1.351</v>
+      </c>
+      <c r="J285" s="13">
+        <f t="shared" si="29"/>
+        <v>1.123059193575372</v>
+      </c>
+      <c r="K285" s="13">
+        <f t="shared" si="29"/>
+        <v>1.1970619349086047</v>
+      </c>
+      <c r="L285" s="13">
+        <f t="shared" si="29"/>
+        <v>9.937120355292377</v>
+      </c>
+      <c r="M285" s="14">
+        <f t="shared" si="30"/>
+        <v>24.52</v>
+      </c>
+    </row>
+    <row r="286" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A286" s="15"/>
+      <c r="B286" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C286" s="15">
+        <v>2048</v>
+      </c>
+      <c r="D286" s="15">
+        <v>64</v>
+      </c>
+      <c r="E286" s="15">
+        <v>50</v>
+      </c>
+      <c r="F286" s="15"/>
+      <c r="G286" s="13">
+        <v>10.64</v>
+      </c>
+      <c r="H286" s="13">
+        <v>9.8480000000000008</v>
+      </c>
+      <c r="I286" s="13">
+        <v>2.5209999999999999</v>
+      </c>
+      <c r="J286" s="13">
+        <f t="shared" si="29"/>
+        <v>2.5235055639097745</v>
+      </c>
+      <c r="K286" s="13">
+        <f t="shared" si="29"/>
+        <v>2.7264519902518276</v>
+      </c>
+      <c r="L286" s="13">
+        <f t="shared" si="29"/>
+        <v>10.650574851249505</v>
+      </c>
+      <c r="M286" s="14">
+        <f t="shared" si="30"/>
+        <v>23.009</v>
+      </c>
+    </row>
+    <row r="287" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A287" s="15"/>
+      <c r="B287" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C287" s="15">
+        <v>2048</v>
+      </c>
+      <c r="D287" s="15">
+        <v>128</v>
+      </c>
+      <c r="E287" s="15">
+        <v>50</v>
+      </c>
+      <c r="F287" s="15"/>
+      <c r="G287" s="13">
+        <v>9.0299999999999994</v>
+      </c>
+      <c r="H287" s="13">
+        <v>8.782</v>
+      </c>
+      <c r="I287" s="13">
+        <v>4.8609999999999998</v>
+      </c>
+      <c r="J287" s="13">
+        <f t="shared" si="29"/>
+        <v>5.9468658250276851</v>
+      </c>
+      <c r="K287" s="13">
+        <f t="shared" si="29"/>
+        <v>6.1148028239580965</v>
+      </c>
+      <c r="L287" s="13">
+        <f t="shared" si="29"/>
+        <v>11.047150462867723</v>
+      </c>
+      <c r="M287" s="14">
+        <f t="shared" si="30"/>
+        <v>22.672999999999998</v>
+      </c>
+    </row>
+    <row r="288" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A288" s="15"/>
+      <c r="B288" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C288" s="15">
+        <v>2560</v>
+      </c>
+      <c r="D288" s="15">
+        <v>16</v>
+      </c>
+      <c r="E288" s="15">
+        <v>50</v>
+      </c>
+      <c r="F288" s="15"/>
+      <c r="G288" s="13">
+        <v>10.359</v>
+      </c>
+      <c r="H288" s="13">
+        <v>9.1669999999999998</v>
+      </c>
+      <c r="I288" s="13">
+        <v>1.2230000000000001</v>
+      </c>
+      <c r="J288" s="13">
+        <f t="shared" si="29"/>
+        <v>1.0124344048653344</v>
+      </c>
+      <c r="K288" s="13">
+        <f t="shared" si="29"/>
+        <v>1.1440829060761428</v>
+      </c>
+      <c r="L288" s="13">
+        <f t="shared" si="29"/>
+        <v>8.5754766966475877</v>
+      </c>
+      <c r="M288" s="14">
+        <f t="shared" si="30"/>
+        <v>20.748999999999999</v>
+      </c>
+    </row>
+    <row r="289" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A289" s="15"/>
+      <c r="B289" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C289" s="15">
+        <v>2560</v>
+      </c>
+      <c r="D289" s="15">
+        <v>32</v>
+      </c>
+      <c r="E289" s="15">
+        <v>50</v>
+      </c>
+      <c r="F289" s="15"/>
+      <c r="G289" s="13">
+        <v>14.692</v>
+      </c>
+      <c r="H289" s="13">
+        <v>13.946999999999999</v>
+      </c>
+      <c r="I289" s="13">
+        <v>2.169</v>
+      </c>
+      <c r="J289" s="13">
+        <f t="shared" si="29"/>
+        <v>1.4276896270078956</v>
+      </c>
+      <c r="K289" s="13">
+        <f t="shared" si="29"/>
+        <v>1.5039518175951818</v>
+      </c>
+      <c r="L289" s="13">
+        <f t="shared" si="29"/>
+        <v>9.670639004149379</v>
+      </c>
+      <c r="M289" s="14">
+        <f t="shared" si="30"/>
+        <v>30.808</v>
+      </c>
+    </row>
+    <row r="290" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A290" s="15"/>
+      <c r="B290" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C290" s="15">
+        <v>2560</v>
+      </c>
+      <c r="D290" s="15">
+        <v>64</v>
+      </c>
+      <c r="E290" s="15">
+        <v>50</v>
+      </c>
+      <c r="F290" s="15"/>
+      <c r="G290" s="13">
+        <v>15.612</v>
+      </c>
+      <c r="H290" s="13">
+        <v>15.25</v>
+      </c>
+      <c r="I290" s="13">
+        <v>3.9769999999999999</v>
+      </c>
+      <c r="J290" s="13">
+        <f t="shared" si="29"/>
+        <v>2.6871145272867021</v>
+      </c>
+      <c r="K290" s="13">
+        <f t="shared" si="29"/>
+        <v>2.7509004590163935</v>
+      </c>
+      <c r="L290" s="13">
+        <f t="shared" si="29"/>
+        <v>10.548461654513453</v>
+      </c>
+      <c r="M290" s="14">
+        <f t="shared" si="30"/>
+        <v>34.838999999999999</v>
+      </c>
+    </row>
+    <row r="291" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A291" s="15"/>
+      <c r="B291" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C291" s="15">
+        <v>2560</v>
+      </c>
+      <c r="D291" s="15">
+        <v>128</v>
+      </c>
+      <c r="E291" s="15">
+        <v>50</v>
+      </c>
+      <c r="F291" s="15"/>
+      <c r="G291" s="13">
+        <v>16.143000000000001</v>
+      </c>
+      <c r="H291" s="13">
+        <v>15.768000000000001</v>
+      </c>
+      <c r="I291" s="13">
+        <v>7.6980000000000004</v>
+      </c>
+      <c r="J291" s="13">
+        <f t="shared" si="29"/>
+        <v>5.1974517747630546</v>
+      </c>
+      <c r="K291" s="13">
+        <f t="shared" si="29"/>
+        <v>5.3210593607305938</v>
+      </c>
+      <c r="L291" s="13">
+        <f t="shared" si="29"/>
+        <v>10.899254871395168</v>
+      </c>
+      <c r="M291" s="14">
+        <f t="shared" si="30"/>
+        <v>39.609000000000002</v>
+      </c>
+    </row>
+    <row r="292" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A292" s="15"/>
+      <c r="B292" s="15"/>
+      <c r="C292" s="15"/>
+      <c r="D292" s="15"/>
+      <c r="E292" s="15"/>
+      <c r="F292" s="15"/>
+      <c r="G292" s="15"/>
+      <c r="H292" s="15"/>
+      <c r="I292" s="15"/>
+      <c r="J292" s="15"/>
+      <c r="K292" s="15"/>
+      <c r="L292" s="15"/>
+      <c r="M292" s="15"/>
+    </row>
+    <row r="293" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A293" s="15"/>
+      <c r="B293" s="15"/>
+      <c r="C293" s="15"/>
+      <c r="D293" s="15"/>
+      <c r="E293" s="15"/>
+      <c r="F293" s="15"/>
+      <c r="G293" s="15"/>
+      <c r="H293" s="15"/>
+      <c r="I293" s="16"/>
+      <c r="J293" s="15"/>
+      <c r="K293" s="15"/>
+      <c r="L293" s="15"/>
+      <c r="M293" s="15"/>
+    </row>
+    <row r="294" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A294" s="15"/>
+      <c r="B294" s="15"/>
+      <c r="C294" s="15"/>
+      <c r="D294" s="15"/>
+      <c r="E294" s="15"/>
+      <c r="F294" s="15"/>
+      <c r="G294" s="15"/>
+      <c r="H294" s="15"/>
+      <c r="I294" s="15"/>
+      <c r="J294" s="15"/>
+      <c r="K294" s="15"/>
+      <c r="L294" s="15"/>
+      <c r="M294" s="15"/>
+    </row>
+    <row r="295" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A295" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B295" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C295" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D295" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E295" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F295" s="15"/>
+      <c r="G295" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="H295" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="I295" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="J295" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K295" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="J278" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="280" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C280" s="5">
-        <v>1760</v>
-      </c>
-      <c r="D280" s="5">
+      <c r="L295" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="M295" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="296" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A296" s="15"/>
+      <c r="B296" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C296" s="15">
+        <v>512</v>
+      </c>
+      <c r="D296" s="15">
         <v>16</v>
       </c>
-      <c r="E280" s="5">
+      <c r="E296" s="15">
+        <v>25</v>
+      </c>
+      <c r="F296" s="15"/>
+      <c r="G296" s="13">
+        <v>1.2589999999999999</v>
+      </c>
+      <c r="H296" s="13">
+        <v>1.4470000000000001</v>
+      </c>
+      <c r="I296" s="13">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="J296" s="13">
+        <f>(8*$E296*$D296*$C296*$C296)/(G296/1000)/10^12</f>
+        <v>0.66629134233518661</v>
+      </c>
+      <c r="K296" s="13">
+        <f>(8*$E296*$D296*$C296*$C296)/(H296/1000)/10^12</f>
+        <v>0.57972411886662045</v>
+      </c>
+      <c r="L296" s="13">
+        <f>(8*$E296*$D296*$C296*$C296)/(I296/1000)/10^12</f>
+        <v>4.8210390804597703</v>
+      </c>
+      <c r="M296" s="14">
+        <f t="shared" ref="M296:M317" si="31">G296+H296+I296</f>
+        <v>2.88</v>
+      </c>
+    </row>
+    <row r="297" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A297" s="15"/>
+      <c r="B297" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C297" s="15">
+        <v>512</v>
+      </c>
+      <c r="D297" s="15">
+        <v>32</v>
+      </c>
+      <c r="E297" s="15">
+        <v>25</v>
+      </c>
+      <c r="F297" s="15"/>
+      <c r="G297" s="13">
+        <v>2.3530000000000002</v>
+      </c>
+      <c r="H297" s="13">
+        <v>5.5640000000000001</v>
+      </c>
+      <c r="I297" s="13">
+        <v>0.27</v>
+      </c>
+      <c r="J297" s="13">
+        <f t="shared" ref="J297:L317" si="32">(8*$E297*$D297*$C297*$C297)/(G297/1000)/10^12</f>
+        <v>0.71301385465363365</v>
+      </c>
+      <c r="K297" s="13">
+        <f t="shared" si="32"/>
+        <v>0.30153156002875631</v>
+      </c>
+      <c r="L297" s="13">
+        <f t="shared" si="32"/>
+        <v>6.2137837037037045</v>
+      </c>
+      <c r="M297" s="14">
+        <f t="shared" si="31"/>
+        <v>8.1869999999999994</v>
+      </c>
+    </row>
+    <row r="298" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A298" s="15"/>
+      <c r="B298" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C298" s="15">
+        <v>512</v>
+      </c>
+      <c r="D298" s="15">
+        <v>64</v>
+      </c>
+      <c r="E298" s="15">
+        <v>25</v>
+      </c>
+      <c r="F298" s="15"/>
+      <c r="G298" s="13">
+        <v>2.0529999999999999</v>
+      </c>
+      <c r="H298" s="13">
+        <v>2.1219999999999999</v>
+      </c>
+      <c r="I298" s="13">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="J298" s="13">
+        <f t="shared" si="32"/>
+        <v>1.6344097418412078</v>
+      </c>
+      <c r="K298" s="13">
+        <f t="shared" si="32"/>
+        <v>1.5812644674835064</v>
+      </c>
+      <c r="L298" s="13">
+        <f t="shared" si="32"/>
+        <v>7.5403217977528083</v>
+      </c>
+      <c r="M298" s="14">
+        <f t="shared" si="31"/>
+        <v>4.62</v>
+      </c>
+    </row>
+    <row r="299" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A299" s="15"/>
+      <c r="B299" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C299" s="15">
+        <v>512</v>
+      </c>
+      <c r="D299" s="15">
+        <v>128</v>
+      </c>
+      <c r="E299" s="15">
+        <v>25</v>
+      </c>
+      <c r="F299" s="15"/>
+      <c r="G299" s="13">
+        <v>2.2970000000000002</v>
+      </c>
+      <c r="H299" s="13">
+        <v>2.5129999999999999</v>
+      </c>
+      <c r="I299" s="13">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="J299" s="13">
+        <f t="shared" si="32"/>
+        <v>2.9215874619068352</v>
+      </c>
+      <c r="K299" s="13">
+        <f t="shared" si="32"/>
+        <v>2.6704681257461202</v>
+      </c>
+      <c r="L299" s="13">
+        <f t="shared" si="32"/>
+        <v>8.8768338624338607</v>
+      </c>
+      <c r="M299" s="14">
+        <f t="shared" si="31"/>
+        <v>5.5660000000000007</v>
+      </c>
+    </row>
+    <row r="300" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A300" s="15"/>
+      <c r="B300" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C300" s="15">
+        <v>1024</v>
+      </c>
+      <c r="D300" s="15">
+        <v>16</v>
+      </c>
+      <c r="E300" s="15">
+        <v>25</v>
+      </c>
+      <c r="F300" s="15"/>
+      <c r="G300" s="13">
+        <v>4.0279999999999996</v>
+      </c>
+      <c r="H300" s="13">
+        <v>2.5470000000000002</v>
+      </c>
+      <c r="I300" s="13">
+        <v>0.53</v>
+      </c>
+      <c r="J300" s="13">
+        <f t="shared" si="32"/>
+        <v>0.83302959285004985</v>
+      </c>
+      <c r="K300" s="13">
+        <f t="shared" si="32"/>
+        <v>1.3174099725166863</v>
+      </c>
+      <c r="L300" s="13">
+        <f t="shared" si="32"/>
+        <v>6.331024905660378</v>
+      </c>
+      <c r="M300" s="14">
+        <f t="shared" si="31"/>
+        <v>7.1049999999999995</v>
+      </c>
+    </row>
+    <row r="301" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A301" s="15"/>
+      <c r="B301" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C301" s="15">
+        <v>1024</v>
+      </c>
+      <c r="D301" s="15">
+        <v>32</v>
+      </c>
+      <c r="E301" s="15">
+        <v>25</v>
+      </c>
+      <c r="F301" s="15"/>
+      <c r="G301" s="13">
+        <v>3.9239999999999999</v>
+      </c>
+      <c r="H301" s="13">
+        <v>10.183999999999999</v>
+      </c>
+      <c r="I301" s="13">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="J301" s="13">
+        <f t="shared" si="32"/>
+        <v>1.7102156982670746</v>
+      </c>
+      <c r="K301" s="13">
+        <f t="shared" si="32"/>
+        <v>0.65896370777690505</v>
+      </c>
+      <c r="L301" s="13">
+        <f t="shared" si="32"/>
+        <v>8.1344077575757581</v>
+      </c>
+      <c r="M301" s="14">
+        <f t="shared" si="31"/>
+        <v>14.932999999999998</v>
+      </c>
+    </row>
+    <row r="302" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A302" s="15"/>
+      <c r="B302" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C302" s="15">
+        <v>1024</v>
+      </c>
+      <c r="D302" s="15">
+        <v>64</v>
+      </c>
+      <c r="E302" s="15">
+        <v>25</v>
+      </c>
+      <c r="F302" s="15"/>
+      <c r="G302" s="13">
+        <v>4.2629999999999999</v>
+      </c>
+      <c r="H302" s="13">
+        <v>3.3660000000000001</v>
+      </c>
+      <c r="I302" s="13">
+        <v>1.423</v>
+      </c>
+      <c r="J302" s="13">
+        <f t="shared" si="32"/>
+        <v>3.1484336851982166</v>
+      </c>
+      <c r="K302" s="13">
+        <f t="shared" si="32"/>
+        <v>3.9874547831253713</v>
+      </c>
+      <c r="L302" s="13">
+        <f t="shared" si="32"/>
+        <v>9.432025860857344</v>
+      </c>
+      <c r="M302" s="14">
+        <f t="shared" si="31"/>
+        <v>9.0519999999999996</v>
+      </c>
+    </row>
+    <row r="303" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A303" s="15"/>
+      <c r="B303" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C303" s="15">
+        <v>1024</v>
+      </c>
+      <c r="D303" s="15">
+        <v>128</v>
+      </c>
+      <c r="E303" s="15">
+        <v>25</v>
+      </c>
+      <c r="F303" s="15"/>
+      <c r="G303" s="13">
+        <v>5.5410000000000004</v>
+      </c>
+      <c r="H303" s="13">
+        <v>4.641</v>
+      </c>
+      <c r="I303" s="13">
+        <v>2.6389999999999998</v>
+      </c>
+      <c r="J303" s="13">
+        <f t="shared" si="32"/>
+        <v>4.8445308789027246</v>
+      </c>
+      <c r="K303" s="13">
+        <f t="shared" si="32"/>
+        <v>5.7840003447532862</v>
+      </c>
+      <c r="L303" s="13">
+        <f t="shared" si="32"/>
+        <v>10.171862675255779</v>
+      </c>
+      <c r="M303" s="14">
+        <f t="shared" si="31"/>
+        <v>12.821</v>
+      </c>
+    </row>
+    <row r="304" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A304" s="15"/>
+      <c r="B304" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C304" s="15">
+        <v>2048</v>
+      </c>
+      <c r="D304" s="15">
+        <v>16</v>
+      </c>
+      <c r="E304" s="15">
+        <v>25</v>
+      </c>
+      <c r="F304" s="15"/>
+      <c r="G304" s="13">
+        <v>20.018000000000001</v>
+      </c>
+      <c r="H304" s="13">
+        <v>9.5090000000000003</v>
+      </c>
+      <c r="I304" s="13">
+        <v>1.756</v>
+      </c>
+      <c r="J304" s="13">
+        <f t="shared" si="32"/>
+        <v>0.67048520331701467</v>
+      </c>
+      <c r="K304" s="13">
+        <f t="shared" si="32"/>
+        <v>1.4114809969502575</v>
+      </c>
+      <c r="L304" s="13">
+        <f t="shared" si="32"/>
+        <v>7.6433785876993161</v>
+      </c>
+      <c r="M304" s="14">
+        <f t="shared" si="31"/>
+        <v>31.283000000000001</v>
+      </c>
+    </row>
+    <row r="305" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A305" s="15"/>
+      <c r="B305" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C305" s="15">
+        <v>2048</v>
+      </c>
+      <c r="D305" s="15">
+        <v>32</v>
+      </c>
+      <c r="E305" s="15">
+        <v>25</v>
+      </c>
+      <c r="F305" s="15"/>
+      <c r="G305" s="13">
+        <v>7.8780000000000001</v>
+      </c>
+      <c r="H305" s="13">
+        <v>20.163</v>
+      </c>
+      <c r="I305" s="13">
+        <v>2.8250000000000002</v>
+      </c>
+      <c r="J305" s="13">
+        <f t="shared" si="32"/>
+        <v>3.4074061436912926</v>
+      </c>
+      <c r="K305" s="13">
+        <f t="shared" si="32"/>
+        <v>1.3313269652333481</v>
+      </c>
+      <c r="L305" s="13">
+        <f t="shared" si="32"/>
+        <v>9.502140035398229</v>
+      </c>
+      <c r="M305" s="14">
+        <f t="shared" si="31"/>
+        <v>30.866</v>
+      </c>
+    </row>
+    <row r="306" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A306" s="15"/>
+      <c r="B306" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C306" s="15">
+        <v>2048</v>
+      </c>
+      <c r="D306" s="15">
+        <v>64</v>
+      </c>
+      <c r="E306" s="15">
+        <v>25</v>
+      </c>
+      <c r="F306" s="15"/>
+      <c r="G306" s="13">
+        <v>10.824</v>
+      </c>
+      <c r="H306" s="13">
+        <v>21.058</v>
+      </c>
+      <c r="I306" s="13">
+        <v>5.1559999999999997</v>
+      </c>
+      <c r="J306" s="13">
+        <f t="shared" si="32"/>
+        <v>4.9600047302291204</v>
+      </c>
+      <c r="K306" s="13">
+        <f t="shared" si="32"/>
+        <v>2.5494867128882133</v>
+      </c>
+      <c r="L306" s="13">
+        <f t="shared" si="32"/>
+        <v>10.412546780449961</v>
+      </c>
+      <c r="M306" s="14">
+        <f t="shared" si="31"/>
+        <v>37.037999999999997</v>
+      </c>
+    </row>
+    <row r="307" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A307" s="15"/>
+      <c r="B307" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C307" s="15">
+        <v>2048</v>
+      </c>
+      <c r="D307" s="15">
+        <v>128</v>
+      </c>
+      <c r="E307" s="15">
+        <v>25</v>
+      </c>
+      <c r="F307" s="15"/>
+      <c r="G307" s="13">
+        <v>16.170999999999999</v>
+      </c>
+      <c r="H307" s="13">
+        <v>13.528</v>
+      </c>
+      <c r="I307" s="13">
+        <v>9.8789999999999996</v>
+      </c>
+      <c r="J307" s="13">
+        <f t="shared" si="32"/>
+        <v>6.6399222311545367</v>
+      </c>
+      <c r="K307" s="13">
+        <f t="shared" si="32"/>
+        <v>7.9371808397397992</v>
+      </c>
+      <c r="L307" s="13">
+        <f t="shared" si="32"/>
+        <v>10.868932321085131</v>
+      </c>
+      <c r="M307" s="14">
+        <f t="shared" si="31"/>
+        <v>39.577999999999996</v>
+      </c>
+    </row>
+    <row r="308" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A308" s="15"/>
+      <c r="B308" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C308" s="15">
+        <v>4096</v>
+      </c>
+      <c r="D308" s="15">
+        <v>16</v>
+      </c>
+      <c r="E308" s="15">
+        <v>25</v>
+      </c>
+      <c r="F308" s="15"/>
+      <c r="G308" s="13">
+        <v>78.805999999999997</v>
+      </c>
+      <c r="H308" s="13">
+        <v>59.868000000000002</v>
+      </c>
+      <c r="I308" s="13">
+        <v>6.5789999999999997</v>
+      </c>
+      <c r="J308" s="13">
+        <f t="shared" si="32"/>
+        <v>0.68125639164530616</v>
+      </c>
+      <c r="K308" s="13">
+        <f t="shared" si="32"/>
+        <v>0.89675772031803291</v>
+      </c>
+      <c r="L308" s="13">
+        <f t="shared" si="32"/>
+        <v>8.1603725794193647</v>
+      </c>
+      <c r="M308" s="14">
+        <f t="shared" si="31"/>
+        <v>145.25300000000001</v>
+      </c>
+    </row>
+    <row r="309" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A309" s="15"/>
+      <c r="B309" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C309" s="15">
+        <v>4096</v>
+      </c>
+      <c r="D309" s="15">
+        <v>32</v>
+      </c>
+      <c r="E309" s="15">
+        <v>25</v>
+      </c>
+      <c r="F309" s="15"/>
+      <c r="G309" s="13">
+        <v>23.265000000000001</v>
+      </c>
+      <c r="H309" s="13">
+        <v>47.344000000000001</v>
+      </c>
+      <c r="I309" s="13">
+        <v>11.05</v>
+      </c>
+      <c r="J309" s="13">
+        <f t="shared" si="32"/>
+        <v>4.6152668128089402</v>
+      </c>
+      <c r="K309" s="13">
+        <f t="shared" si="32"/>
+        <v>2.2679575532274412</v>
+      </c>
+      <c r="L309" s="13">
+        <f t="shared" si="32"/>
+        <v>9.7171205791855204</v>
+      </c>
+      <c r="M309" s="14">
+        <f t="shared" si="31"/>
+        <v>81.659000000000006</v>
+      </c>
+    </row>
+    <row r="310" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A310" s="15"/>
+      <c r="B310" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C310" s="15">
+        <v>4096</v>
+      </c>
+      <c r="D310" s="15">
+        <v>64</v>
+      </c>
+      <c r="E310" s="15">
+        <v>25</v>
+      </c>
+      <c r="F310" s="15"/>
+      <c r="G310" s="13">
+        <v>47.372</v>
+      </c>
+      <c r="H310" s="13">
+        <v>51.853999999999999</v>
+      </c>
+      <c r="I310" s="13">
+        <v>20.285</v>
+      </c>
+      <c r="J310" s="13">
+        <f t="shared" si="32"/>
+        <v>4.5332340792029049</v>
+      </c>
+      <c r="K310" s="13">
+        <f t="shared" si="32"/>
+        <v>4.1414040344042888</v>
+      </c>
+      <c r="L310" s="13">
+        <f t="shared" si="32"/>
+        <v>10.58655976337195</v>
+      </c>
+      <c r="M310" s="14">
+        <f t="shared" si="31"/>
+        <v>119.511</v>
+      </c>
+    </row>
+    <row r="311" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A311" s="15"/>
+      <c r="B311" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C311" s="15">
+        <v>4096</v>
+      </c>
+      <c r="D311" s="15">
+        <v>128</v>
+      </c>
+      <c r="E311" s="15">
+        <v>25</v>
+      </c>
+      <c r="F311" s="15"/>
+      <c r="G311" s="13">
+        <v>52.192</v>
+      </c>
+      <c r="H311" s="13">
+        <v>66.594999999999999</v>
+      </c>
+      <c r="I311" s="13">
+        <v>38.988999999999997</v>
+      </c>
+      <c r="J311" s="13">
+        <f t="shared" si="32"/>
+        <v>8.2291678724708763</v>
+      </c>
+      <c r="K311" s="13">
+        <f t="shared" si="32"/>
+        <v>6.4493840318342217</v>
+      </c>
+      <c r="L311" s="13">
+        <f t="shared" si="32"/>
+        <v>11.015843689245685</v>
+      </c>
+      <c r="M311" s="14">
+        <f t="shared" si="31"/>
+        <v>157.77600000000001</v>
+      </c>
+    </row>
+    <row r="312" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A312" s="15"/>
+      <c r="B312" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C312" s="15">
+        <v>1536</v>
+      </c>
+      <c r="D312" s="15">
+        <v>8</v>
+      </c>
+      <c r="E312" s="15">
         <v>50</v>
       </c>
-      <c r="G280" s="6">
-        <v>4.2770000000000001</v>
-      </c>
-      <c r="H280" s="6">
-        <v>3.1550000000000002</v>
-      </c>
-      <c r="I280" s="6">
-        <f t="shared" ref="I280:I291" si="29">(2*$E280*$D280*$C280*$C280+$E280*$D280*$C280)/(G280/1000)/10^12</f>
-        <v>1.1591227495908345</v>
-      </c>
-      <c r="J280" s="6">
-        <f t="shared" ref="J280:J291" si="30">(2*$E280*$D280*$C280*$C280+$E280*$D280*$C280)/(H280/1000)/10^12</f>
-        <v>1.5713369255150553</v>
-      </c>
-    </row>
-    <row r="281" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C281" s="5">
-        <v>1760</v>
-      </c>
-      <c r="D281" s="5">
+      <c r="F312" s="15"/>
+      <c r="G312" s="13">
+        <v>11.683</v>
+      </c>
+      <c r="H312" s="13">
+        <v>7.2060000000000004</v>
+      </c>
+      <c r="I312" s="13">
+        <v>1.075</v>
+      </c>
+      <c r="J312" s="13">
+        <f t="shared" si="32"/>
+        <v>0.64621648549174016</v>
+      </c>
+      <c r="K312" s="13">
+        <f t="shared" si="32"/>
+        <v>1.0477029142381347</v>
+      </c>
+      <c r="L312" s="13">
+        <f t="shared" si="32"/>
+        <v>7.0230206511627911</v>
+      </c>
+      <c r="M312" s="14">
+        <f t="shared" si="31"/>
+        <v>19.963999999999999</v>
+      </c>
+    </row>
+    <row r="313" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A313" s="15"/>
+      <c r="B313" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C313" s="15">
+        <v>1536</v>
+      </c>
+      <c r="D313" s="15">
+        <v>16</v>
+      </c>
+      <c r="E313" s="15">
+        <v>50</v>
+      </c>
+      <c r="F313" s="15"/>
+      <c r="G313" s="13">
+        <v>21.974</v>
+      </c>
+      <c r="H313" s="13">
+        <v>10.997</v>
+      </c>
+      <c r="I313" s="13">
+        <v>1.78</v>
+      </c>
+      <c r="J313" s="13">
+        <f t="shared" si="32"/>
+        <v>0.68715274415217986</v>
+      </c>
+      <c r="K313" s="13">
+        <f t="shared" si="32"/>
+        <v>1.3730557788487769</v>
+      </c>
+      <c r="L313" s="13">
+        <f t="shared" si="32"/>
+        <v>8.4828620224719096</v>
+      </c>
+      <c r="M313" s="14">
+        <f t="shared" si="31"/>
+        <v>34.751000000000005</v>
+      </c>
+    </row>
+    <row r="314" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A314" s="15"/>
+      <c r="B314" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C314" s="15">
+        <v>1536</v>
+      </c>
+      <c r="D314" s="15">
         <v>32</v>
       </c>
-      <c r="E281" s="5">
+      <c r="E314" s="15">
         <v>50</v>
       </c>
-      <c r="G281" s="6">
-        <v>9.9870000000000001</v>
-      </c>
-      <c r="H281" s="6">
-        <v>9.3510000000000009</v>
-      </c>
-      <c r="I281" s="6">
-        <f t="shared" si="29"/>
-        <v>0.99280424551917501</v>
-      </c>
-      <c r="J281" s="6">
-        <f t="shared" si="30"/>
-        <v>1.0603289487755319</v>
-      </c>
-    </row>
-    <row r="282" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C282" s="5">
-        <v>1760</v>
-      </c>
-      <c r="D282" s="5">
+      <c r="F314" s="15"/>
+      <c r="G314" s="13">
+        <v>11.484999999999999</v>
+      </c>
+      <c r="H314" s="13">
+        <v>30.913</v>
+      </c>
+      <c r="I314" s="13">
+        <v>3.06</v>
+      </c>
+      <c r="J314" s="13">
+        <f t="shared" si="32"/>
+        <v>2.629428715716152</v>
+      </c>
+      <c r="K314" s="13">
+        <f t="shared" si="32"/>
+        <v>0.97690255879403487</v>
+      </c>
+      <c r="L314" s="13">
+        <f t="shared" si="32"/>
+        <v>9.8689505882352933</v>
+      </c>
+      <c r="M314" s="14">
+        <f t="shared" si="31"/>
+        <v>45.457999999999998</v>
+      </c>
+    </row>
+    <row r="315" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A315" s="15"/>
+      <c r="B315" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C315" s="15">
+        <v>256</v>
+      </c>
+      <c r="D315" s="15">
+        <v>16</v>
+      </c>
+      <c r="E315" s="15">
+        <v>150</v>
+      </c>
+      <c r="F315" s="15"/>
+      <c r="G315" s="13">
+        <v>3.714</v>
+      </c>
+      <c r="H315" s="13">
+        <v>4.2549999999999999</v>
+      </c>
+      <c r="I315" s="13">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="J315" s="13">
+        <f t="shared" si="32"/>
+        <v>0.33879676898222943</v>
+      </c>
+      <c r="K315" s="13">
+        <f t="shared" si="32"/>
+        <v>0.29572061104582842</v>
+      </c>
+      <c r="L315" s="13">
+        <f t="shared" si="32"/>
+        <v>5.9353358490566039</v>
+      </c>
+      <c r="M315" s="14">
+        <f t="shared" si="31"/>
+        <v>8.1809999999999992</v>
+      </c>
+    </row>
+    <row r="316" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A316" s="15"/>
+      <c r="B316" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C316" s="15">
+        <v>256</v>
+      </c>
+      <c r="D316" s="15">
+        <v>32</v>
+      </c>
+      <c r="E316" s="15">
+        <v>150</v>
+      </c>
+      <c r="F316" s="15"/>
+      <c r="G316" s="13">
+        <v>6.8609999999999998</v>
+      </c>
+      <c r="H316" s="13">
+        <v>14.831</v>
+      </c>
+      <c r="I316" s="13">
+        <v>0.33900000000000002</v>
+      </c>
+      <c r="J316" s="13">
+        <f t="shared" si="32"/>
+        <v>0.36679527765631831</v>
+      </c>
+      <c r="K316" s="13">
+        <f t="shared" si="32"/>
+        <v>0.16968393230395795</v>
+      </c>
+      <c r="L316" s="13">
+        <f t="shared" si="32"/>
+        <v>7.4235469026548673</v>
+      </c>
+      <c r="M316" s="14">
+        <f t="shared" si="31"/>
+        <v>22.030999999999999</v>
+      </c>
+    </row>
+    <row r="317" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A317" s="15"/>
+      <c r="B317" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C317" s="15">
+        <v>256</v>
+      </c>
+      <c r="D317" s="15">
         <v>64</v>
       </c>
-      <c r="E282" s="5">
-        <v>50</v>
-      </c>
-      <c r="G282" s="6">
-        <v>4.944</v>
-      </c>
-      <c r="H282" s="6">
-        <v>4.3659999999999997</v>
-      </c>
-      <c r="I282" s="6">
-        <f t="shared" si="29"/>
-        <v>4.0109773462783176</v>
-      </c>
-      <c r="J282" s="6">
-        <f t="shared" si="30"/>
-        <v>4.5419770957398073</v>
-      </c>
-    </row>
-    <row r="283" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C283" s="5">
-        <v>1760</v>
-      </c>
-      <c r="D283" s="5">
-        <v>128</v>
-      </c>
-      <c r="E283" s="5">
-        <v>50</v>
-      </c>
-      <c r="G283" s="6">
-        <v>6.0910000000000002</v>
-      </c>
-      <c r="H283" s="6">
-        <v>5.867</v>
-      </c>
-      <c r="I283" s="6">
-        <f t="shared" si="29"/>
-        <v>6.5113354129042849</v>
-      </c>
-      <c r="J283" s="6">
-        <f t="shared" si="30"/>
-        <v>6.7599359127322316</v>
-      </c>
-    </row>
-    <row r="284" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C284" s="5">
+      <c r="E317" s="15">
+        <v>150</v>
+      </c>
+      <c r="F317" s="15"/>
+      <c r="G317" s="13">
+        <v>6.4790000000000001</v>
+      </c>
+      <c r="H317" s="13">
+        <v>9.1430000000000007</v>
+      </c>
+      <c r="I317" s="13">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="J317" s="13">
+        <f t="shared" si="32"/>
+        <v>0.77684284611822807</v>
+      </c>
+      <c r="K317" s="13">
+        <f t="shared" si="32"/>
+        <v>0.55049379853439795</v>
+      </c>
+      <c r="L317" s="13">
+        <f t="shared" si="32"/>
+        <v>8.5598040816326542</v>
+      </c>
+      <c r="M317" s="14">
+        <f t="shared" si="31"/>
+        <v>16.21</v>
+      </c>
+    </row>
+    <row r="318" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A318" s="15"/>
+      <c r="B318" s="15"/>
+      <c r="C318" s="15"/>
+      <c r="D318" s="15"/>
+      <c r="E318" s="15"/>
+      <c r="F318" s="15"/>
+      <c r="G318" s="15"/>
+      <c r="H318" s="15"/>
+      <c r="I318" s="15"/>
+      <c r="J318" s="15"/>
+      <c r="K318" s="15"/>
+      <c r="L318" s="15"/>
+      <c r="M318" s="15"/>
+    </row>
+    <row r="319" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A319" s="15"/>
+      <c r="B319" s="15"/>
+      <c r="C319" s="15"/>
+      <c r="D319" s="15"/>
+      <c r="E319" s="15"/>
+      <c r="F319" s="15"/>
+      <c r="G319" s="15"/>
+      <c r="H319" s="15"/>
+      <c r="I319" s="15"/>
+      <c r="J319" s="15"/>
+      <c r="K319" s="15"/>
+      <c r="L319" s="15"/>
+      <c r="M319" s="15"/>
+    </row>
+    <row r="320" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A320" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B320" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C320" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D320" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E320" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F320" s="15"/>
+      <c r="G320" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="H320" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="I320" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="J320" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K320" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="L320" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="M320" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="321" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A321" s="15"/>
+      <c r="B321" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C321" s="15">
+        <v>2816</v>
+      </c>
+      <c r="D321" s="15">
+        <v>32</v>
+      </c>
+      <c r="E321" s="15">
+        <v>1500</v>
+      </c>
+      <c r="F321" s="15"/>
+      <c r="G321" s="13">
+        <v>585.63599999999997</v>
+      </c>
+      <c r="H321" s="13">
+        <v>1261.2339999999999</v>
+      </c>
+      <c r="I321" s="13">
+        <v>217.49100000000001</v>
+      </c>
+      <c r="J321" s="13">
+        <f>(6*$E321*$D321*$C321*$C321)/(G321/1000)/10^12</f>
+        <v>3.8996894453209849</v>
+      </c>
+      <c r="K321" s="13">
+        <f>(6*$E321*$D321*$C321*$C321)/(H321/1000)/10^12</f>
+        <v>1.8107651141659677</v>
+      </c>
+      <c r="L321" s="13">
+        <f>(6*$E321*$D321*$C321*$C321)/(I321/1000)/10^12</f>
+        <v>10.50065762721216</v>
+      </c>
+      <c r="M321" s="14">
+        <f t="shared" ref="M321:M339" si="33">G321+H321+I321</f>
+        <v>2064.3609999999999</v>
+      </c>
+    </row>
+    <row r="322" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A322" s="15"/>
+      <c r="B322" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C322" s="15">
+        <v>2816</v>
+      </c>
+      <c r="D322" s="15">
+        <v>32</v>
+      </c>
+      <c r="E322" s="15">
+        <v>750</v>
+      </c>
+      <c r="F322" s="15"/>
+      <c r="G322" s="13">
+        <v>295.24599999999998</v>
+      </c>
+      <c r="H322" s="13">
+        <v>632.51199999999994</v>
+      </c>
+      <c r="I322" s="13">
+        <v>108.706</v>
+      </c>
+      <c r="J322" s="13">
+        <f>(6*$E322*$D322*$C322*$C322)/(G322/1000)/10^12</f>
+        <v>3.8676197611483305</v>
+      </c>
+      <c r="K322" s="13">
+        <f>(6*$E322*$D322*$C322*$C322)/(H322/1000)/10^12</f>
+        <v>1.8053400789234038</v>
+      </c>
+      <c r="L322" s="13">
+        <f>(6*$E322*$D322*$C322*$C322)/(I322/1000)/10^12</f>
+        <v>10.504473202951081</v>
+      </c>
+      <c r="M322" s="14">
+        <f t="shared" si="33"/>
+        <v>1036.4639999999999</v>
+      </c>
+    </row>
+    <row r="323" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A323" s="15"/>
+      <c r="B323" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C323" s="15">
+        <v>2816</v>
+      </c>
+      <c r="D323" s="15">
+        <v>32</v>
+      </c>
+      <c r="E323" s="15">
+        <v>375</v>
+      </c>
+      <c r="F323" s="15"/>
+      <c r="G323" s="13">
+        <v>148.61500000000001</v>
+      </c>
+      <c r="H323" s="13">
+        <v>317.92399999999998</v>
+      </c>
+      <c r="I323" s="13">
+        <v>54.100999999999999</v>
+      </c>
+      <c r="J323" s="13">
+        <f>(6*$E323*$D323*$C323*$C323)/(G323/1000)/10^12</f>
+        <v>3.8418035326178379</v>
+      </c>
+      <c r="K323" s="13">
+        <f>(6*$E323*$D323*$C323*$C323)/(H323/1000)/10^12</f>
+        <v>1.7958682955674941</v>
+      </c>
+      <c r="L323" s="13">
+        <f>(6*$E323*$D323*$C323*$C323)/(I323/1000)/10^12</f>
+        <v>10.553402561875012</v>
+      </c>
+      <c r="M323" s="14">
+        <f t="shared" si="33"/>
+        <v>520.64</v>
+      </c>
+    </row>
+    <row r="324" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A324" s="15"/>
+      <c r="B324" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C324" s="15">
+        <v>2816</v>
+      </c>
+      <c r="D324" s="15">
+        <v>32</v>
+      </c>
+      <c r="E324" s="15">
+        <v>187</v>
+      </c>
+      <c r="F324" s="15"/>
+      <c r="G324" s="13">
+        <v>75.204999999999998</v>
+      </c>
+      <c r="H324" s="13">
+        <v>159.351</v>
+      </c>
+      <c r="I324" s="13">
+        <v>26.96</v>
+      </c>
+      <c r="J324" s="13">
+        <f>(6*$E324*$D324*$C324*$C324)/(G324/1000)/10^12</f>
+        <v>3.7858327215477696</v>
+      </c>
+      <c r="K324" s="13">
+        <f>(6*$E324*$D324*$C324*$C324)/(H324/1000)/10^12</f>
+        <v>1.7867070167366381</v>
+      </c>
+      <c r="L324" s="13">
+        <f>(6*$E324*$D324*$C324*$C324)/(I324/1000)/10^12</f>
+        <v>10.560591610682492</v>
+      </c>
+      <c r="M324" s="14">
+        <f t="shared" si="33"/>
+        <v>261.51599999999996</v>
+      </c>
+    </row>
+    <row r="325" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A325" s="15"/>
+      <c r="B325" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C325" s="15">
         <v>2048</v>
       </c>
-      <c r="D284" s="5">
-        <v>16</v>
-      </c>
-      <c r="E284" s="5">
-        <v>50</v>
-      </c>
-      <c r="G284" s="6">
-        <v>5.6269999999999998</v>
-      </c>
-      <c r="H284" s="6">
-        <v>4.7629999999999999</v>
-      </c>
-      <c r="I284" s="6">
-        <f t="shared" si="29"/>
-        <v>1.1929135951661631</v>
-      </c>
-      <c r="J284" s="6">
-        <f t="shared" si="30"/>
-        <v>1.4093060676044509</v>
-      </c>
-    </row>
-    <row r="285" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C285" s="5">
+      <c r="D325" s="15">
+        <v>32</v>
+      </c>
+      <c r="E325" s="15">
+        <v>1500</v>
+      </c>
+      <c r="F325" s="15"/>
+      <c r="G325" s="13">
+        <v>392.97899999999998</v>
+      </c>
+      <c r="H325" s="13">
+        <v>903.86400000000003</v>
+      </c>
+      <c r="I325" s="13">
+        <v>115.94199999999999</v>
+      </c>
+      <c r="J325" s="13">
+        <f>(6*$E325*$D325*$C325*$C325)/(G325/1000)/10^12</f>
+        <v>3.0738526791507943</v>
+      </c>
+      <c r="K325" s="13">
+        <f>(6*$E325*$D325*$C325*$C325)/(H325/1000)/10^12</f>
+        <v>1.3364394997477498</v>
+      </c>
+      <c r="L325" s="13">
+        <f>(6*$E325*$D325*$C325*$C325)/(I325/1000)/10^12</f>
+        <v>10.418653740663435</v>
+      </c>
+      <c r="M325" s="14">
+        <f t="shared" si="33"/>
+        <v>1412.7850000000001</v>
+      </c>
+    </row>
+    <row r="326" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A326" s="15"/>
+      <c r="B326" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C326" s="15">
         <v>2048</v>
       </c>
-      <c r="D285" s="5">
+      <c r="D326" s="15">
         <v>32</v>
       </c>
-      <c r="E285" s="5">
-        <v>50</v>
-      </c>
-      <c r="G285" s="6">
-        <v>10.920999999999999</v>
-      </c>
-      <c r="H285" s="6">
-        <v>10.59</v>
-      </c>
-      <c r="I285" s="6">
-        <f t="shared" si="29"/>
-        <v>1.229287574397949</v>
-      </c>
-      <c r="J285" s="6">
-        <f t="shared" si="30"/>
-        <v>1.2677100661000944</v>
-      </c>
-    </row>
-    <row r="286" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C286" s="5">
+      <c r="E326" s="15">
+        <v>750</v>
+      </c>
+      <c r="F326" s="15"/>
+      <c r="G326" s="13">
+        <v>197.22399999999999</v>
+      </c>
+      <c r="H326" s="13">
+        <v>454.303</v>
+      </c>
+      <c r="I326" s="13">
+        <v>57.698</v>
+      </c>
+      <c r="J326" s="13">
+        <f>(6*$E326*$D326*$C326*$C326)/(G326/1000)/10^12</f>
+        <v>3.0624050622642276</v>
+      </c>
+      <c r="K326" s="13">
+        <f>(6*$E326*$D326*$C326*$C326)/(H326/1000)/10^12</f>
+        <v>1.3294646436409179</v>
+      </c>
+      <c r="L326" s="13">
+        <f>(6*$E326*$D326*$C326*$C326)/(I326/1000)/10^12</f>
+        <v>10.467949946271968</v>
+      </c>
+      <c r="M326" s="14">
+        <f t="shared" si="33"/>
+        <v>709.22500000000002</v>
+      </c>
+    </row>
+    <row r="327" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A327" s="15"/>
+      <c r="B327" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C327" s="15">
         <v>2048</v>
       </c>
-      <c r="D286" s="5">
+      <c r="D327" s="15">
+        <v>32</v>
+      </c>
+      <c r="E327" s="15">
+        <v>375</v>
+      </c>
+      <c r="F327" s="15"/>
+      <c r="G327" s="13">
+        <v>99.793999999999997</v>
+      </c>
+      <c r="H327" s="13">
+        <v>228.535</v>
+      </c>
+      <c r="I327" s="13">
+        <v>28.791</v>
+      </c>
+      <c r="J327" s="13">
+        <f>(6*$E327*$D327*$C327*$C327)/(G327/1000)/10^12</f>
+        <v>3.0261327133895826</v>
+      </c>
+      <c r="K327" s="13">
+        <f>(6*$E327*$D327*$C327*$C327)/(H327/1000)/10^12</f>
+        <v>1.3214163607324918</v>
+      </c>
+      <c r="L327" s="13">
+        <f>(6*$E327*$D327*$C327*$C327)/(I327/1000)/10^12</f>
+        <v>10.4890378243201</v>
+      </c>
+      <c r="M327" s="14">
+        <f t="shared" si="33"/>
+        <v>357.12</v>
+      </c>
+    </row>
+    <row r="328" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A328" s="15"/>
+      <c r="B328" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C328" s="15">
+        <v>2048</v>
+      </c>
+      <c r="D328" s="15">
+        <v>32</v>
+      </c>
+      <c r="E328" s="15">
+        <v>187</v>
+      </c>
+      <c r="F328" s="15"/>
+      <c r="G328" s="13">
+        <v>50.968000000000004</v>
+      </c>
+      <c r="H328" s="13">
+        <v>114.82</v>
+      </c>
+      <c r="I328" s="13">
+        <v>14.363</v>
+      </c>
+      <c r="J328" s="13">
+        <f>(6*$E328*$D328*$C328*$C328)/(G328/1000)/10^12</f>
+        <v>2.9546439102181759</v>
+      </c>
+      <c r="K328" s="13">
+        <f>(6*$E328*$D328*$C328*$C328)/(H328/1000)/10^12</f>
+        <v>1.3115510435115836</v>
+      </c>
+      <c r="L328" s="13">
+        <f>(6*$E328*$D328*$C328*$C328)/(I328/1000)/10^12</f>
+        <v>10.484737924946042</v>
+      </c>
+      <c r="M328" s="14">
+        <f t="shared" si="33"/>
+        <v>180.15100000000001</v>
+      </c>
+    </row>
+    <row r="329" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A329" s="15"/>
+      <c r="B329" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C329" s="15">
+        <v>1536</v>
+      </c>
+      <c r="D329" s="15">
+        <v>32</v>
+      </c>
+      <c r="E329" s="15">
+        <v>1500</v>
+      </c>
+      <c r="F329" s="15"/>
+      <c r="G329" s="13">
+        <v>293.21300000000002</v>
+      </c>
+      <c r="H329" s="13">
+        <v>674.33600000000001</v>
+      </c>
+      <c r="I329" s="13">
+        <v>67.492000000000004</v>
+      </c>
+      <c r="J329" s="13">
+        <f>(6*$E329*$D329*$C329*$C329)/(G329/1000)/10^12</f>
+        <v>2.3173503494046988</v>
+      </c>
+      <c r="K329" s="13">
+        <f>(6*$E329*$D329*$C329*$C329)/(H329/1000)/10^12</f>
+        <v>1.0076241636216958</v>
+      </c>
+      <c r="L329" s="13">
+        <f>(6*$E329*$D329*$C329*$C329)/(I329/1000)/10^12</f>
+        <v>10.06752278788597</v>
+      </c>
+      <c r="M329" s="14">
+        <f t="shared" si="33"/>
+        <v>1035.0409999999999</v>
+      </c>
+    </row>
+    <row r="330" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A330" s="15"/>
+      <c r="B330" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C330" s="15">
+        <v>1536</v>
+      </c>
+      <c r="D330" s="15">
+        <v>32</v>
+      </c>
+      <c r="E330" s="15">
+        <v>750</v>
+      </c>
+      <c r="F330" s="15"/>
+      <c r="G330" s="13">
+        <v>148.19800000000001</v>
+      </c>
+      <c r="H330" s="13">
+        <v>339.38</v>
+      </c>
+      <c r="I330" s="13">
+        <v>33.643999999999998</v>
+      </c>
+      <c r="J330" s="13">
+        <f>(6*$E330*$D330*$C330*$C330)/(G330/1000)/10^12</f>
+        <v>2.2924642977638028</v>
+      </c>
+      <c r="K330" s="13">
+        <f>(6*$E330*$D330*$C330*$C330)/(H330/1000)/10^12</f>
+        <v>1.0010567034003182</v>
+      </c>
+      <c r="L330" s="13">
+        <f>(6*$E330*$D330*$C330*$C330)/(I330/1000)/10^12</f>
+        <v>10.098044941148496</v>
+      </c>
+      <c r="M330" s="14">
+        <f t="shared" si="33"/>
+        <v>521.22199999999998</v>
+      </c>
+    </row>
+    <row r="331" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A331" s="15"/>
+      <c r="B331" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C331" s="15">
+        <v>1536</v>
+      </c>
+      <c r="D331" s="15">
+        <v>32</v>
+      </c>
+      <c r="E331" s="15">
+        <v>375</v>
+      </c>
+      <c r="F331" s="15"/>
+      <c r="G331" s="13">
+        <v>75.906000000000006</v>
+      </c>
+      <c r="H331" s="13">
+        <v>171.06</v>
+      </c>
+      <c r="I331" s="13">
+        <v>16.687000000000001</v>
+      </c>
+      <c r="J331" s="13">
+        <f>(6*$E331*$D331*$C331*$C331)/(G331/1000)/10^12</f>
+        <v>2.2378904434432059</v>
+      </c>
+      <c r="K331" s="13">
+        <f>(6*$E331*$D331*$C331*$C331)/(H331/1000)/10^12</f>
+        <v>0.99303935461241677</v>
+      </c>
+      <c r="L331" s="13">
+        <f>(6*$E331*$D331*$C331*$C331)/(I331/1000)/10^12</f>
+        <v>10.179739437885779</v>
+      </c>
+      <c r="M331" s="14">
+        <f t="shared" si="33"/>
+        <v>263.65300000000002</v>
+      </c>
+    </row>
+    <row r="332" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A332" s="15"/>
+      <c r="B332" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C332" s="15">
+        <v>1536</v>
+      </c>
+      <c r="D332" s="15">
+        <v>32</v>
+      </c>
+      <c r="E332" s="15">
+        <v>187</v>
+      </c>
+      <c r="F332" s="15"/>
+      <c r="G332" s="13">
+        <v>39.252000000000002</v>
+      </c>
+      <c r="H332" s="13">
+        <v>86.341999999999999</v>
+      </c>
+      <c r="I332" s="13">
+        <v>8.2550000000000008</v>
+      </c>
+      <c r="J332" s="13">
+        <f>(6*$E332*$D332*$C332*$C332)/(G332/1000)/10^12</f>
+        <v>2.1580598080097828</v>
+      </c>
+      <c r="K332" s="13">
+        <f>(6*$E332*$D332*$C332*$C332)/(H332/1000)/10^12</f>
+        <v>0.98107715345949831</v>
+      </c>
+      <c r="L332" s="13">
+        <f>(6*$E332*$D332*$C332*$C332)/(I332/1000)/10^12</f>
+        <v>10.261437139188372</v>
+      </c>
+      <c r="M332" s="14">
+        <f t="shared" si="33"/>
+        <v>133.84899999999999</v>
+      </c>
+    </row>
+    <row r="333" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A333" s="15"/>
+      <c r="B333" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C333" s="15">
+        <v>2560</v>
+      </c>
+      <c r="D333" s="15">
+        <v>32</v>
+      </c>
+      <c r="E333" s="15">
+        <v>1500</v>
+      </c>
+      <c r="F333" s="15"/>
+      <c r="G333" s="13">
+        <v>521.322</v>
+      </c>
+      <c r="H333" s="13">
+        <v>1140.662</v>
+      </c>
+      <c r="I333" s="13">
+        <v>181.99100000000001</v>
+      </c>
+      <c r="J333" s="13">
+        <f>(6*$E333*$D333*$C333*$C333)/(G333/1000)/10^12</f>
+        <v>3.6204817751792562</v>
+      </c>
+      <c r="K333" s="13">
+        <f>(6*$E333*$D333*$C333*$C333)/(H333/1000)/10^12</f>
+        <v>1.65468543705322</v>
+      </c>
+      <c r="L333" s="13">
+        <f>(6*$E333*$D333*$C333*$C333)/(I333/1000)/10^12</f>
+        <v>10.371044721991746</v>
+      </c>
+      <c r="M333" s="14">
+        <f t="shared" si="33"/>
+        <v>1843.9749999999999</v>
+      </c>
+    </row>
+    <row r="334" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A334" s="15"/>
+      <c r="B334" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C334" s="15">
+        <v>2560</v>
+      </c>
+      <c r="D334" s="15">
+        <v>32</v>
+      </c>
+      <c r="E334" s="15">
+        <v>750</v>
+      </c>
+      <c r="F334" s="15"/>
+      <c r="G334" s="13">
+        <v>262.81</v>
+      </c>
+      <c r="H334" s="13">
+        <v>572.12400000000002</v>
+      </c>
+      <c r="I334" s="13">
+        <v>90.897000000000006</v>
+      </c>
+      <c r="J334" s="13">
+        <f>(6*$E334*$D334*$C334*$C334)/(G334/1000)/10^12</f>
+        <v>3.5908770594726231</v>
+      </c>
+      <c r="K334" s="13">
+        <f>(6*$E334*$D334*$C334*$C334)/(H334/1000)/10^12</f>
+        <v>1.649499758793548</v>
+      </c>
+      <c r="L334" s="13">
+        <f>(6*$E334*$D334*$C334*$C334)/(I334/1000)/10^12</f>
+        <v>10.382283243671408</v>
+      </c>
+      <c r="M334" s="14">
+        <f t="shared" si="33"/>
+        <v>925.83100000000002</v>
+      </c>
+    </row>
+    <row r="335" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A335" s="15"/>
+      <c r="B335" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C335" s="15">
+        <v>2560</v>
+      </c>
+      <c r="D335" s="15">
+        <v>32</v>
+      </c>
+      <c r="E335" s="15">
+        <v>375</v>
+      </c>
+      <c r="F335" s="15"/>
+      <c r="G335" s="13">
+        <v>132.14400000000001</v>
+      </c>
+      <c r="H335" s="13">
+        <v>287.13</v>
+      </c>
+      <c r="I335" s="13">
+        <v>45.295000000000002</v>
+      </c>
+      <c r="J335" s="13">
+        <f>(6*$E335*$D335*$C335*$C335)/(G335/1000)/10^12</f>
+        <v>3.5707954958227384</v>
+      </c>
+      <c r="K335" s="13">
+        <f>(6*$E335*$D335*$C335*$C335)/(H335/1000)/10^12</f>
+        <v>1.6433643297461082</v>
+      </c>
+      <c r="L335" s="13">
+        <f>(6*$E335*$D335*$C335*$C335)/(I335/1000)/10^12</f>
+        <v>10.417467711667953</v>
+      </c>
+      <c r="M335" s="14">
+        <f t="shared" si="33"/>
+        <v>464.56900000000002</v>
+      </c>
+    </row>
+    <row r="336" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A336" s="15"/>
+      <c r="B336" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C336" s="15">
+        <v>2560</v>
+      </c>
+      <c r="D336" s="15">
+        <v>32</v>
+      </c>
+      <c r="E336" s="15">
+        <v>187</v>
+      </c>
+      <c r="F336" s="15"/>
+      <c r="G336" s="13">
+        <v>66.885999999999996</v>
+      </c>
+      <c r="H336" s="13">
+        <v>144.10900000000001</v>
+      </c>
+      <c r="I336" s="13">
+        <v>22.536000000000001</v>
+      </c>
+      <c r="J336" s="13">
+        <f>(6*$E336*$D336*$C336*$C336)/(G336/1000)/10^12</f>
+        <v>3.5179328170319648</v>
+      </c>
+      <c r="K336" s="13">
+        <f>(6*$E336*$D336*$C336*$C336)/(H336/1000)/10^12</f>
+        <v>1.6327949982305059</v>
+      </c>
+      <c r="L336" s="13">
+        <f>(6*$E336*$D336*$C336*$C336)/(I336/1000)/10^12</f>
+        <v>10.441092225772097</v>
+      </c>
+      <c r="M336" s="14">
+        <f t="shared" si="33"/>
+        <v>233.53100000000001</v>
+      </c>
+    </row>
+    <row r="337" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A337" s="15"/>
+      <c r="B337" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C337" s="15">
+        <v>512</v>
+      </c>
+      <c r="D337" s="15">
+        <v>32</v>
+      </c>
+      <c r="E337" s="15">
+        <v>1</v>
+      </c>
+      <c r="F337" s="15"/>
+      <c r="G337" s="13">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="H337" s="13">
+        <v>0.183</v>
+      </c>
+      <c r="I337" s="13">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="J337" s="13">
+        <f>(6*$E337*$D337*$C337*$C337)/(G337/1000)/10^12</f>
+        <v>0.57195054545454538</v>
+      </c>
+      <c r="K337" s="13">
+        <f>(6*$E337*$D337*$C337*$C337)/(H337/1000)/10^12</f>
+        <v>0.27503632786885246</v>
+      </c>
+      <c r="L337" s="13">
+        <f>(6*$E337*$D337*$C337*$C337)/(I337/1000)/10^12</f>
+        <v>1.3245170526315788</v>
+      </c>
+      <c r="M337" s="14">
+        <f t="shared" si="33"/>
+        <v>0.309</v>
+      </c>
+    </row>
+    <row r="338" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A338" s="15"/>
+      <c r="B338" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C338" s="15">
+        <v>1024</v>
+      </c>
+      <c r="D338" s="15">
+        <v>32</v>
+      </c>
+      <c r="E338" s="15">
+        <v>1500</v>
+      </c>
+      <c r="F338" s="15"/>
+      <c r="G338" s="13">
+        <v>177.661</v>
+      </c>
+      <c r="H338" s="13">
+        <v>454.89</v>
+      </c>
+      <c r="I338" s="13">
+        <v>31.425999999999998</v>
+      </c>
+      <c r="J338" s="13">
+        <f>(6*$E338*$D338*$C338*$C338)/(G338/1000)/10^12</f>
+        <v>1.6998096824851823</v>
+      </c>
+      <c r="K338" s="13">
+        <f>(6*$E338*$D338*$C338*$C338)/(H338/1000)/10^12</f>
+        <v>0.66387453670118057</v>
+      </c>
+      <c r="L338" s="13">
+        <f>(6*$E338*$D338*$C338*$C338)/(I338/1000)/10^12</f>
+        <v>9.6095553999872738</v>
+      </c>
+      <c r="M338" s="14">
+        <f t="shared" si="33"/>
+        <v>663.97699999999998</v>
+      </c>
+    </row>
+    <row r="339" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A339" s="15"/>
+      <c r="B339" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C339" s="15">
+        <v>1024</v>
+      </c>
+      <c r="D339" s="15">
         <v>64</v>
       </c>
-      <c r="E286" s="5">
-        <v>50</v>
-      </c>
-      <c r="G286" s="6">
-        <v>9.9760000000000009</v>
-      </c>
-      <c r="H286" s="6">
-        <v>9.213000000000001</v>
-      </c>
-      <c r="I286" s="6">
-        <f t="shared" si="29"/>
-        <v>2.6914694466720128</v>
-      </c>
-      <c r="J286" s="6">
-        <f t="shared" si="30"/>
-        <v>2.9143709106697058</v>
-      </c>
-    </row>
-    <row r="287" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C287" s="5">
-        <v>2048</v>
-      </c>
-      <c r="D287" s="5">
-        <v>128</v>
-      </c>
-      <c r="E287" s="5">
-        <v>50</v>
-      </c>
-      <c r="G287" s="6">
-        <v>8.2379999999999995</v>
-      </c>
-      <c r="H287" s="6">
-        <v>7.9550000000000001</v>
-      </c>
-      <c r="I287" s="6">
-        <f t="shared" si="29"/>
-        <v>6.5185965525613021</v>
-      </c>
-      <c r="J287" s="6">
-        <f t="shared" si="30"/>
-        <v>6.7504963419233182</v>
-      </c>
-    </row>
-    <row r="288" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C288" s="5">
-        <v>2560</v>
-      </c>
-      <c r="D288" s="5">
-        <v>16</v>
-      </c>
-      <c r="E288" s="5">
-        <v>50</v>
-      </c>
-      <c r="G288" s="6">
-        <v>8.49</v>
-      </c>
-      <c r="H288" s="6">
-        <v>7.6340000000000003</v>
-      </c>
-      <c r="I288" s="6">
-        <f t="shared" si="29"/>
-        <v>1.2353130742049467</v>
-      </c>
-      <c r="J288" s="6">
-        <f t="shared" si="30"/>
-        <v>1.3738286612522923</v>
-      </c>
-    </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C289" s="5">
-        <v>2560</v>
-      </c>
-      <c r="D289" s="5">
-        <v>32</v>
-      </c>
-      <c r="E289" s="5">
-        <v>50</v>
-      </c>
-      <c r="G289" s="6">
-        <v>13.502000000000001</v>
-      </c>
-      <c r="H289" s="6">
-        <v>13.005000000000001</v>
-      </c>
-      <c r="I289" s="6">
-        <f t="shared" si="29"/>
-        <v>1.5535191823433565</v>
-      </c>
-      <c r="J289" s="6">
-        <f t="shared" si="30"/>
-        <v>1.6128885813148786</v>
-      </c>
-    </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C290" s="5">
-        <v>2560</v>
-      </c>
-      <c r="D290" s="5">
-        <v>64</v>
-      </c>
-      <c r="E290" s="5">
-        <v>50</v>
-      </c>
-      <c r="G290" s="6">
-        <v>12.272</v>
-      </c>
-      <c r="H290" s="6">
-        <v>11.597</v>
-      </c>
-      <c r="I290" s="6">
-        <f t="shared" si="29"/>
-        <v>3.4184511082138203</v>
-      </c>
-      <c r="J290" s="6">
-        <f t="shared" si="30"/>
-        <v>3.6174210571699579</v>
-      </c>
-    </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C291" s="5">
-        <v>2560</v>
-      </c>
-      <c r="D291" s="5">
-        <v>128</v>
-      </c>
-      <c r="E291" s="5">
-        <v>50</v>
-      </c>
-      <c r="G291" s="6">
-        <v>12.307</v>
-      </c>
-      <c r="H291" s="6">
-        <v>12.093</v>
-      </c>
-      <c r="I291" s="6">
-        <f t="shared" si="29"/>
-        <v>6.8174586820508649</v>
-      </c>
-      <c r="J291" s="6">
-        <f t="shared" si="30"/>
-        <v>6.9381017117340615</v>
-      </c>
-    </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A295" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C295" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D295" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E295" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G295" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H295" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I295" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="J295" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="296" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C296" s="5">
-        <v>512</v>
-      </c>
-      <c r="D296" s="5">
-        <v>16</v>
-      </c>
-      <c r="E296" s="5">
-        <v>25</v>
-      </c>
-      <c r="G296" s="6">
-        <v>0.97699999999999998</v>
-      </c>
-      <c r="H296" s="6">
-        <v>1.1890000000000001</v>
-      </c>
-      <c r="I296" s="6">
-        <f t="shared" ref="I296:I317" si="31">(8*$E296*$D296*$C296*$C296)/(G296/1000)/10^12</f>
-        <v>0.85860880245649951</v>
-      </c>
-      <c r="J296" s="6">
-        <f t="shared" ref="J296:J311" si="32">(8*$E296*$D296*$C296*$C296)/(H296/1000)/10^12</f>
-        <v>0.70551791421362486</v>
-      </c>
-    </row>
-    <row r="297" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C297" s="5">
-        <v>512</v>
-      </c>
-      <c r="D297" s="5">
-        <v>32</v>
-      </c>
-      <c r="E297" s="5">
-        <v>25</v>
-      </c>
-      <c r="G297" s="6">
-        <v>2.0169999999999999</v>
-      </c>
-      <c r="H297" s="6">
-        <v>5.2869999999999999</v>
-      </c>
-      <c r="I297" s="6">
-        <f t="shared" si="31"/>
-        <v>0.8317905800694102</v>
-      </c>
-      <c r="J297" s="6">
-        <f t="shared" si="32"/>
-        <v>0.31732960090788725</v>
-      </c>
-    </row>
-    <row r="298" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C298" s="5">
-        <v>512</v>
-      </c>
-      <c r="D298" s="5">
-        <v>64</v>
-      </c>
-      <c r="E298" s="5">
-        <v>25</v>
-      </c>
-      <c r="G298" s="6">
-        <v>1.9160000000000001</v>
-      </c>
-      <c r="H298" s="6">
-        <v>1.9470000000000001</v>
-      </c>
-      <c r="I298" s="6">
-        <f t="shared" si="31"/>
-        <v>1.7512751565762001</v>
-      </c>
-      <c r="J298" s="6">
-        <f t="shared" si="32"/>
-        <v>1.7233914740626604</v>
-      </c>
-    </row>
-    <row r="299" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C299" s="5">
-        <v>512</v>
-      </c>
-      <c r="D299" s="5">
-        <v>128</v>
-      </c>
-      <c r="E299" s="5">
-        <v>25</v>
-      </c>
-      <c r="G299" s="6">
-        <v>2.141</v>
-      </c>
-      <c r="H299" s="6">
-        <v>2.177</v>
-      </c>
-      <c r="I299" s="6">
-        <f t="shared" si="31"/>
-        <v>3.1344635217188226</v>
-      </c>
-      <c r="J299" s="6">
-        <f t="shared" si="32"/>
-        <v>3.082630408819476</v>
-      </c>
-    </row>
-    <row r="300" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C300" s="5">
-        <v>1024</v>
-      </c>
-      <c r="D300" s="5">
-        <v>16</v>
-      </c>
-      <c r="E300" s="5">
-        <v>25</v>
-      </c>
-      <c r="G300" s="6">
-        <v>3.2690000000000001</v>
-      </c>
-      <c r="H300" s="6">
-        <v>2.181</v>
-      </c>
-      <c r="I300" s="6">
-        <f t="shared" si="31"/>
-        <v>1.0264433159987765</v>
-      </c>
-      <c r="J300" s="6">
-        <f t="shared" si="32"/>
-        <v>1.5384883998165977</v>
-      </c>
-    </row>
-    <row r="301" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C301" s="5">
-        <v>1024</v>
-      </c>
-      <c r="D301" s="5">
-        <v>32</v>
-      </c>
-      <c r="E301" s="5">
-        <v>25</v>
-      </c>
-      <c r="G301" s="6">
-        <v>3.56</v>
-      </c>
-      <c r="H301" s="6">
-        <v>9.7720000000000002</v>
-      </c>
-      <c r="I301" s="6">
-        <f t="shared" si="31"/>
-        <v>1.8850804494382021</v>
-      </c>
-      <c r="J301" s="6">
-        <f t="shared" si="32"/>
-        <v>0.68674645927138767</v>
-      </c>
-    </row>
-    <row r="302" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C302" s="5">
-        <v>1024</v>
-      </c>
-      <c r="D302" s="5">
-        <v>64</v>
-      </c>
-      <c r="E302" s="5">
-        <v>25</v>
-      </c>
-      <c r="G302" s="6">
-        <v>3.9180000000000001</v>
-      </c>
-      <c r="H302" s="6">
-        <v>3.0710000000000002</v>
-      </c>
-      <c r="I302" s="6">
-        <f t="shared" si="31"/>
-        <v>3.4256694231750888</v>
-      </c>
-      <c r="J302" s="6">
-        <f t="shared" si="32"/>
-        <v>4.3704893520026049</v>
-      </c>
-    </row>
-    <row r="303" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C303" s="5">
-        <v>1024</v>
-      </c>
-      <c r="D303" s="5">
-        <v>128</v>
-      </c>
-      <c r="E303" s="5">
-        <v>25</v>
-      </c>
-      <c r="G303" s="6">
-        <v>5.1050000000000004</v>
-      </c>
-      <c r="H303" s="6">
-        <v>4.4009999999999998</v>
-      </c>
-      <c r="I303" s="6">
-        <f t="shared" si="31"/>
-        <v>5.2582851322233104</v>
-      </c>
-      <c r="J303" s="6">
-        <f t="shared" si="32"/>
-        <v>6.0994195864576239</v>
-      </c>
-    </row>
-    <row r="304" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C304" s="5">
-        <v>2048</v>
-      </c>
-      <c r="D304" s="5">
-        <v>16</v>
-      </c>
-      <c r="E304" s="5">
-        <v>25</v>
-      </c>
-      <c r="G304" s="6">
-        <v>16.792000000000002</v>
-      </c>
-      <c r="H304" s="6">
-        <v>9.213000000000001</v>
-      </c>
-      <c r="I304" s="6">
-        <f t="shared" si="31"/>
-        <v>0.79929566460219137</v>
-      </c>
-      <c r="J304" s="6">
-        <f t="shared" si="32"/>
-        <v>1.4568297840008682</v>
-      </c>
-    </row>
-    <row r="305" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C305" s="5">
-        <v>2048</v>
-      </c>
-      <c r="D305" s="5">
-        <v>32</v>
-      </c>
-      <c r="E305" s="5">
-        <v>25</v>
-      </c>
-      <c r="G305" s="6">
-        <v>7.4050000000000002</v>
-      </c>
-      <c r="H305" s="6">
-        <v>18.954000000000001</v>
-      </c>
-      <c r="I305" s="6">
-        <f t="shared" si="31"/>
-        <v>3.6250567994598244</v>
-      </c>
-      <c r="J305" s="6">
-        <f t="shared" si="32"/>
-        <v>1.416246997995146</v>
-      </c>
-    </row>
-    <row r="306" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C306" s="5">
-        <v>2048</v>
-      </c>
-      <c r="D306" s="5">
-        <v>64</v>
-      </c>
-      <c r="E306" s="5">
-        <v>25</v>
-      </c>
-      <c r="G306" s="6">
-        <v>10.322000000000001</v>
-      </c>
-      <c r="H306" s="6">
-        <v>19.594000000000001</v>
-      </c>
-      <c r="I306" s="6">
-        <f t="shared" si="31"/>
-        <v>5.2012295291610142</v>
-      </c>
-      <c r="J306" s="6">
-        <f t="shared" si="32"/>
-        <v>2.739976074308462</v>
-      </c>
-    </row>
-    <row r="307" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C307" s="5">
-        <v>2048</v>
-      </c>
-      <c r="D307" s="5">
-        <v>128</v>
-      </c>
-      <c r="E307" s="5">
-        <v>25</v>
-      </c>
-      <c r="G307" s="6">
-        <v>14.926</v>
-      </c>
-      <c r="H307" s="6">
-        <v>12.38</v>
-      </c>
-      <c r="I307" s="6">
-        <f t="shared" si="31"/>
-        <v>7.193768082540533</v>
-      </c>
-      <c r="J307" s="6">
-        <f t="shared" si="32"/>
-        <v>8.6731972859450721</v>
-      </c>
-    </row>
-    <row r="308" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C308" s="5">
-        <v>4096</v>
-      </c>
-      <c r="D308" s="5">
-        <v>16</v>
-      </c>
-      <c r="E308" s="5">
-        <v>25</v>
-      </c>
-      <c r="G308" s="6">
-        <v>65.119</v>
-      </c>
-      <c r="H308" s="6">
-        <v>49.279000000000003</v>
-      </c>
-      <c r="I308" s="6">
-        <f t="shared" si="31"/>
-        <v>0.82444587908290978</v>
-      </c>
-      <c r="J308" s="6">
-        <f t="shared" si="32"/>
-        <v>1.0894517177702467</v>
-      </c>
-    </row>
-    <row r="309" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C309" s="5">
-        <v>4096</v>
-      </c>
-      <c r="D309" s="5">
-        <v>32</v>
-      </c>
-      <c r="E309" s="5">
-        <v>25</v>
-      </c>
-      <c r="G309" s="6">
-        <v>21.256</v>
-      </c>
-      <c r="H309" s="6">
-        <v>43.652999999999999</v>
-      </c>
-      <c r="I309" s="6">
-        <f t="shared" si="31"/>
-        <v>5.0514764019570944</v>
-      </c>
-      <c r="J309" s="6">
-        <f t="shared" si="32"/>
-        <v>2.4597205781962295</v>
-      </c>
-    </row>
-    <row r="310" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C310" s="5">
-        <v>4096</v>
-      </c>
-      <c r="D310" s="5">
-        <v>64</v>
-      </c>
-      <c r="E310" s="5">
-        <v>25</v>
-      </c>
-      <c r="G310" s="6">
-        <v>39.892000000000003</v>
-      </c>
-      <c r="H310" s="6">
-        <v>50.067</v>
-      </c>
-      <c r="I310" s="6">
-        <f t="shared" si="31"/>
-        <v>5.3832438784718741</v>
-      </c>
-      <c r="J310" s="6">
-        <f t="shared" si="32"/>
-        <v>4.2892197415463285</v>
-      </c>
-    </row>
-    <row r="311" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C311" s="5">
-        <v>4096</v>
-      </c>
-      <c r="D311" s="5">
-        <v>128</v>
-      </c>
-      <c r="E311" s="5">
-        <v>25</v>
-      </c>
-      <c r="G311" s="6">
-        <v>48.026000000000003</v>
-      </c>
-      <c r="H311" s="6">
-        <v>64.896000000000001</v>
-      </c>
-      <c r="I311" s="6">
-        <f t="shared" si="31"/>
-        <v>8.9430044059467768</v>
-      </c>
-      <c r="J311" s="6">
-        <f t="shared" si="32"/>
-        <v>6.6182311637080868</v>
-      </c>
-    </row>
-    <row r="312" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C312" s="5">
-        <v>1536</v>
-      </c>
-      <c r="D312" s="5">
-        <v>8</v>
-      </c>
-      <c r="E312" s="5">
-        <v>50</v>
-      </c>
-      <c r="G312" s="6">
-        <v>9.5820000000000007</v>
-      </c>
-      <c r="H312" s="6">
-        <v>6.1589999999999998</v>
-      </c>
-      <c r="I312" s="6">
-        <f t="shared" si="31"/>
-        <v>0.78790932999373831</v>
-      </c>
-      <c r="J312" s="6">
-        <f t="shared" ref="J312:J317" si="33">(8*$E312*$D312*$C312*$C312)/(H312/1000)/10^12</f>
-        <v>1.2258073063809061</v>
-      </c>
-    </row>
-    <row r="313" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C313" s="5">
-        <v>1536</v>
-      </c>
-      <c r="D313" s="5">
-        <v>16</v>
-      </c>
-      <c r="E313" s="5">
-        <v>50</v>
-      </c>
-      <c r="G313" s="6">
-        <v>17.681999999999999</v>
-      </c>
-      <c r="H313" s="6">
-        <v>9.7270000000000003</v>
-      </c>
-      <c r="I313" s="6">
-        <f t="shared" si="31"/>
-        <v>0.85394720054292506</v>
-      </c>
-      <c r="J313" s="6">
+      <c r="E339" s="15">
+        <v>1500</v>
+      </c>
+      <c r="F339" s="15"/>
+      <c r="G339" s="13">
+        <v>205.328</v>
+      </c>
+      <c r="H339" s="13">
+        <v>172.066</v>
+      </c>
+      <c r="I339" s="13">
+        <v>64.963999999999999</v>
+      </c>
+      <c r="J339" s="13">
+        <f>(6*$E339*$D339*$C339*$C339)/(G339/1000)/10^12</f>
+        <v>2.9415363515935478</v>
+      </c>
+      <c r="K339" s="13">
+        <f>(6*$E339*$D339*$C339*$C339)/(H339/1000)/10^12</f>
+        <v>3.5101634024153525</v>
+      </c>
+      <c r="L339" s="13">
+        <f>(6*$E339*$D339*$C339*$C339)/(I339/1000)/10^12</f>
+        <v>9.2971457422572517</v>
+      </c>
+      <c r="M339" s="14">
         <f t="shared" si="33"/>
-        <v>1.5523279942428294</v>
-      </c>
-    </row>
-    <row r="314" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C314" s="5">
-        <v>1536</v>
-      </c>
-      <c r="D314" s="5">
-        <v>32</v>
-      </c>
-      <c r="E314" s="5">
-        <v>50</v>
-      </c>
-      <c r="G314" s="6">
-        <v>10.656000000000001</v>
-      </c>
-      <c r="H314" s="6">
-        <v>29.04</v>
-      </c>
-      <c r="I314" s="6">
-        <f t="shared" si="31"/>
-        <v>2.8339891891891891</v>
-      </c>
-      <c r="J314" s="6">
-        <f t="shared" si="33"/>
-        <v>1.0399100826446281</v>
-      </c>
-    </row>
-    <row r="315" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C315" s="5">
-        <v>256</v>
-      </c>
-      <c r="D315" s="5">
-        <v>16</v>
-      </c>
-      <c r="E315" s="5">
-        <v>150</v>
-      </c>
-      <c r="G315" s="6">
-        <v>3.028</v>
-      </c>
-      <c r="H315" s="6">
-        <v>3.4660000000000002</v>
-      </c>
-      <c r="I315" s="6">
-        <f t="shared" si="31"/>
-        <v>0.41555191545574638</v>
-      </c>
-      <c r="J315" s="6">
-        <f t="shared" si="33"/>
-        <v>0.36303843046739753</v>
-      </c>
-    </row>
-    <row r="316" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C316" s="5">
-        <v>256</v>
-      </c>
-      <c r="D316" s="5">
-        <v>32</v>
-      </c>
-      <c r="E316" s="5">
-        <v>150</v>
-      </c>
-      <c r="G316" s="6">
-        <v>6.0579999999999998</v>
-      </c>
-      <c r="H316" s="6">
-        <v>14.347</v>
-      </c>
-      <c r="I316" s="6">
-        <f t="shared" si="31"/>
-        <v>0.41541472433146254</v>
-      </c>
-      <c r="J316" s="6">
-        <f t="shared" si="33"/>
-        <v>0.17540826653655817</v>
-      </c>
-    </row>
-    <row r="317" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C317" s="5">
-        <v>256</v>
-      </c>
-      <c r="D317" s="5">
-        <v>64</v>
-      </c>
-      <c r="E317" s="5">
-        <v>150</v>
-      </c>
-      <c r="G317" s="6">
-        <v>5.6029999999999998</v>
-      </c>
-      <c r="H317" s="6">
-        <v>8.0190000000000001</v>
-      </c>
-      <c r="I317" s="6">
-        <f t="shared" si="31"/>
-        <v>0.89829819739425321</v>
-      </c>
-      <c r="J317" s="6">
-        <f t="shared" si="33"/>
-        <v>0.62765491956603059</v>
-      </c>
-    </row>
-    <row r="318" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G318" s="6"/>
-      <c r="H318" s="6"/>
-    </row>
-    <row r="319" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G319" s="6"/>
-      <c r="H319" s="6"/>
-    </row>
-    <row r="320" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A320" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C320" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D320" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E320" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G320" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="H320" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="I320" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="J320" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="321" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C321" s="5">
-        <v>2816</v>
-      </c>
-      <c r="D321" s="5">
-        <v>32</v>
-      </c>
-      <c r="E321" s="5">
-        <v>1500</v>
-      </c>
-      <c r="G321" s="6">
-        <v>561.25300000000004</v>
-      </c>
-      <c r="H321" s="6">
-        <v>1213.086</v>
-      </c>
-      <c r="I321" s="6">
-        <f>(6*$E321*$D321*$C321*$C321)/(G321/1000)/10^12</f>
-        <v>4.0691070301628676</v>
-      </c>
-      <c r="J321" s="6">
-        <f>(6*$E321*$D321*$C321*$C321)/(H321/1000)/10^12</f>
-        <v>1.882635302031348</v>
-      </c>
-    </row>
-    <row r="322" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C322" s="5">
-        <v>2816</v>
-      </c>
-      <c r="D322" s="5">
-        <v>32</v>
-      </c>
-      <c r="E322" s="5">
-        <v>750</v>
-      </c>
-      <c r="G322" s="6">
-        <v>282.279</v>
-      </c>
-      <c r="H322" s="6">
-        <v>607.95400000000006</v>
-      </c>
-      <c r="I322" s="6">
-        <f t="shared" ref="I322:I339" si="34">(6*$E322*$D322*$C322*$C322)/(G322/1000)/10^12</f>
-        <v>4.0452859192501034</v>
-      </c>
-      <c r="J322" s="6">
-        <f t="shared" ref="J322:J339" si="35">(6*$E322*$D322*$C322*$C322)/(H322/1000)/10^12</f>
-        <v>1.8782658951170645</v>
-      </c>
-    </row>
-    <row r="323" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C323" s="5">
-        <v>2816</v>
-      </c>
-      <c r="D323" s="5">
-        <v>32</v>
-      </c>
-      <c r="E323" s="5">
-        <v>375</v>
-      </c>
-      <c r="G323" s="6">
-        <v>142.01300000000001</v>
-      </c>
-      <c r="H323" s="6">
-        <v>304.291</v>
-      </c>
-      <c r="I323" s="6">
-        <f t="shared" si="34"/>
-        <v>4.0204039911839056</v>
-      </c>
-      <c r="J323" s="6">
-        <f t="shared" si="35"/>
-        <v>1.8763276994718872</v>
-      </c>
-    </row>
-    <row r="324" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C324" s="5">
-        <v>2816</v>
-      </c>
-      <c r="D324" s="5">
-        <v>32</v>
-      </c>
-      <c r="E324" s="5">
-        <v>187</v>
-      </c>
-      <c r="G324" s="6">
-        <v>71.36</v>
-      </c>
-      <c r="H324" s="6">
-        <v>152.19400000000002</v>
-      </c>
-      <c r="I324" s="6">
-        <f t="shared" si="34"/>
-        <v>3.9898199246636779</v>
-      </c>
-      <c r="J324" s="6">
-        <f t="shared" si="35"/>
-        <v>1.8707278199140569</v>
-      </c>
-    </row>
-    <row r="325" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C325" s="5">
-        <v>2048</v>
-      </c>
-      <c r="D325" s="5">
-        <v>32</v>
-      </c>
-      <c r="E325" s="5">
-        <v>1500</v>
-      </c>
-      <c r="G325" s="6">
-        <v>383.34699999999998</v>
-      </c>
-      <c r="H325" s="6">
-        <v>866.298</v>
-      </c>
-      <c r="I325" s="6">
-        <f t="shared" si="34"/>
-        <v>3.1510864882208551</v>
-      </c>
-      <c r="J325" s="6">
-        <f t="shared" si="35"/>
-        <v>1.3943926362521903</v>
-      </c>
-    </row>
-    <row r="326" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C326" s="5">
-        <v>2048</v>
-      </c>
-      <c r="D326" s="5">
-        <v>32</v>
-      </c>
-      <c r="E326" s="5">
-        <v>750</v>
-      </c>
-      <c r="G326" s="6">
-        <v>191.446</v>
-      </c>
-      <c r="H326" s="6">
-        <v>431.84800000000001</v>
-      </c>
-      <c r="I326" s="6">
-        <f t="shared" si="34"/>
-        <v>3.154831001953553</v>
-      </c>
-      <c r="J326" s="6">
-        <f t="shared" si="35"/>
-        <v>1.398593431022026</v>
-      </c>
-    </row>
-    <row r="327" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C327" s="5">
-        <v>2048</v>
-      </c>
-      <c r="D327" s="5">
-        <v>32</v>
-      </c>
-      <c r="E327" s="5">
-        <v>375</v>
-      </c>
-      <c r="G327" s="6">
-        <v>96.722999999999999</v>
-      </c>
-      <c r="H327" s="6">
-        <v>217.494</v>
-      </c>
-      <c r="I327" s="6">
-        <f t="shared" si="34"/>
-        <v>3.1222138271145434</v>
-      </c>
-      <c r="J327" s="6">
-        <f t="shared" si="35"/>
-        <v>1.3884975585533395</v>
-      </c>
-    </row>
-    <row r="328" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C328" s="5">
-        <v>2048</v>
-      </c>
-      <c r="D328" s="5">
-        <v>32</v>
-      </c>
-      <c r="E328" s="5">
-        <v>187</v>
-      </c>
-      <c r="G328" s="6">
-        <v>48.928000000000004</v>
-      </c>
-      <c r="H328" s="6">
-        <v>108.84400000000001</v>
-      </c>
-      <c r="I328" s="6">
-        <f t="shared" si="34"/>
-        <v>3.0778345899280573</v>
-      </c>
-      <c r="J328" s="6">
-        <f t="shared" si="35"/>
-        <v>1.383560791738635</v>
-      </c>
-    </row>
-    <row r="329" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C329" s="5">
-        <v>1536</v>
-      </c>
-      <c r="D329" s="5">
-        <v>32</v>
-      </c>
-      <c r="E329" s="5">
-        <v>1500</v>
-      </c>
-      <c r="G329" s="6">
-        <v>272.92500000000001</v>
-      </c>
-      <c r="H329" s="6">
-        <v>649.56200000000001</v>
-      </c>
-      <c r="I329" s="6">
-        <f t="shared" si="34"/>
-        <v>2.489611607584501</v>
-      </c>
-      <c r="J329" s="6">
-        <f t="shared" si="35"/>
-        <v>1.0460544921039101</v>
-      </c>
-    </row>
-    <row r="330" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C330" s="5">
-        <v>1536</v>
-      </c>
-      <c r="D330" s="5">
-        <v>32</v>
-      </c>
-      <c r="E330" s="5">
-        <v>750</v>
-      </c>
-      <c r="G330" s="6">
-        <v>136.11799999999999</v>
-      </c>
-      <c r="H330" s="6">
-        <v>324.69200000000001</v>
-      </c>
-      <c r="I330" s="6">
-        <f t="shared" si="34"/>
-        <v>2.4959125464670362</v>
-      </c>
-      <c r="J330" s="6">
-        <f t="shared" si="35"/>
-        <v>1.0463412218348467</v>
-      </c>
-    </row>
-    <row r="331" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C331" s="5">
-        <v>1536</v>
-      </c>
-      <c r="D331" s="5">
-        <v>32</v>
-      </c>
-      <c r="E331" s="5">
-        <v>375</v>
-      </c>
-      <c r="G331" s="6">
-        <v>69.292000000000002</v>
-      </c>
-      <c r="H331" s="6">
-        <v>163.18899999999999</v>
-      </c>
-      <c r="I331" s="6">
-        <f t="shared" si="34"/>
-        <v>2.4514996247763086</v>
-      </c>
-      <c r="J331" s="6">
-        <f t="shared" si="35"/>
-        <v>1.040936043483323</v>
-      </c>
-    </row>
-    <row r="332" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C332" s="5">
-        <v>1536</v>
-      </c>
-      <c r="D332" s="5">
-        <v>32</v>
-      </c>
-      <c r="E332" s="5">
-        <v>187</v>
-      </c>
-      <c r="G332" s="6">
-        <v>35.615000000000002</v>
-      </c>
-      <c r="H332" s="6">
-        <v>82.433000000000007</v>
-      </c>
-      <c r="I332" s="6">
-        <f t="shared" si="34"/>
-        <v>2.3784406453460618</v>
-      </c>
-      <c r="J332" s="6">
-        <f t="shared" si="35"/>
-        <v>1.0276001550835223</v>
-      </c>
-    </row>
-    <row r="333" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C333" s="5">
-        <v>2560</v>
-      </c>
-      <c r="D333" s="7">
-        <v>32</v>
-      </c>
-      <c r="E333" s="7">
-        <v>1500</v>
-      </c>
-      <c r="G333" s="6">
-        <v>487.29300000000001</v>
-      </c>
-      <c r="H333" s="6">
-        <v>1093.913</v>
-      </c>
-      <c r="I333" s="6">
-        <f t="shared" si="34"/>
-        <v>3.8733098977411942</v>
-      </c>
-      <c r="J333" s="6">
-        <f t="shared" si="35"/>
-        <v>1.725399369054029</v>
-      </c>
-    </row>
-    <row r="334" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C334" s="5">
-        <v>2560</v>
-      </c>
-      <c r="D334" s="7">
-        <v>32</v>
-      </c>
-      <c r="E334" s="7">
-        <v>750</v>
-      </c>
-      <c r="G334" s="6">
-        <v>245.44300000000001</v>
-      </c>
-      <c r="H334" s="6">
-        <v>548.52499999999998</v>
-      </c>
-      <c r="I334" s="6">
-        <f t="shared" si="34"/>
-        <v>3.8449595221701167</v>
-      </c>
-      <c r="J334" s="6">
-        <f t="shared" si="35"/>
-        <v>1.7204656123239599</v>
-      </c>
-    </row>
-    <row r="335" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C335" s="5">
-        <v>2560</v>
-      </c>
-      <c r="D335" s="7">
-        <v>32</v>
-      </c>
-      <c r="E335" s="7">
-        <v>375</v>
-      </c>
-      <c r="G335" s="6">
-        <v>123.435</v>
-      </c>
-      <c r="H335" s="6">
-        <v>274.72199999999998</v>
-      </c>
-      <c r="I335" s="6">
-        <f t="shared" si="34"/>
-        <v>3.8227342325920524</v>
-      </c>
-      <c r="J335" s="6">
-        <f t="shared" si="35"/>
-        <v>1.7175879616485032</v>
-      </c>
-    </row>
-    <row r="336" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C336" s="5">
-        <v>2560</v>
-      </c>
-      <c r="D336" s="7">
-        <v>32</v>
-      </c>
-      <c r="E336" s="7">
-        <v>187</v>
-      </c>
-      <c r="G336" s="6">
-        <v>62.187000000000005</v>
-      </c>
-      <c r="H336" s="6">
-        <v>137.38900000000001</v>
-      </c>
-      <c r="I336" s="6">
-        <f t="shared" si="34"/>
-        <v>3.7837563220608805</v>
-      </c>
-      <c r="J336" s="6">
-        <f t="shared" si="35"/>
-        <v>1.7126586145906875</v>
-      </c>
-    </row>
-    <row r="337" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C337" s="5">
-        <v>512</v>
-      </c>
-      <c r="D337" s="7">
-        <v>32</v>
-      </c>
-      <c r="E337" s="7">
-        <v>1</v>
-      </c>
-      <c r="G337" s="6">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="H337" s="6">
-        <v>0.16400000000000001</v>
-      </c>
-      <c r="I337" s="6">
-        <f t="shared" si="34"/>
-        <v>0.86778703448275862</v>
-      </c>
-      <c r="J337" s="6">
-        <f t="shared" si="35"/>
-        <v>0.30690029268292685</v>
-      </c>
-    </row>
-    <row r="338" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C338" s="5">
-        <v>1024</v>
-      </c>
-      <c r="D338" s="7">
-        <v>32</v>
-      </c>
-      <c r="E338" s="7">
-        <v>1500</v>
-      </c>
-      <c r="G338" s="6">
-        <v>168.239</v>
-      </c>
-      <c r="H338" s="6">
-        <v>440.72800000000001</v>
-      </c>
-      <c r="I338" s="6">
-        <f t="shared" si="34"/>
-        <v>1.7950052484857852</v>
-      </c>
-      <c r="J338" s="6">
-        <f t="shared" si="35"/>
-        <v>0.68520694850338526</v>
-      </c>
-    </row>
-    <row r="339" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C339" s="5">
-        <v>1024</v>
-      </c>
-      <c r="D339" s="7">
-        <v>64</v>
-      </c>
-      <c r="E339" s="7">
-        <v>1500</v>
-      </c>
-      <c r="G339" s="6">
-        <v>195.11799999999999</v>
-      </c>
-      <c r="H339" s="6">
-        <v>156.56300000000002</v>
-      </c>
-      <c r="I339" s="6">
-        <f t="shared" si="34"/>
-        <v>3.0954590350454598</v>
-      </c>
-      <c r="J339" s="6">
-        <f t="shared" si="35"/>
-        <v>3.8577427361509424</v>
+        <v>442.358</v>
       </c>
     </row>
     <row r="340" spans="1:15" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -13248,25 +14242,25 @@
     </row>
     <row r="348" spans="1:15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
+        <v>67</v>
+      </c>
+      <c r="C348" t="s">
+        <v>68</v>
+      </c>
+      <c r="D348" t="s">
         <v>69</v>
       </c>
-      <c r="C348" t="s">
+      <c r="G348" t="s">
         <v>70</v>
       </c>
-      <c r="D348" t="s">
+      <c r="I348" t="s">
         <v>71</v>
       </c>
-      <c r="G348" t="s">
+      <c r="J348" t="s">
         <v>72</v>
       </c>
-      <c r="I348" t="s">
+      <c r="K348" t="s">
         <v>73</v>
-      </c>
-      <c r="J348" t="s">
-        <v>74</v>
-      </c>
-      <c r="K348" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="349" spans="1:15" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -13285,7 +14279,7 @@
         <v>12.835097316911146</v>
       </c>
       <c r="J350" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K350" s="13">
         <v>2.771354371816102E-3</v>
@@ -13309,7 +14303,7 @@
         <v>17.568133338618413</v>
       </c>
       <c r="J351" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K351" s="13">
         <v>3.1081657181485163E-3</v>
@@ -13333,7 +14327,7 @@
         <v>21.613808521919442</v>
       </c>
       <c r="J352" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K352" s="13">
         <v>2.7382020897316023E-3</v>
@@ -13360,7 +14354,7 @@
         <v>12.683225542430842</v>
       </c>
       <c r="J353" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K353" s="13">
         <v>1.4179616806863056E-2</v>
@@ -13385,7 +14379,7 @@
         <v>15.79122812082165</v>
       </c>
       <c r="J354" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K354" s="13">
         <v>2.8936258206434941E-2</v>
@@ -13407,7 +14401,7 @@
         <v>23.731852135606193</v>
       </c>
       <c r="J355" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K355" s="13">
         <v>3.4120529396769019E-3</v>
@@ -13431,7 +14425,7 @@
         <v>28.819072539613313</v>
       </c>
       <c r="J356" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K356" s="13">
         <v>2.1974866025578255E-3</v>
@@ -13455,7 +14449,7 @@
         <v>39.558659023908042</v>
       </c>
       <c r="J357" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K357" s="13">
         <v>5.0596776473147715E-3</v>
@@ -13482,7 +14476,7 @@
         <v>44.12763479595634</v>
       </c>
       <c r="J358" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K358" s="13">
         <v>0.13407438703550872</v>
@@ -13507,7 +14501,7 @@
         <v>85.614661814865158</v>
       </c>
       <c r="J359" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K359" s="13">
         <v>9.5564268900705421E-2</v>
@@ -13529,7 +14523,7 @@
         <v>23.982011935818178</v>
       </c>
       <c r="J360" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K360" s="13">
         <v>3.3130523372675203E-3</v>
@@ -13553,7 +14547,7 @@
         <v>29.01377604842197</v>
       </c>
       <c r="J361" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K361" s="13">
         <v>2.3169853371637567E-3</v>
@@ -13577,7 +14571,7 @@
         <v>39.497711966108255</v>
       </c>
       <c r="J362" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K362" s="13">
         <v>1.786874366036955E-3</v>
@@ -13604,7 +14598,7 @@
         <v>44.922131896148869</v>
       </c>
       <c r="J363" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K363" s="13">
         <v>7.6055643584500903E-3</v>
@@ -13629,7 +14623,7 @@
         <v>88.854658986255586</v>
       </c>
       <c r="J364" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K364" s="13">
         <v>0.19492017565835568</v>
@@ -13651,7 +14645,7 @@
         <v>24.097439904398577</v>
       </c>
       <c r="J365" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K365" s="13">
         <v>1.8945906376340066E-3</v>
@@ -13675,7 +14669,7 @@
         <v>29.332848450940624</v>
       </c>
       <c r="J366" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K366" s="13">
         <v>3.1434978841042975E-3</v>
@@ -13699,7 +14693,7 @@
         <v>39.469115820378669</v>
       </c>
       <c r="J367" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K367" s="13">
         <v>4.977845655343466E-3</v>
@@ -13726,7 +14720,7 @@
         <v>45.485056899373731</v>
       </c>
       <c r="J368" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K368" s="13">
         <v>8.1828182637063429E-3</v>
@@ -13751,7 +14745,7 @@
         <v>75.955594369660886</v>
       </c>
       <c r="J369" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K369" s="13">
         <v>0.34646444410114541</v>
@@ -13773,7 +14767,7 @@
         <v>24.260088749107531</v>
       </c>
       <c r="J370" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K370" s="13">
         <v>3.4101242453056131E-3</v>
@@ -13797,7 +14791,7 @@
         <v>29.352927360006991</v>
       </c>
       <c r="J371" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K371" s="13">
         <v>6.0341135484666842E-3</v>
@@ -13821,7 +14815,7 @@
         <v>39.581887632662536</v>
       </c>
       <c r="J372" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K372" s="13">
         <v>8.720665112249169E-3</v>
@@ -13848,7 +14842,7 @@
         <v>18.858364725395088</v>
       </c>
       <c r="J373" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K373" s="13">
         <v>0.53443442340576508</v>
@@ -13873,7 +14867,7 @@
         <v>34.116869923736488</v>
       </c>
       <c r="J374" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K374" s="13">
         <v>0.40676579786873596</v>
@@ -13895,7 +14889,7 @@
         <v>24.386522568340752</v>
       </c>
       <c r="J375" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K375" s="13">
         <v>7.5253956007218402E-3</v>
@@ -13916,7 +14910,7 @@
         <v>29.51436141820507</v>
       </c>
       <c r="J376" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K376" s="13">
         <v>1.4455375980472994E-2</v>
@@ -13937,7 +14931,7 @@
         <v>39.774351064898376</v>
       </c>
       <c r="J377" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K377" s="13">
         <v>1.0036250086036608E-2</v>
@@ -13961,7 +14955,7 @@
         <v>45.536169457821465</v>
       </c>
       <c r="J378" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K378" s="13">
         <v>4.3722356981296812E-2</v>
@@ -13985,7 +14979,7 @@
         <v>53.063780922995392</v>
       </c>
       <c r="J379" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K379" s="13">
         <v>2.0521634074351365</v>
@@ -14006,7 +15000,7 @@
         <v>24.414131807923237</v>
       </c>
       <c r="J380" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K380" s="13">
         <v>1.1580837166357418E-2</v>
@@ -14027,7 +15021,7 @@
         <v>29.396977409619254</v>
       </c>
       <c r="J381" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K381" s="13">
         <v>2.0194514627804788E-2</v>
@@ -14048,7 +15042,7 @@
         <v>39.83260271513997</v>
       </c>
       <c r="J382" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K382" s="13">
         <v>2.4471842035931668E-2</v>
@@ -14072,7 +15066,7 @@
         <v>45.539023512278831</v>
       </c>
       <c r="J383" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K383" s="13">
         <v>7.679382582089879E-2</v>
@@ -14096,7 +15090,7 @@
         <v>62.52556004907531</v>
       </c>
       <c r="J384" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K384" s="13">
         <v>0.28406578185528109</v>
@@ -14109,7 +15103,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14120,53 +15114,53 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B7" s="4">
         <v>375.66</v>
@@ -14174,15 +15168,15 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B9" s="5">
         <v>3502</v>
@@ -14190,19 +15184,19 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B10" s="5"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B11" s="5"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B12" s="5"/>
     </row>

</xml_diff>